<commit_message>
Update Listing 1.7 and 1.8
</commit_message>
<xml_diff>
--- a/Listings.xlsx
+++ b/Listings.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="27022"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="8420" yWindow="0" windowWidth="22420" windowHeight="20340"/>
+    <workbookView xWindow="8415" yWindow="0" windowWidth="22425" windowHeight="17520"/>
   </bookViews>
   <sheets>
     <sheet name="Listings" sheetId="1" r:id="rId1"/>
@@ -174,11 +174,11 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Cannot create computed columns in Access.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="L9" authorId="1">
+Cannot index on calculated column in Access (calcuated columns was introduced in Access 2010 and later)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M9" authorId="1">
       <text>
         <r>
           <rPr>
@@ -198,11 +198,11 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Not possible in Oracle.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="M9" authorId="1">
+Not possible in PostgreSQL</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I10" authorId="1">
       <text>
         <r>
           <rPr>
@@ -222,11 +222,11 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Not possible in PostgreSQL</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H10" authorId="1">
+Cannot index on calculated column in Access (calcuated columns was introduced in Access 2010 and later)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M10" authorId="1">
       <text>
         <r>
           <rPr>
@@ -246,103 +246,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Listing is Oracle-specific.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I10" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>John Viescas:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Listing is Oracle-specific.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="J10" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>John Viescas:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Listing is Oracle-specific.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="K10" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>John Viescas:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Listing is Oracle-specific.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="M10" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>John Viescas:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Listing is Oracle-specific.</t>
+Not possible in PostgreSQL</t>
         </r>
       </text>
     </comment>
@@ -10502,7 +10406,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -10517,25 +10421,25 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I34" sqref="I34:I35"/>
+      <selection pane="bottomLeft" activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="106.83203125" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="106.85546875" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="26" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="11" width="10.6640625" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="11" width="10.7109375" customWidth="1"/>
     <col min="12" max="12" width="11" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.6640625" customWidth="1"/>
-    <col min="19" max="19" width="8.83203125" customWidth="1"/>
+    <col min="13" max="13" width="10.7109375" customWidth="1"/>
+    <col min="19" max="19" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -10576,7 +10480,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -10599,7 +10503,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -10628,7 +10532,7 @@
       <c r="L3" s="7"/>
       <c r="M3" s="7"/>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>1</v>
       </c>
@@ -10657,7 +10561,7 @@
       <c r="L4" s="7"/>
       <c r="M4" s="7"/>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>1</v>
       </c>
@@ -10686,7 +10590,7 @@
       <c r="L5" s="7"/>
       <c r="M5" s="7"/>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>1</v>
       </c>
@@ -10715,7 +10619,7 @@
       <c r="L6" s="7"/>
       <c r="M6" s="7"/>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>1</v>
       </c>
@@ -10744,7 +10648,7 @@
       <c r="L7" s="7"/>
       <c r="M7" s="7"/>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>1</v>
       </c>
@@ -10773,7 +10677,7 @@
       <c r="L8" s="8"/>
       <c r="M8" s="8"/>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>1</v>
       </c>
@@ -10793,16 +10697,16 @@
         <v>486</v>
       </c>
       <c r="G9" s="15" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="H9" s="7"/>
       <c r="I9" s="8"/>
       <c r="J9" s="7"/>
       <c r="K9" s="7"/>
-      <c r="L9" s="8"/>
+      <c r="L9" s="7"/>
       <c r="M9" s="8"/>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>1</v>
       </c>
@@ -10822,16 +10726,16 @@
         <v>486</v>
       </c>
       <c r="G10" s="15" t="s">
-        <v>490</v>
-      </c>
-      <c r="H10" s="8"/>
+        <v>489</v>
+      </c>
+      <c r="H10" s="7"/>
       <c r="I10" s="8"/>
-      <c r="J10" s="8"/>
-      <c r="K10" s="8"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
       <c r="L10" s="7"/>
       <c r="M10" s="8"/>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>1</v>
       </c>
@@ -10860,7 +10764,7 @@
       <c r="L11" s="7"/>
       <c r="M11" s="7"/>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>1</v>
       </c>
@@ -10889,7 +10793,7 @@
       <c r="L12" s="7"/>
       <c r="M12" s="7"/>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>1</v>
       </c>
@@ -10918,7 +10822,7 @@
       <c r="L13" s="7"/>
       <c r="M13" s="7"/>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>1</v>
       </c>
@@ -10947,7 +10851,7 @@
       <c r="L14" s="7"/>
       <c r="M14" s="7"/>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>1</v>
       </c>
@@ -10970,7 +10874,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="16" spans="1:13">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>1</v>
       </c>
@@ -10993,7 +10897,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="17" spans="1:13">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>2</v>
       </c>
@@ -11022,7 +10926,7 @@
       <c r="L17" s="8"/>
       <c r="M17" s="8"/>
     </row>
-    <row r="18" spans="1:13">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>2</v>
       </c>
@@ -11051,7 +10955,7 @@
       <c r="L18" s="8"/>
       <c r="M18" s="8"/>
     </row>
-    <row r="19" spans="1:13">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>2</v>
       </c>
@@ -11080,7 +10984,7 @@
       <c r="L19" s="8"/>
       <c r="M19" s="8"/>
     </row>
-    <row r="20" spans="1:13">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>2</v>
       </c>
@@ -11109,7 +11013,7 @@
       <c r="L20" s="8"/>
       <c r="M20" s="8"/>
     </row>
-    <row r="21" spans="1:13">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>2</v>
       </c>
@@ -11138,7 +11042,7 @@
       <c r="L21" s="7"/>
       <c r="M21" s="8"/>
     </row>
-    <row r="22" spans="1:13">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>2</v>
       </c>
@@ -11167,7 +11071,7 @@
       <c r="L22" s="7"/>
       <c r="M22" s="8"/>
     </row>
-    <row r="23" spans="1:13">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>2</v>
       </c>
@@ -11196,7 +11100,7 @@
       <c r="L23" s="8"/>
       <c r="M23" s="7"/>
     </row>
-    <row r="24" spans="1:13">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>2</v>
       </c>
@@ -11225,7 +11129,7 @@
       <c r="L24" s="7"/>
       <c r="M24" s="7"/>
     </row>
-    <row r="25" spans="1:13">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>2</v>
       </c>
@@ -11254,7 +11158,7 @@
       <c r="L25" s="7"/>
       <c r="M25" s="7"/>
     </row>
-    <row r="26" spans="1:13">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>2</v>
       </c>
@@ -11283,7 +11187,7 @@
       <c r="L26" s="7"/>
       <c r="M26" s="7"/>
     </row>
-    <row r="27" spans="1:13">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>2</v>
       </c>
@@ -11312,7 +11216,7 @@
       <c r="L27" s="7"/>
       <c r="M27" s="7"/>
     </row>
-    <row r="28" spans="1:13">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>2</v>
       </c>
@@ -11341,7 +11245,7 @@
       <c r="L28" s="7"/>
       <c r="M28" s="7"/>
     </row>
-    <row r="29" spans="1:13">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>2</v>
       </c>
@@ -11370,7 +11274,7 @@
       <c r="L29" s="7"/>
       <c r="M29" s="7"/>
     </row>
-    <row r="30" spans="1:13">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>2</v>
       </c>
@@ -11399,7 +11303,7 @@
       <c r="L30" s="7"/>
       <c r="M30" s="7"/>
     </row>
-    <row r="31" spans="1:13">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>2</v>
       </c>
@@ -11428,7 +11332,7 @@
       <c r="L31" s="7"/>
       <c r="M31" s="7"/>
     </row>
-    <row r="32" spans="1:13">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>2</v>
       </c>
@@ -11457,7 +11361,7 @@
       <c r="L32" s="7"/>
       <c r="M32" s="7"/>
     </row>
-    <row r="33" spans="1:13">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>2</v>
       </c>
@@ -11486,7 +11390,7 @@
       <c r="L33" s="7"/>
       <c r="M33" s="7"/>
     </row>
-    <row r="34" spans="1:13">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>2</v>
       </c>
@@ -11515,7 +11419,7 @@
       <c r="L34" s="7"/>
       <c r="M34" s="7"/>
     </row>
-    <row r="35" spans="1:13">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>2</v>
       </c>
@@ -11544,7 +11448,7 @@
       <c r="L35" s="9"/>
       <c r="M35" s="7"/>
     </row>
-    <row r="36" spans="1:13">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>2</v>
       </c>
@@ -11573,7 +11477,7 @@
       <c r="L36" s="9"/>
       <c r="M36" s="7"/>
     </row>
-    <row r="37" spans="1:13">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>2</v>
       </c>
@@ -11602,7 +11506,7 @@
       <c r="L37" s="7"/>
       <c r="M37" s="7"/>
     </row>
-    <row r="38" spans="1:13">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
         <v>2</v>
       </c>
@@ -11631,7 +11535,7 @@
       <c r="L38" s="7"/>
       <c r="M38" s="7"/>
     </row>
-    <row r="39" spans="1:13">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>2</v>
       </c>
@@ -11660,7 +11564,7 @@
       <c r="L39" s="7"/>
       <c r="M39" s="7"/>
     </row>
-    <row r="40" spans="1:13">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
         <v>2</v>
       </c>
@@ -11689,7 +11593,7 @@
       <c r="L40" s="7"/>
       <c r="M40" s="7"/>
     </row>
-    <row r="41" spans="1:13">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <v>2</v>
       </c>
@@ -11718,7 +11622,7 @@
       <c r="L41" s="7"/>
       <c r="M41" s="7"/>
     </row>
-    <row r="42" spans="1:13">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
         <v>2</v>
       </c>
@@ -11742,7 +11646,7 @@
       </c>
       <c r="J42" s="11"/>
     </row>
-    <row r="43" spans="1:13">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
         <v>2</v>
       </c>
@@ -11766,7 +11670,7 @@
       </c>
       <c r="J43" s="11"/>
     </row>
-    <row r="44" spans="1:13">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
         <v>2</v>
       </c>
@@ -11795,7 +11699,7 @@
       <c r="L44" s="7"/>
       <c r="M44" s="7"/>
     </row>
-    <row r="45" spans="1:13">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
         <v>2</v>
       </c>
@@ -11824,7 +11728,7 @@
       <c r="L45" s="7"/>
       <c r="M45" s="7"/>
     </row>
-    <row r="46" spans="1:13">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
         <v>2</v>
       </c>
@@ -11853,7 +11757,7 @@
       <c r="L46" s="7"/>
       <c r="M46" s="7"/>
     </row>
-    <row r="47" spans="1:13">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
         <v>2</v>
       </c>
@@ -11882,7 +11786,7 @@
       <c r="L47" s="7"/>
       <c r="M47" s="7"/>
     </row>
-    <row r="48" spans="1:13">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
         <v>2</v>
       </c>
@@ -11911,7 +11815,7 @@
       <c r="L48" s="7"/>
       <c r="M48" s="7"/>
     </row>
-    <row r="49" spans="1:13">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
         <v>3</v>
       </c>
@@ -11940,7 +11844,7 @@
       <c r="L49" s="7"/>
       <c r="M49" s="7"/>
     </row>
-    <row r="50" spans="1:13">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" s="3">
         <v>3</v>
       </c>
@@ -11969,7 +11873,7 @@
       <c r="L50" s="7"/>
       <c r="M50" s="7"/>
     </row>
-    <row r="51" spans="1:13">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" s="3">
         <v>3</v>
       </c>
@@ -11998,7 +11902,7 @@
       <c r="L51" s="7"/>
       <c r="M51" s="7"/>
     </row>
-    <row r="52" spans="1:13">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" s="3">
         <v>3</v>
       </c>
@@ -12027,7 +11931,7 @@
       <c r="L52" s="7"/>
       <c r="M52" s="7"/>
     </row>
-    <row r="53" spans="1:13">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" s="3">
         <v>3</v>
       </c>
@@ -12056,7 +11960,7 @@
       <c r="L53" s="7"/>
       <c r="M53" s="7"/>
     </row>
-    <row r="54" spans="1:13">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" s="3">
         <v>3</v>
       </c>
@@ -12085,7 +11989,7 @@
       <c r="L54" s="8"/>
       <c r="M54" s="8"/>
     </row>
-    <row r="55" spans="1:13">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55" s="3">
         <v>3</v>
       </c>
@@ -12114,7 +12018,7 @@
       <c r="L55" s="9"/>
       <c r="M55" s="8"/>
     </row>
-    <row r="56" spans="1:13">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" s="3">
         <v>3</v>
       </c>
@@ -12143,7 +12047,7 @@
       <c r="L56" s="7"/>
       <c r="M56" s="7"/>
     </row>
-    <row r="57" spans="1:13">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57" s="3">
         <v>3</v>
       </c>
@@ -12172,7 +12076,7 @@
       <c r="L57" s="7"/>
       <c r="M57" s="7"/>
     </row>
-    <row r="58" spans="1:13">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58" s="3">
         <v>3</v>
       </c>
@@ -12201,7 +12105,7 @@
       <c r="L58" s="7"/>
       <c r="M58" s="7"/>
     </row>
-    <row r="59" spans="1:13">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59" s="3">
         <v>3</v>
       </c>
@@ -12230,7 +12134,7 @@
       <c r="L59" s="9"/>
       <c r="M59" s="7"/>
     </row>
-    <row r="60" spans="1:13">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60" s="3">
         <v>4</v>
       </c>
@@ -12259,7 +12163,7 @@
       <c r="L60" s="7"/>
       <c r="M60" s="7"/>
     </row>
-    <row r="61" spans="1:13">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61" s="3">
         <v>4</v>
       </c>
@@ -12288,7 +12192,7 @@
       <c r="L61" s="7"/>
       <c r="M61" s="7"/>
     </row>
-    <row r="62" spans="1:13">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A62" s="3">
         <v>4</v>
       </c>
@@ -12317,7 +12221,7 @@
       <c r="L62" s="7"/>
       <c r="M62" s="7"/>
     </row>
-    <row r="63" spans="1:13">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63" s="3">
         <v>4</v>
       </c>
@@ -12346,7 +12250,7 @@
       <c r="L63" s="7"/>
       <c r="M63" s="7"/>
     </row>
-    <row r="64" spans="1:13">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A64" s="3">
         <v>4</v>
       </c>
@@ -12375,7 +12279,7 @@
       <c r="L64" s="7"/>
       <c r="M64" s="7"/>
     </row>
-    <row r="65" spans="1:13">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A65" s="3">
         <v>4</v>
       </c>
@@ -12404,7 +12308,7 @@
       <c r="L65" s="7"/>
       <c r="M65" s="7"/>
     </row>
-    <row r="66" spans="1:13">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A66" s="3">
         <v>4</v>
       </c>
@@ -12433,7 +12337,7 @@
       <c r="L66" s="16"/>
       <c r="M66" s="16"/>
     </row>
-    <row r="67" spans="1:13">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A67" s="3">
         <v>4</v>
       </c>
@@ -12462,7 +12366,7 @@
       <c r="L67" s="7"/>
       <c r="M67" s="7"/>
     </row>
-    <row r="68" spans="1:13">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A68" s="3">
         <v>4</v>
       </c>
@@ -12491,7 +12395,7 @@
       <c r="L68" s="7"/>
       <c r="M68" s="7"/>
     </row>
-    <row r="69" spans="1:13">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A69" s="3">
         <v>4</v>
       </c>
@@ -12520,7 +12424,7 @@
       <c r="L69" s="7"/>
       <c r="M69" s="7"/>
     </row>
-    <row r="70" spans="1:13">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A70" s="3">
         <v>4</v>
       </c>
@@ -12549,7 +12453,7 @@
       <c r="L70" s="7"/>
       <c r="M70" s="7"/>
     </row>
-    <row r="71" spans="1:13">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A71" s="3">
         <v>4</v>
       </c>
@@ -12578,7 +12482,7 @@
       <c r="L71" s="7"/>
       <c r="M71" s="7"/>
     </row>
-    <row r="72" spans="1:13">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A72" s="3">
         <v>4</v>
       </c>
@@ -12607,7 +12511,7 @@
       <c r="L72" s="7"/>
       <c r="M72" s="7"/>
     </row>
-    <row r="73" spans="1:13">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A73" s="3">
         <v>4</v>
       </c>
@@ -12636,7 +12540,7 @@
       <c r="L73" s="7"/>
       <c r="M73" s="7"/>
     </row>
-    <row r="74" spans="1:13">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A74" s="3">
         <v>4</v>
       </c>
@@ -12665,7 +12569,7 @@
       <c r="L74" s="7"/>
       <c r="M74" s="7"/>
     </row>
-    <row r="75" spans="1:13">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A75" s="3">
         <v>4</v>
       </c>
@@ -12694,7 +12598,7 @@
       <c r="L75" s="7"/>
       <c r="M75" s="7"/>
     </row>
-    <row r="76" spans="1:13">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A76" s="3">
         <v>4</v>
       </c>
@@ -12723,7 +12627,7 @@
       <c r="L76" s="7"/>
       <c r="M76" s="7"/>
     </row>
-    <row r="77" spans="1:13">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A77" s="3">
         <v>4</v>
       </c>
@@ -12752,7 +12656,7 @@
       <c r="L77" s="7"/>
       <c r="M77" s="7"/>
     </row>
-    <row r="78" spans="1:13">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A78" s="3">
         <v>4</v>
       </c>
@@ -12781,7 +12685,7 @@
       <c r="L78" s="7"/>
       <c r="M78" s="7"/>
     </row>
-    <row r="79" spans="1:13">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A79" s="3">
         <v>4</v>
       </c>
@@ -12810,7 +12714,7 @@
       <c r="L79" s="7"/>
       <c r="M79" s="7"/>
     </row>
-    <row r="80" spans="1:13">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A80" s="3">
         <v>4</v>
       </c>
@@ -12839,7 +12743,7 @@
       <c r="L80" s="7"/>
       <c r="M80" s="7"/>
     </row>
-    <row r="81" spans="1:13">
+    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A81" s="3">
         <v>4</v>
       </c>
@@ -12868,7 +12772,7 @@
       <c r="L81" s="7"/>
       <c r="M81" s="7"/>
     </row>
-    <row r="82" spans="1:13">
+    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A82" s="3">
         <v>4</v>
       </c>
@@ -12897,7 +12801,7 @@
       <c r="L82" s="7"/>
       <c r="M82" s="7"/>
     </row>
-    <row r="83" spans="1:13">
+    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A83" s="3">
         <v>4</v>
       </c>
@@ -12926,7 +12830,7 @@
       <c r="L83" s="7"/>
       <c r="M83" s="7"/>
     </row>
-    <row r="84" spans="1:13">
+    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A84" s="3">
         <v>4</v>
       </c>
@@ -12955,7 +12859,7 @@
       <c r="L84" s="7"/>
       <c r="M84" s="7"/>
     </row>
-    <row r="85" spans="1:13">
+    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A85" s="3">
         <v>4</v>
       </c>
@@ -12984,7 +12888,7 @@
       <c r="L85" s="7"/>
       <c r="M85" s="7"/>
     </row>
-    <row r="86" spans="1:13">
+    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A86" s="3">
         <v>4</v>
       </c>
@@ -13013,7 +12917,7 @@
       <c r="L86" s="7"/>
       <c r="M86" s="7"/>
     </row>
-    <row r="87" spans="1:13">
+    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A87" s="3">
         <v>4</v>
       </c>
@@ -13042,7 +12946,7 @@
       <c r="L87" s="7"/>
       <c r="M87" s="7"/>
     </row>
-    <row r="88" spans="1:13">
+    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A88" s="3">
         <v>4</v>
       </c>
@@ -13071,7 +12975,7 @@
       <c r="L88" s="7"/>
       <c r="M88" s="7"/>
     </row>
-    <row r="89" spans="1:13">
+    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A89" s="3">
         <v>4</v>
       </c>
@@ -13100,7 +13004,7 @@
       <c r="L89" s="7"/>
       <c r="M89" s="7"/>
     </row>
-    <row r="90" spans="1:13">
+    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A90" s="3">
         <v>4</v>
       </c>
@@ -13129,7 +13033,7 @@
       <c r="L90" s="7"/>
       <c r="M90" s="7"/>
     </row>
-    <row r="91" spans="1:13">
+    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A91" s="3">
         <v>4</v>
       </c>
@@ -13158,7 +13062,7 @@
       <c r="L91" s="7"/>
       <c r="M91" s="7"/>
     </row>
-    <row r="92" spans="1:13">
+    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A92" s="3">
         <v>4</v>
       </c>
@@ -13187,7 +13091,7 @@
       <c r="L92" s="7"/>
       <c r="M92" s="7"/>
     </row>
-    <row r="93" spans="1:13">
+    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A93" s="3">
         <v>4</v>
       </c>
@@ -13216,7 +13120,7 @@
       <c r="L93" s="7"/>
       <c r="M93" s="7"/>
     </row>
-    <row r="94" spans="1:13">
+    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A94" s="3">
         <v>4</v>
       </c>
@@ -13245,7 +13149,7 @@
       <c r="L94" s="7"/>
       <c r="M94" s="7"/>
     </row>
-    <row r="95" spans="1:13">
+    <row r="95" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A95" s="3">
         <v>4</v>
       </c>
@@ -13274,7 +13178,7 @@
       <c r="L95" s="7"/>
       <c r="M95" s="7"/>
     </row>
-    <row r="96" spans="1:13">
+    <row r="96" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A96" s="3">
         <v>4</v>
       </c>
@@ -13303,7 +13207,7 @@
       <c r="L96" s="7"/>
       <c r="M96" s="7"/>
     </row>
-    <row r="97" spans="1:13">
+    <row r="97" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A97" s="3">
         <v>4</v>
       </c>
@@ -13332,7 +13236,7 @@
       <c r="L97" s="7"/>
       <c r="M97" s="7"/>
     </row>
-    <row r="98" spans="1:13">
+    <row r="98" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A98" s="3">
         <v>4</v>
       </c>
@@ -13361,7 +13265,7 @@
       <c r="L98" s="7"/>
       <c r="M98" s="7"/>
     </row>
-    <row r="99" spans="1:13">
+    <row r="99" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A99" s="3">
         <v>4</v>
       </c>
@@ -13390,7 +13294,7 @@
       <c r="L99" s="7"/>
       <c r="M99" s="7"/>
     </row>
-    <row r="100" spans="1:13">
+    <row r="100" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A100" s="3">
         <v>5</v>
       </c>
@@ -13419,7 +13323,7 @@
       <c r="L100" s="16"/>
       <c r="M100" s="16"/>
     </row>
-    <row r="101" spans="1:13">
+    <row r="101" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A101" s="3">
         <v>5</v>
       </c>
@@ -13448,7 +13352,7 @@
       <c r="L101" s="16"/>
       <c r="M101" s="16"/>
     </row>
-    <row r="102" spans="1:13">
+    <row r="102" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A102" s="3">
         <v>5</v>
       </c>
@@ -13477,7 +13381,7 @@
       <c r="L102" s="16"/>
       <c r="M102" s="16"/>
     </row>
-    <row r="103" spans="1:13">
+    <row r="103" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A103" s="3">
         <v>5</v>
       </c>
@@ -13506,7 +13410,7 @@
       <c r="L103" s="7"/>
       <c r="M103" s="7"/>
     </row>
-    <row r="104" spans="1:13">
+    <row r="104" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A104" s="3">
         <v>5</v>
       </c>
@@ -13535,7 +13439,7 @@
       <c r="L104" s="7"/>
       <c r="M104" s="7"/>
     </row>
-    <row r="105" spans="1:13">
+    <row r="105" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A105" s="3">
         <v>5</v>
       </c>
@@ -13564,7 +13468,7 @@
       <c r="L105" s="7"/>
       <c r="M105" s="7"/>
     </row>
-    <row r="106" spans="1:13">
+    <row r="106" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A106" s="3">
         <v>5</v>
       </c>
@@ -13593,7 +13497,7 @@
       <c r="L106" s="7"/>
       <c r="M106" s="7"/>
     </row>
-    <row r="107" spans="1:13">
+    <row r="107" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A107" s="3">
         <v>5</v>
       </c>
@@ -13622,7 +13526,7 @@
       <c r="L107" s="7"/>
       <c r="M107" s="7"/>
     </row>
-    <row r="108" spans="1:13">
+    <row r="108" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A108" s="3">
         <v>5</v>
       </c>
@@ -13651,7 +13555,7 @@
       <c r="L108" s="7"/>
       <c r="M108" s="7"/>
     </row>
-    <row r="109" spans="1:13">
+    <row r="109" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A109" s="3">
         <v>5</v>
       </c>
@@ -13680,7 +13584,7 @@
       <c r="L109" s="7"/>
       <c r="M109" s="7"/>
     </row>
-    <row r="110" spans="1:13">
+    <row r="110" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A110" s="3">
         <v>5</v>
       </c>
@@ -13709,7 +13613,7 @@
       <c r="L110" s="8"/>
       <c r="M110" s="7"/>
     </row>
-    <row r="111" spans="1:13">
+    <row r="111" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A111" s="3">
         <v>5</v>
       </c>
@@ -13738,7 +13642,7 @@
       <c r="L111" s="7"/>
       <c r="M111" s="7"/>
     </row>
-    <row r="112" spans="1:13">
+    <row r="112" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A112" s="3">
         <v>5</v>
       </c>
@@ -13767,7 +13671,7 @@
       <c r="L112" s="7"/>
       <c r="M112" s="7"/>
     </row>
-    <row r="113" spans="1:13">
+    <row r="113" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A113" s="3">
         <v>5</v>
       </c>
@@ -13796,7 +13700,7 @@
       <c r="L113" s="7"/>
       <c r="M113" s="7"/>
     </row>
-    <row r="114" spans="1:13">
+    <row r="114" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A114" s="3">
         <v>5</v>
       </c>
@@ -13825,7 +13729,7 @@
       <c r="L114" s="9"/>
       <c r="M114" s="7"/>
     </row>
-    <row r="115" spans="1:13">
+    <row r="115" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A115" s="3">
         <v>5</v>
       </c>
@@ -13854,7 +13758,7 @@
       <c r="L115" s="9"/>
       <c r="M115" s="7"/>
     </row>
-    <row r="116" spans="1:13">
+    <row r="116" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A116" s="3">
         <v>5</v>
       </c>
@@ -13883,7 +13787,7 @@
       <c r="L116" s="7"/>
       <c r="M116" s="7"/>
     </row>
-    <row r="117" spans="1:13">
+    <row r="117" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A117" s="3">
         <v>5</v>
       </c>
@@ -13912,7 +13816,7 @@
       <c r="L117" s="7"/>
       <c r="M117" s="7"/>
     </row>
-    <row r="118" spans="1:13">
+    <row r="118" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A118" s="3">
         <v>5</v>
       </c>
@@ -13941,7 +13845,7 @@
       <c r="L118" s="7"/>
       <c r="M118" s="7"/>
     </row>
-    <row r="119" spans="1:13">
+    <row r="119" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A119" s="3">
         <v>5</v>
       </c>
@@ -13970,7 +13874,7 @@
       <c r="L119" s="7"/>
       <c r="M119" s="7"/>
     </row>
-    <row r="120" spans="1:13">
+    <row r="120" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A120" s="3">
         <v>5</v>
       </c>
@@ -13999,7 +13903,7 @@
       <c r="L120" s="7"/>
       <c r="M120" s="7"/>
     </row>
-    <row r="121" spans="1:13">
+    <row r="121" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A121" s="3">
         <v>5</v>
       </c>
@@ -14028,7 +13932,7 @@
       <c r="L121" s="7"/>
       <c r="M121" s="7"/>
     </row>
-    <row r="122" spans="1:13">
+    <row r="122" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A122" s="3">
         <v>5</v>
       </c>
@@ -14057,7 +13961,7 @@
       <c r="L122" s="7"/>
       <c r="M122" s="7"/>
     </row>
-    <row r="123" spans="1:13">
+    <row r="123" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A123" s="3">
         <v>5</v>
       </c>
@@ -14086,7 +13990,7 @@
       <c r="L123" s="7"/>
       <c r="M123" s="9"/>
     </row>
-    <row r="124" spans="1:13">
+    <row r="124" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A124" s="3">
         <v>5</v>
       </c>
@@ -14115,7 +14019,7 @@
       <c r="L124" s="7"/>
       <c r="M124" s="9"/>
     </row>
-    <row r="125" spans="1:13">
+    <row r="125" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A125" s="3">
         <v>5</v>
       </c>
@@ -14144,7 +14048,7 @@
       <c r="L125" s="7"/>
       <c r="M125" s="9"/>
     </row>
-    <row r="126" spans="1:13">
+    <row r="126" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A126" s="3">
         <v>5</v>
       </c>
@@ -14173,7 +14077,7 @@
       <c r="L126" s="7"/>
       <c r="M126" s="7"/>
     </row>
-    <row r="127" spans="1:13">
+    <row r="127" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A127" s="3">
         <v>5</v>
       </c>
@@ -14202,7 +14106,7 @@
       <c r="L127" s="9"/>
       <c r="M127" s="7"/>
     </row>
-    <row r="128" spans="1:13">
+    <row r="128" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A128" s="3">
         <v>5</v>
       </c>
@@ -14231,7 +14135,7 @@
       <c r="L128" s="7"/>
       <c r="M128" s="7"/>
     </row>
-    <row r="129" spans="1:13">
+    <row r="129" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A129" s="3">
         <v>5</v>
       </c>
@@ -14260,7 +14164,7 @@
       <c r="L129" s="7"/>
       <c r="M129" s="7"/>
     </row>
-    <row r="130" spans="1:13">
+    <row r="130" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A130" s="3">
         <v>5</v>
       </c>
@@ -14289,7 +14193,7 @@
       <c r="L130" s="7"/>
       <c r="M130" s="7"/>
     </row>
-    <row r="131" spans="1:13">
+    <row r="131" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A131" s="3">
         <v>5</v>
       </c>
@@ -14318,7 +14222,7 @@
       <c r="L131" s="7"/>
       <c r="M131" s="7"/>
     </row>
-    <row r="132" spans="1:13">
+    <row r="132" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A132" s="3">
         <v>5</v>
       </c>
@@ -14347,7 +14251,7 @@
       <c r="L132" s="7"/>
       <c r="M132" s="7"/>
     </row>
-    <row r="133" spans="1:13">
+    <row r="133" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A133" s="3">
         <v>5</v>
       </c>
@@ -14376,7 +14280,7 @@
       <c r="L133" s="7"/>
       <c r="M133" s="7"/>
     </row>
-    <row r="134" spans="1:13">
+    <row r="134" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A134" s="3">
         <v>6</v>
       </c>
@@ -14405,7 +14309,7 @@
       <c r="L134" s="7"/>
       <c r="M134" s="7"/>
     </row>
-    <row r="135" spans="1:13">
+    <row r="135" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A135" s="3">
         <v>6</v>
       </c>
@@ -14434,7 +14338,7 @@
       <c r="L135" s="7"/>
       <c r="M135" s="7"/>
     </row>
-    <row r="136" spans="1:13">
+    <row r="136" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A136" s="3">
         <v>6</v>
       </c>
@@ -14463,7 +14367,7 @@
       <c r="L136" s="7"/>
       <c r="M136" s="7"/>
     </row>
-    <row r="137" spans="1:13">
+    <row r="137" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A137" s="3">
         <v>6</v>
       </c>
@@ -14492,7 +14396,7 @@
       <c r="L137" s="7"/>
       <c r="M137" s="7"/>
     </row>
-    <row r="138" spans="1:13">
+    <row r="138" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A138" s="3">
         <v>6</v>
       </c>
@@ -14521,7 +14425,7 @@
       <c r="L138" s="7"/>
       <c r="M138" s="7"/>
     </row>
-    <row r="139" spans="1:13">
+    <row r="139" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A139" s="3">
         <v>6</v>
       </c>
@@ -14550,7 +14454,7 @@
       <c r="L139" s="7"/>
       <c r="M139" s="7"/>
     </row>
-    <row r="140" spans="1:13">
+    <row r="140" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A140" s="3">
         <v>6</v>
       </c>
@@ -14579,7 +14483,7 @@
       <c r="L140" s="7"/>
       <c r="M140" s="7"/>
     </row>
-    <row r="141" spans="1:13">
+    <row r="141" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A141" s="3">
         <v>6</v>
       </c>
@@ -14608,7 +14512,7 @@
       <c r="L141" s="7"/>
       <c r="M141" s="7"/>
     </row>
-    <row r="142" spans="1:13">
+    <row r="142" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A142" s="3">
         <v>6</v>
       </c>
@@ -14637,7 +14541,7 @@
       <c r="L142" s="7"/>
       <c r="M142" s="7"/>
     </row>
-    <row r="143" spans="1:13">
+    <row r="143" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A143" s="3">
         <v>6</v>
       </c>
@@ -14666,7 +14570,7 @@
       <c r="L143" s="7"/>
       <c r="M143" s="7"/>
     </row>
-    <row r="144" spans="1:13">
+    <row r="144" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A144" s="3">
         <v>6</v>
       </c>
@@ -14695,7 +14599,7 @@
       <c r="L144" s="7"/>
       <c r="M144" s="7"/>
     </row>
-    <row r="145" spans="1:13">
+    <row r="145" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A145" s="3">
         <v>6</v>
       </c>
@@ -14724,7 +14628,7 @@
       <c r="L145" s="7"/>
       <c r="M145" s="7"/>
     </row>
-    <row r="146" spans="1:13">
+    <row r="146" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A146" s="3">
         <v>6</v>
       </c>
@@ -14753,7 +14657,7 @@
       <c r="L146" s="7"/>
       <c r="M146" s="7"/>
     </row>
-    <row r="147" spans="1:13">
+    <row r="147" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A147" s="3">
         <v>6</v>
       </c>
@@ -14782,7 +14686,7 @@
       <c r="L147" s="7"/>
       <c r="M147" s="7"/>
     </row>
-    <row r="148" spans="1:13">
+    <row r="148" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A148" s="3">
         <v>6</v>
       </c>
@@ -14811,7 +14715,7 @@
       <c r="L148" s="7"/>
       <c r="M148" s="7"/>
     </row>
-    <row r="149" spans="1:13">
+    <row r="149" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A149" s="3">
         <v>6</v>
       </c>
@@ -14840,7 +14744,7 @@
       <c r="L149" s="7"/>
       <c r="M149" s="7"/>
     </row>
-    <row r="150" spans="1:13">
+    <row r="150" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A150" s="3">
         <v>6</v>
       </c>
@@ -14869,7 +14773,7 @@
       <c r="L150" s="7"/>
       <c r="M150" s="7"/>
     </row>
-    <row r="151" spans="1:13">
+    <row r="151" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A151" s="3">
         <v>6</v>
       </c>
@@ -14898,7 +14802,7 @@
       <c r="L151" s="7"/>
       <c r="M151" s="7"/>
     </row>
-    <row r="152" spans="1:13">
+    <row r="152" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A152" s="3">
         <v>6</v>
       </c>
@@ -14927,7 +14831,7 @@
       <c r="L152" s="7"/>
       <c r="M152" s="7"/>
     </row>
-    <row r="153" spans="1:13">
+    <row r="153" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A153" s="3">
         <v>7</v>
       </c>
@@ -14956,7 +14860,7 @@
       <c r="L153" s="8"/>
       <c r="M153" s="8"/>
     </row>
-    <row r="154" spans="1:13">
+    <row r="154" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A154" s="3">
         <v>7</v>
       </c>
@@ -14985,7 +14889,7 @@
       <c r="L154" s="8"/>
       <c r="M154" s="8"/>
     </row>
-    <row r="155" spans="1:13">
+    <row r="155" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A155" s="3">
         <v>7</v>
       </c>
@@ -15014,7 +14918,7 @@
       <c r="L155" s="8"/>
       <c r="M155" s="8"/>
     </row>
-    <row r="156" spans="1:13">
+    <row r="156" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A156" s="3">
         <v>7</v>
       </c>
@@ -15043,7 +14947,7 @@
       <c r="L156" s="8"/>
       <c r="M156" s="8"/>
     </row>
-    <row r="157" spans="1:13">
+    <row r="157" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A157" s="3">
         <v>7</v>
       </c>
@@ -15072,7 +14976,7 @@
       <c r="L157" s="8"/>
       <c r="M157" s="8"/>
     </row>
-    <row r="158" spans="1:13">
+    <row r="158" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A158" s="3">
         <v>7</v>
       </c>
@@ -15101,7 +15005,7 @@
       <c r="L158" s="8"/>
       <c r="M158" s="8"/>
     </row>
-    <row r="159" spans="1:13">
+    <row r="159" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A159" s="3">
         <v>7</v>
       </c>
@@ -15130,7 +15034,7 @@
       <c r="L159" s="8"/>
       <c r="M159" s="8"/>
     </row>
-    <row r="160" spans="1:13">
+    <row r="160" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A160" s="3">
         <v>7</v>
       </c>
@@ -15159,7 +15063,7 @@
       <c r="L160" s="8"/>
       <c r="M160" s="8"/>
     </row>
-    <row r="161" spans="1:13">
+    <row r="161" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A161" s="3">
         <v>7</v>
       </c>
@@ -15188,7 +15092,7 @@
       <c r="L161" s="7"/>
       <c r="M161" s="8"/>
     </row>
-    <row r="162" spans="1:13">
+    <row r="162" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A162" s="3">
         <v>7</v>
       </c>
@@ -15217,7 +15121,7 @@
       <c r="L162" s="7"/>
       <c r="M162" s="8"/>
     </row>
-    <row r="163" spans="1:13">
+    <row r="163" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A163" s="3">
         <v>7</v>
       </c>
@@ -15246,7 +15150,7 @@
       <c r="L163" s="8"/>
       <c r="M163" s="7"/>
     </row>
-    <row r="164" spans="1:13">
+    <row r="164" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A164" s="3">
         <v>7</v>
       </c>
@@ -15275,7 +15179,7 @@
       <c r="L164" s="8"/>
       <c r="M164" s="7"/>
     </row>
-    <row r="165" spans="1:13">
+    <row r="165" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A165" s="3">
         <v>7</v>
       </c>
@@ -15304,7 +15208,7 @@
       <c r="L165" s="8"/>
       <c r="M165" s="7"/>
     </row>
-    <row r="166" spans="1:13">
+    <row r="166" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A166" s="3">
         <v>7</v>
       </c>
@@ -15333,7 +15237,7 @@
       <c r="L166" s="8"/>
       <c r="M166" s="7"/>
     </row>
-    <row r="167" spans="1:13">
+    <row r="167" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A167" s="3">
         <v>7</v>
       </c>
@@ -15362,7 +15266,7 @@
       <c r="L167" s="8"/>
       <c r="M167" s="7"/>
     </row>
-    <row r="168" spans="1:13">
+    <row r="168" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A168" s="3">
         <v>7</v>
       </c>
@@ -15391,7 +15295,7 @@
       <c r="L168" s="8"/>
       <c r="M168" s="7"/>
     </row>
-    <row r="169" spans="1:13">
+    <row r="169" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A169" s="3">
         <v>7</v>
       </c>
@@ -15420,7 +15324,7 @@
       <c r="L169" s="8"/>
       <c r="M169" s="7"/>
     </row>
-    <row r="170" spans="1:13">
+    <row r="170" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A170" s="3">
         <v>7</v>
       </c>
@@ -15449,7 +15353,7 @@
       <c r="L170" s="7"/>
       <c r="M170" s="7"/>
     </row>
-    <row r="171" spans="1:13">
+    <row r="171" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A171" s="3">
         <v>7</v>
       </c>
@@ -15478,7 +15382,7 @@
       <c r="L171" s="8"/>
       <c r="M171" s="8"/>
     </row>
-    <row r="172" spans="1:13">
+    <row r="172" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A172" s="3">
         <v>7</v>
       </c>
@@ -15507,7 +15411,7 @@
       <c r="L172" s="8"/>
       <c r="M172" s="8"/>
     </row>
-    <row r="173" spans="1:13">
+    <row r="173" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A173" s="3">
         <v>7</v>
       </c>
@@ -15536,7 +15440,7 @@
       <c r="L173" s="7"/>
       <c r="M173" s="7"/>
     </row>
-    <row r="174" spans="1:13">
+    <row r="174" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A174" s="3">
         <v>7</v>
       </c>
@@ -15565,7 +15469,7 @@
       <c r="L174" s="7"/>
       <c r="M174" s="7"/>
     </row>
-    <row r="175" spans="1:13">
+    <row r="175" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A175" s="3">
         <v>7</v>
       </c>
@@ -15594,7 +15498,7 @@
       <c r="L175" s="7"/>
       <c r="M175" s="7"/>
     </row>
-    <row r="176" spans="1:13">
+    <row r="176" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A176" s="3">
         <v>7</v>
       </c>
@@ -15623,7 +15527,7 @@
       <c r="L176" s="7"/>
       <c r="M176" s="7"/>
     </row>
-    <row r="177" spans="1:13">
+    <row r="177" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A177" s="3">
         <v>7</v>
       </c>
@@ -15652,7 +15556,7 @@
       <c r="L177" s="9"/>
       <c r="M177" s="9"/>
     </row>
-    <row r="178" spans="1:13">
+    <row r="178" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A178" s="3">
         <v>8</v>
       </c>
@@ -15681,7 +15585,7 @@
       <c r="L178" s="7"/>
       <c r="M178" s="7"/>
     </row>
-    <row r="179" spans="1:13">
+    <row r="179" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A179" s="3">
         <v>8</v>
       </c>
@@ -15710,7 +15614,7 @@
       <c r="L179" s="7"/>
       <c r="M179" s="7"/>
     </row>
-    <row r="180" spans="1:13">
+    <row r="180" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A180" s="3">
         <v>8</v>
       </c>
@@ -15739,7 +15643,7 @@
       <c r="L180" s="7"/>
       <c r="M180" s="7"/>
     </row>
-    <row r="181" spans="1:13">
+    <row r="181" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A181" s="3">
         <v>8</v>
       </c>
@@ -15768,7 +15672,7 @@
       <c r="L181" s="7"/>
       <c r="M181" s="7"/>
     </row>
-    <row r="182" spans="1:13">
+    <row r="182" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A182" s="3">
         <v>8</v>
       </c>
@@ -15797,7 +15701,7 @@
       <c r="L182" s="7"/>
       <c r="M182" s="7"/>
     </row>
-    <row r="183" spans="1:13">
+    <row r="183" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A183" s="3">
         <v>8</v>
       </c>
@@ -15826,7 +15730,7 @@
       <c r="L183" s="7"/>
       <c r="M183" s="7"/>
     </row>
-    <row r="184" spans="1:13">
+    <row r="184" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A184" s="3">
         <v>8</v>
       </c>
@@ -15855,7 +15759,7 @@
       <c r="L184" s="7"/>
       <c r="M184" s="7"/>
     </row>
-    <row r="185" spans="1:13">
+    <row r="185" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A185" s="3">
         <v>8</v>
       </c>
@@ -15884,7 +15788,7 @@
       <c r="L185" s="7"/>
       <c r="M185" s="7"/>
     </row>
-    <row r="186" spans="1:13">
+    <row r="186" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A186" s="3">
         <v>8</v>
       </c>
@@ -15913,7 +15817,7 @@
       <c r="L186" s="7"/>
       <c r="M186" s="7"/>
     </row>
-    <row r="187" spans="1:13">
+    <row r="187" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A187" s="3">
         <v>8</v>
       </c>
@@ -15942,7 +15846,7 @@
       <c r="L187" s="7"/>
       <c r="M187" s="7"/>
     </row>
-    <row r="188" spans="1:13">
+    <row r="188" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A188" s="3">
         <v>8</v>
       </c>
@@ -15971,7 +15875,7 @@
       <c r="L188" s="7"/>
       <c r="M188" s="7"/>
     </row>
-    <row r="189" spans="1:13">
+    <row r="189" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A189" s="3">
         <v>8</v>
       </c>
@@ -16000,7 +15904,7 @@
       <c r="L189" s="7"/>
       <c r="M189" s="7"/>
     </row>
-    <row r="190" spans="1:13">
+    <row r="190" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A190" s="3">
         <v>8</v>
       </c>
@@ -16029,7 +15933,7 @@
       <c r="L190" s="7"/>
       <c r="M190" s="7"/>
     </row>
-    <row r="191" spans="1:13">
+    <row r="191" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A191" s="3">
         <v>9</v>
       </c>
@@ -16058,7 +15962,7 @@
       <c r="L191" s="7"/>
       <c r="M191" s="7"/>
     </row>
-    <row r="192" spans="1:13">
+    <row r="192" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A192" s="3">
         <v>9</v>
       </c>
@@ -16087,7 +15991,7 @@
       <c r="L192" s="7"/>
       <c r="M192" s="7"/>
     </row>
-    <row r="193" spans="1:13">
+    <row r="193" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A193" s="3">
         <v>9</v>
       </c>
@@ -16116,7 +16020,7 @@
       <c r="L193" s="7"/>
       <c r="M193" s="7"/>
     </row>
-    <row r="194" spans="1:13">
+    <row r="194" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A194" s="3">
         <v>9</v>
       </c>
@@ -16145,7 +16049,7 @@
       <c r="L194" s="7"/>
       <c r="M194" s="7"/>
     </row>
-    <row r="195" spans="1:13">
+    <row r="195" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A195" s="3">
         <v>9</v>
       </c>
@@ -16174,7 +16078,7 @@
       <c r="L195" s="16"/>
       <c r="M195" s="16"/>
     </row>
-    <row r="196" spans="1:13">
+    <row r="196" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A196" s="3">
         <v>9</v>
       </c>
@@ -16203,7 +16107,7 @@
       <c r="L196" s="7"/>
       <c r="M196" s="7"/>
     </row>
-    <row r="197" spans="1:13">
+    <row r="197" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A197" s="3">
         <v>9</v>
       </c>
@@ -16232,7 +16136,7 @@
       <c r="L197" s="7"/>
       <c r="M197" s="7"/>
     </row>
-    <row r="198" spans="1:13">
+    <row r="198" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A198" s="3">
         <v>9</v>
       </c>
@@ -16261,7 +16165,7 @@
       <c r="L198" s="7"/>
       <c r="M198" s="7"/>
     </row>
-    <row r="199" spans="1:13">
+    <row r="199" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A199" s="3">
         <v>9</v>
       </c>
@@ -16290,7 +16194,7 @@
       <c r="L199" s="7"/>
       <c r="M199" s="7"/>
     </row>
-    <row r="200" spans="1:13">
+    <row r="200" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A200" s="3">
         <v>9</v>
       </c>
@@ -16319,7 +16223,7 @@
       <c r="L200" s="7"/>
       <c r="M200" s="7"/>
     </row>
-    <row r="201" spans="1:13">
+    <row r="201" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A201" s="3">
         <v>9</v>
       </c>
@@ -16348,7 +16252,7 @@
       <c r="L201" s="7"/>
       <c r="M201" s="7"/>
     </row>
-    <row r="202" spans="1:13">
+    <row r="202" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A202" s="3">
         <v>9</v>
       </c>
@@ -16377,7 +16281,7 @@
       <c r="L202" s="7"/>
       <c r="M202" s="7"/>
     </row>
-    <row r="203" spans="1:13">
+    <row r="203" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A203" s="3">
         <v>9</v>
       </c>
@@ -16406,7 +16310,7 @@
       <c r="L203" s="7"/>
       <c r="M203" s="7"/>
     </row>
-    <row r="204" spans="1:13">
+    <row r="204" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A204" s="3">
         <v>9</v>
       </c>
@@ -16435,7 +16339,7 @@
       <c r="L204" s="7"/>
       <c r="M204" s="7"/>
     </row>
-    <row r="205" spans="1:13">
+    <row r="205" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A205" s="3">
         <v>9</v>
       </c>
@@ -16464,7 +16368,7 @@
       <c r="L205" s="7"/>
       <c r="M205" s="7"/>
     </row>
-    <row r="206" spans="1:13">
+    <row r="206" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A206" s="3">
         <v>9</v>
       </c>
@@ -16493,7 +16397,7 @@
       <c r="L206" s="7"/>
       <c r="M206" s="7"/>
     </row>
-    <row r="207" spans="1:13">
+    <row r="207" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A207" s="3">
         <v>9</v>
       </c>
@@ -16522,7 +16426,7 @@
       <c r="L207" s="7"/>
       <c r="M207" s="7"/>
     </row>
-    <row r="208" spans="1:13">
+    <row r="208" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A208" s="3">
         <v>9</v>
       </c>
@@ -16551,7 +16455,7 @@
       <c r="L208" s="7"/>
       <c r="M208" s="7"/>
     </row>
-    <row r="209" spans="1:13">
+    <row r="209" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A209" s="3">
         <v>9</v>
       </c>
@@ -16580,7 +16484,7 @@
       <c r="L209" s="7"/>
       <c r="M209" s="7"/>
     </row>
-    <row r="210" spans="1:13">
+    <row r="210" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A210" s="3">
         <v>9</v>
       </c>
@@ -16609,7 +16513,7 @@
       <c r="L210" s="7"/>
       <c r="M210" s="7"/>
     </row>
-    <row r="211" spans="1:13">
+    <row r="211" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A211" s="3">
         <v>9</v>
       </c>
@@ -16638,7 +16542,7 @@
       <c r="L211" s="9"/>
       <c r="M211" s="9"/>
     </row>
-    <row r="212" spans="1:13">
+    <row r="212" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A212" s="3">
         <v>9</v>
       </c>
@@ -16667,7 +16571,7 @@
       <c r="L212" s="7"/>
       <c r="M212" s="7"/>
     </row>
-    <row r="213" spans="1:13">
+    <row r="213" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A213" s="3">
         <v>9</v>
       </c>
@@ -16696,7 +16600,7 @@
       <c r="L213" s="7"/>
       <c r="M213" s="7"/>
     </row>
-    <row r="214" spans="1:13">
+    <row r="214" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A214" s="3">
         <v>9</v>
       </c>
@@ -16725,7 +16629,7 @@
       <c r="L214" s="7"/>
       <c r="M214" s="7"/>
     </row>
-    <row r="215" spans="1:13">
+    <row r="215" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A215" s="3">
         <v>9</v>
       </c>
@@ -16754,7 +16658,7 @@
       <c r="L215" s="7"/>
       <c r="M215" s="7"/>
     </row>
-    <row r="216" spans="1:13">
+    <row r="216" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A216" s="3">
         <v>10</v>
       </c>
@@ -16783,7 +16687,7 @@
       <c r="L216" s="7"/>
       <c r="M216" s="7"/>
     </row>
-    <row r="217" spans="1:13">
+    <row r="217" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A217" s="3">
         <v>10</v>
       </c>
@@ -16812,7 +16716,7 @@
       <c r="L217" s="7"/>
       <c r="M217" s="7"/>
     </row>
-    <row r="218" spans="1:13">
+    <row r="218" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A218" s="3">
         <v>10</v>
       </c>
@@ -16841,7 +16745,7 @@
       <c r="L218" s="7"/>
       <c r="M218" s="7"/>
     </row>
-    <row r="219" spans="1:13">
+    <row r="219" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A219" s="3">
         <v>10</v>
       </c>
@@ -16870,7 +16774,7 @@
       <c r="L219" s="7"/>
       <c r="M219" s="7"/>
     </row>
-    <row r="220" spans="1:13">
+    <row r="220" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A220" s="3">
         <v>10</v>
       </c>
@@ -16899,7 +16803,7 @@
       <c r="L220" s="7"/>
       <c r="M220" s="7"/>
     </row>
-    <row r="221" spans="1:13">
+    <row r="221" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A221" s="3">
         <v>10</v>
       </c>
@@ -16928,7 +16832,7 @@
       <c r="L221" s="7"/>
       <c r="M221" s="7"/>
     </row>
-    <row r="222" spans="1:13">
+    <row r="222" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A222" s="3">
         <v>10</v>
       </c>
@@ -16957,7 +16861,7 @@
       <c r="L222" s="7"/>
       <c r="M222" s="7"/>
     </row>
-    <row r="223" spans="1:13">
+    <row r="223" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A223" s="3">
         <v>10</v>
       </c>
@@ -16986,7 +16890,7 @@
       <c r="L223" s="7"/>
       <c r="M223" s="7"/>
     </row>
-    <row r="224" spans="1:13">
+    <row r="224" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A224" s="3">
         <v>10</v>
       </c>
@@ -17015,7 +16919,7 @@
       <c r="L224" s="7"/>
       <c r="M224" s="7"/>
     </row>
-    <row r="225" spans="1:13">
+    <row r="225" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A225" s="3">
         <v>10</v>
       </c>
@@ -17044,7 +16948,7 @@
       <c r="L225" s="7"/>
       <c r="M225" s="7"/>
     </row>
-    <row r="226" spans="1:13">
+    <row r="226" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A226" s="3">
         <v>10</v>
       </c>
@@ -17073,7 +16977,7 @@
       <c r="L226" s="7"/>
       <c r="M226" s="7"/>
     </row>
-    <row r="227" spans="1:13">
+    <row r="227" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A227" s="3">
         <v>10</v>
       </c>
@@ -17102,7 +17006,7 @@
       <c r="L227" s="7"/>
       <c r="M227" s="7"/>
     </row>
-    <row r="228" spans="1:13">
+    <row r="228" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A228" s="3">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
Create 3.7 Listing for MSSQL & PostgreSQL
</commit_message>
<xml_diff>
--- a/Listings.xlsx
+++ b/Listings.xlsx
@@ -2161,16 +2161,16 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Doug:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
+          </rPr>
+          <t>Doug:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Listing is Oracle-specific</t>
@@ -2185,70 +2185,70 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Doug:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
+          </rPr>
+          <t>Doug:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Listing is Oracle-specific</t>
         </r>
       </text>
     </comment>
-    <comment ref="J55" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Doug:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
+    <comment ref="J55" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Ben Clothier:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Implemented as an indexed view.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K55" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Doug:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Listing is Oracle-specific</t>
         </r>
       </text>
     </comment>
-    <comment ref="K55" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Doug:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Listing is Oracle-specific</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="L55" authorId="2">
       <text>
         <r>
@@ -2257,7 +2257,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Ben Clothier:</t>
         </r>
@@ -2266,35 +2266,11 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Cannot test due to a licensing restriction.
 </t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="M55" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Doug:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Listing is Oracle-specific</t>
         </r>
       </text>
     </comment>
@@ -9869,9 +9845,6 @@
     <t>Item20DB2Example</t>
   </si>
   <si>
-    <t>Item20OracleExample</t>
-  </si>
-  <si>
     <t>Item27Example</t>
   </si>
   <si>
@@ -9900,13 +9873,16 @@
   </si>
   <si>
     <t>&lt;No listings in item&gt;</t>
+  </si>
+  <si>
+    <t>Item20***Example</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -9987,6 +9963,32 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="7">
@@ -10406,7 +10408,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -10420,8 +10422,8 @@
   <dimension ref="A1:M228"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I10" sqref="I10"/>
+      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L57" sqref="L57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10456,10 +10458,10 @@
         <v>441</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="H1" s="5" t="s">
         <v>456</v>
@@ -10488,7 +10490,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>440</v>
@@ -10500,7 +10502,7 @@
         <v>476</v>
       </c>
       <c r="G2" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -10520,10 +10522,10 @@
         <v>442</v>
       </c>
       <c r="F3" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G3" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H3" s="7"/>
       <c r="I3" s="7"/>
@@ -10549,10 +10551,10 @@
         <v>443</v>
       </c>
       <c r="F4" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G4" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H4" s="7"/>
       <c r="I4" s="7"/>
@@ -10578,10 +10580,10 @@
         <v>465</v>
       </c>
       <c r="F5" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G5" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H5" s="7"/>
       <c r="I5" s="7"/>
@@ -10607,10 +10609,10 @@
         <v>465</v>
       </c>
       <c r="F6" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G6" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H6" s="7"/>
       <c r="I6" s="7"/>
@@ -10636,10 +10638,10 @@
         <v>444</v>
       </c>
       <c r="F7" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G7" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H7" s="7"/>
       <c r="I7" s="7"/>
@@ -10665,10 +10667,10 @@
         <v>444</v>
       </c>
       <c r="F8" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G8" s="15" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="H8" s="8"/>
       <c r="I8" s="8"/>
@@ -10694,10 +10696,10 @@
         <v>444</v>
       </c>
       <c r="F9" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G9" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H9" s="7"/>
       <c r="I9" s="8"/>
@@ -10723,10 +10725,10 @@
         <v>444</v>
       </c>
       <c r="F10" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G10" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H10" s="7"/>
       <c r="I10" s="8"/>
@@ -10752,10 +10754,10 @@
         <v>444</v>
       </c>
       <c r="F11" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G11" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H11" s="7"/>
       <c r="I11" s="7"/>
@@ -10781,10 +10783,10 @@
         <v>444</v>
       </c>
       <c r="F12" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G12" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H12" s="7"/>
       <c r="I12" s="7"/>
@@ -10810,10 +10812,10 @@
         <v>444</v>
       </c>
       <c r="F13" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G13" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H13" s="7"/>
       <c r="I13" s="8"/>
@@ -10839,10 +10841,10 @@
         <v>444</v>
       </c>
       <c r="F14" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G14" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H14" s="7"/>
       <c r="I14" s="7"/>
@@ -10859,7 +10861,7 @@
         <v>8</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>440</v>
@@ -10871,7 +10873,7 @@
         <v>476</v>
       </c>
       <c r="G15" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -10882,7 +10884,7 @@
         <v>9</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>440</v>
@@ -10894,7 +10896,7 @@
         <v>476</v>
       </c>
       <c r="G16" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
@@ -10914,10 +10916,10 @@
         <v>444</v>
       </c>
       <c r="F17" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G17" s="15" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="H17" s="7"/>
       <c r="I17" s="8"/>
@@ -10943,10 +10945,10 @@
         <v>444</v>
       </c>
       <c r="F18" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G18" s="15" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="H18" s="7"/>
       <c r="I18" s="8"/>
@@ -10972,10 +10974,10 @@
         <v>444</v>
       </c>
       <c r="F19" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G19" s="15" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="H19" s="8"/>
       <c r="I19" s="7"/>
@@ -11001,10 +11003,10 @@
         <v>444</v>
       </c>
       <c r="F20" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G20" s="15" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="H20" s="8"/>
       <c r="I20" s="8"/>
@@ -11030,10 +11032,10 @@
         <v>444</v>
       </c>
       <c r="F21" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G21" s="15" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="H21" s="8"/>
       <c r="I21" s="8"/>
@@ -11059,10 +11061,10 @@
         <v>444</v>
       </c>
       <c r="F22" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G22" s="15" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="H22" s="8"/>
       <c r="I22" s="8"/>
@@ -11088,10 +11090,10 @@
         <v>444</v>
       </c>
       <c r="F23" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G23" s="15" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="H23" s="8"/>
       <c r="I23" s="8"/>
@@ -11120,7 +11122,7 @@
         <v>42</v>
       </c>
       <c r="G24" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H24" s="7"/>
       <c r="I24" s="9"/>
@@ -11149,7 +11151,7 @@
         <v>42</v>
       </c>
       <c r="G25" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H25" s="7"/>
       <c r="I25" s="7"/>
@@ -11178,7 +11180,7 @@
         <v>42</v>
       </c>
       <c r="G26" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H26" s="7"/>
       <c r="I26" s="7"/>
@@ -11204,10 +11206,10 @@
         <v>444</v>
       </c>
       <c r="F27" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G27" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H27" s="7"/>
       <c r="I27" s="7"/>
@@ -11233,10 +11235,10 @@
         <v>444</v>
       </c>
       <c r="F28" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G28" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H28" s="7"/>
       <c r="I28" s="7"/>
@@ -11262,10 +11264,10 @@
         <v>444</v>
       </c>
       <c r="F29" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G29" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H29" s="7"/>
       <c r="I29" s="7"/>
@@ -11291,10 +11293,10 @@
         <v>444</v>
       </c>
       <c r="F30" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G30" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H30" s="7"/>
       <c r="I30" s="7"/>
@@ -11320,10 +11322,10 @@
         <v>444</v>
       </c>
       <c r="F31" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G31" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H31" s="7"/>
       <c r="I31" s="7"/>
@@ -11349,10 +11351,10 @@
         <v>444</v>
       </c>
       <c r="F32" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G32" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H32" s="7"/>
       <c r="I32" s="7"/>
@@ -11378,10 +11380,10 @@
         <v>444</v>
       </c>
       <c r="F33" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G33" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H33" s="7"/>
       <c r="I33" s="7"/>
@@ -11407,10 +11409,10 @@
         <v>444</v>
       </c>
       <c r="F34" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G34" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H34" s="7"/>
       <c r="I34" s="8"/>
@@ -11436,10 +11438,10 @@
         <v>444</v>
       </c>
       <c r="F35" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G35" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H35" s="9"/>
       <c r="I35" s="8"/>
@@ -11468,7 +11470,7 @@
         <v>62</v>
       </c>
       <c r="G36" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H36" s="9"/>
       <c r="I36" s="7"/>
@@ -11494,10 +11496,10 @@
         <v>444</v>
       </c>
       <c r="F37" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G37" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H37" s="7"/>
       <c r="I37" s="8"/>
@@ -11526,7 +11528,7 @@
         <v>66</v>
       </c>
       <c r="G38" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H38" s="7"/>
       <c r="I38" s="8"/>
@@ -11555,7 +11557,7 @@
         <v>66</v>
       </c>
       <c r="G39" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H39" s="7"/>
       <c r="I39" s="8"/>
@@ -11581,10 +11583,10 @@
         <v>444</v>
       </c>
       <c r="F40" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G40" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H40" s="7"/>
       <c r="I40" s="8"/>
@@ -11610,10 +11612,10 @@
         <v>444</v>
       </c>
       <c r="F41" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G41" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H41" s="7"/>
       <c r="I41" s="8"/>
@@ -11630,7 +11632,7 @@
         <v>15</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="D42" s="4" t="s">
         <v>440</v>
@@ -11642,7 +11644,7 @@
         <v>476</v>
       </c>
       <c r="G42" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="J42" s="11"/>
     </row>
@@ -11654,7 +11656,7 @@
         <v>16</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="D43" s="4" t="s">
         <v>440</v>
@@ -11666,7 +11668,7 @@
         <v>476</v>
       </c>
       <c r="G43" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="J43" s="11"/>
     </row>
@@ -11687,10 +11689,10 @@
         <v>444</v>
       </c>
       <c r="F44" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G44" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H44" s="7"/>
       <c r="I44" s="7"/>
@@ -11716,10 +11718,10 @@
         <v>444</v>
       </c>
       <c r="F45" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G45" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H45" s="7"/>
       <c r="I45" s="7"/>
@@ -11745,10 +11747,10 @@
         <v>444</v>
       </c>
       <c r="F46" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G46" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H46" s="7"/>
       <c r="I46" s="8"/>
@@ -11774,10 +11776,10 @@
         <v>444</v>
       </c>
       <c r="F47" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G47" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H47" s="7"/>
       <c r="I47" s="9"/>
@@ -11803,10 +11805,10 @@
         <v>444</v>
       </c>
       <c r="F48" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G48" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H48" s="7"/>
       <c r="I48" s="7"/>
@@ -11832,10 +11834,10 @@
         <v>445</v>
       </c>
       <c r="F49" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G49" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H49" s="7"/>
       <c r="I49" s="9"/>
@@ -11861,10 +11863,10 @@
         <v>445</v>
       </c>
       <c r="F50" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G50" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H50" s="7"/>
       <c r="I50" s="9"/>
@@ -11890,10 +11892,10 @@
         <v>444</v>
       </c>
       <c r="F51" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G51" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H51" s="7"/>
       <c r="I51" s="9"/>
@@ -11919,10 +11921,10 @@
         <v>444</v>
       </c>
       <c r="F52" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G52" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H52" s="7"/>
       <c r="I52" s="7"/>
@@ -11948,10 +11950,10 @@
         <v>466</v>
       </c>
       <c r="F53" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G53" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H53" s="7"/>
       <c r="I53" s="7"/>
@@ -11980,7 +11982,7 @@
         <v>94</v>
       </c>
       <c r="G54" s="15" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="H54" s="7"/>
       <c r="I54" s="8"/>
@@ -12003,20 +12005,20 @@
         <v>97</v>
       </c>
       <c r="E55" s="6" t="s">
-        <v>481</v>
+        <v>491</v>
       </c>
       <c r="F55" t="s">
         <v>96</v>
       </c>
       <c r="G55" s="15" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="H55" s="8"/>
       <c r="I55" s="8"/>
-      <c r="J55" s="8"/>
+      <c r="J55" s="9"/>
       <c r="K55" s="8"/>
       <c r="L55" s="9"/>
-      <c r="M55" s="8"/>
+      <c r="M55" s="7"/>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" s="3">
@@ -12035,10 +12037,10 @@
         <v>446</v>
       </c>
       <c r="F56" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G56" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H56" s="7"/>
       <c r="I56" s="7"/>
@@ -12064,10 +12066,10 @@
         <v>446</v>
       </c>
       <c r="F57" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G57" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H57" s="7"/>
       <c r="I57" s="7"/>
@@ -12093,10 +12095,10 @@
         <v>446</v>
       </c>
       <c r="F58" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G58" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H58" s="7"/>
       <c r="I58" s="7"/>
@@ -12122,10 +12124,10 @@
         <v>446</v>
       </c>
       <c r="F59" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G59" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H59" s="7"/>
       <c r="I59" s="7"/>
@@ -12151,10 +12153,10 @@
         <v>444</v>
       </c>
       <c r="F60" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G60" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H60" s="7"/>
       <c r="I60" s="8"/>
@@ -12180,10 +12182,10 @@
         <v>444</v>
       </c>
       <c r="F61" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G61" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H61" s="7"/>
       <c r="I61" s="7"/>
@@ -12209,10 +12211,10 @@
         <v>444</v>
       </c>
       <c r="F62" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G62" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H62" s="7"/>
       <c r="I62" s="8"/>
@@ -12238,10 +12240,10 @@
         <v>444</v>
       </c>
       <c r="F63" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G63" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H63" s="7"/>
       <c r="I63" s="7"/>
@@ -12267,10 +12269,10 @@
         <v>444</v>
       </c>
       <c r="F64" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G64" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H64" s="7"/>
       <c r="I64" s="7"/>
@@ -12296,10 +12298,10 @@
         <v>444</v>
       </c>
       <c r="F65" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G65" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H65" s="7"/>
       <c r="I65" s="7"/>
@@ -12328,7 +12330,7 @@
         <v>476</v>
       </c>
       <c r="G66" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H66" s="16"/>
       <c r="I66" s="8"/>
@@ -12354,10 +12356,10 @@
         <v>444</v>
       </c>
       <c r="F67" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G67" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H67" s="7"/>
       <c r="I67" s="8"/>
@@ -12383,10 +12385,10 @@
         <v>444</v>
       </c>
       <c r="F68" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G68" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H68" s="7"/>
       <c r="I68" s="7"/>
@@ -12412,10 +12414,10 @@
         <v>444</v>
       </c>
       <c r="F69" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G69" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H69" s="7"/>
       <c r="I69" s="8"/>
@@ -12441,10 +12443,10 @@
         <v>444</v>
       </c>
       <c r="F70" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G70" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H70" s="7"/>
       <c r="I70" s="7"/>
@@ -12470,10 +12472,10 @@
         <v>444</v>
       </c>
       <c r="F71" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G71" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H71" s="7"/>
       <c r="I71" s="7"/>
@@ -12499,10 +12501,10 @@
         <v>444</v>
       </c>
       <c r="F72" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G72" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H72" s="7"/>
       <c r="I72" s="8"/>
@@ -12528,10 +12530,10 @@
         <v>444</v>
       </c>
       <c r="F73" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G73" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H73" s="7"/>
       <c r="I73" s="7"/>
@@ -12557,10 +12559,10 @@
         <v>444</v>
       </c>
       <c r="F74" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G74" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H74" s="7"/>
       <c r="I74" s="7"/>
@@ -12586,10 +12588,10 @@
         <v>444</v>
       </c>
       <c r="F75" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G75" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H75" s="7"/>
       <c r="I75" s="8"/>
@@ -12615,10 +12617,10 @@
         <v>444</v>
       </c>
       <c r="F76" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G76" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H76" s="7"/>
       <c r="I76" s="7"/>
@@ -12644,10 +12646,10 @@
         <v>444</v>
       </c>
       <c r="F77" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G77" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H77" s="7"/>
       <c r="I77" s="7"/>
@@ -12673,10 +12675,10 @@
         <v>444</v>
       </c>
       <c r="F78" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G78" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H78" s="7"/>
       <c r="I78" s="7"/>
@@ -12702,10 +12704,10 @@
         <v>444</v>
       </c>
       <c r="F79" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G79" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H79" s="7"/>
       <c r="I79" s="7"/>
@@ -12728,13 +12730,13 @@
         <v>146</v>
       </c>
       <c r="E80" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="F80" t="s">
         <v>145</v>
       </c>
       <c r="G80" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H80" s="7"/>
       <c r="I80" s="7"/>
@@ -12757,13 +12759,13 @@
         <v>148</v>
       </c>
       <c r="E81" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="F81" t="s">
         <v>145</v>
       </c>
       <c r="G81" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H81" s="7"/>
       <c r="I81" s="7"/>
@@ -12786,13 +12788,13 @@
         <v>150</v>
       </c>
       <c r="E82" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="F82" t="s">
         <v>145</v>
       </c>
       <c r="G82" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H82" s="7"/>
       <c r="I82" s="8"/>
@@ -12815,13 +12817,13 @@
         <v>152</v>
       </c>
       <c r="E83" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="F83" t="s">
         <v>145</v>
       </c>
       <c r="G83" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H83" s="7"/>
       <c r="I83" s="7"/>
@@ -12844,13 +12846,13 @@
         <v>154</v>
       </c>
       <c r="E84" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="F84" t="s">
         <v>145</v>
       </c>
       <c r="G84" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H84" s="7"/>
       <c r="I84" s="7"/>
@@ -12873,13 +12875,13 @@
         <v>156</v>
       </c>
       <c r="E85" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="F85" t="s">
         <v>145</v>
       </c>
       <c r="G85" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H85" s="7"/>
       <c r="I85" s="7"/>
@@ -12902,13 +12904,13 @@
         <v>158</v>
       </c>
       <c r="E86" s="6" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="F86" t="s">
         <v>145</v>
       </c>
       <c r="G86" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H86" s="7"/>
       <c r="I86" s="7"/>
@@ -12931,13 +12933,13 @@
         <v>160</v>
       </c>
       <c r="E87" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="F87" t="s">
         <v>159</v>
       </c>
       <c r="G87" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H87" s="7"/>
       <c r="I87" s="8"/>
@@ -12960,13 +12962,13 @@
         <v>162</v>
       </c>
       <c r="E88" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="F88" t="s">
         <v>159</v>
       </c>
       <c r="G88" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H88" s="7"/>
       <c r="I88" s="7"/>
@@ -12989,13 +12991,13 @@
         <v>164</v>
       </c>
       <c r="E89" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="F89" t="s">
         <v>159</v>
       </c>
       <c r="G89" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H89" s="7"/>
       <c r="I89" s="7"/>
@@ -13018,13 +13020,13 @@
         <v>166</v>
       </c>
       <c r="E90" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="F90" t="s">
         <v>159</v>
       </c>
       <c r="G90" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H90" s="7"/>
       <c r="I90" s="7"/>
@@ -13047,13 +13049,13 @@
         <v>168</v>
       </c>
       <c r="E91" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="F91" t="s">
         <v>159</v>
       </c>
       <c r="G91" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H91" s="7"/>
       <c r="I91" s="7"/>
@@ -13076,13 +13078,13 @@
         <v>170</v>
       </c>
       <c r="E92" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="F92" t="s">
         <v>159</v>
       </c>
       <c r="G92" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H92" s="7"/>
       <c r="I92" s="7"/>
@@ -13105,13 +13107,13 @@
         <v>172</v>
       </c>
       <c r="E93" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="F93" t="s">
         <v>159</v>
       </c>
       <c r="G93" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H93" s="7"/>
       <c r="I93" s="7"/>
@@ -13134,13 +13136,13 @@
         <v>174</v>
       </c>
       <c r="E94" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="F94" t="s">
         <v>159</v>
       </c>
       <c r="G94" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H94" s="7"/>
       <c r="I94" s="7"/>
@@ -13163,13 +13165,13 @@
         <v>176</v>
       </c>
       <c r="E95" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="F95" t="s">
         <v>159</v>
       </c>
       <c r="G95" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H95" s="7"/>
       <c r="I95" s="7"/>
@@ -13192,13 +13194,13 @@
         <v>178</v>
       </c>
       <c r="E96" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="F96" t="s">
         <v>159</v>
       </c>
       <c r="G96" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H96" s="7"/>
       <c r="I96" s="7"/>
@@ -13224,10 +13226,10 @@
         <v>444</v>
       </c>
       <c r="F97" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G97" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H97" s="7"/>
       <c r="I97" s="7"/>
@@ -13253,10 +13255,10 @@
         <v>444</v>
       </c>
       <c r="F98" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G98" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H98" s="7"/>
       <c r="I98" s="7"/>
@@ -13282,10 +13284,10 @@
         <v>444</v>
       </c>
       <c r="F99" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G99" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H99" s="7"/>
       <c r="I99" s="7"/>
@@ -13314,7 +13316,7 @@
         <v>476</v>
       </c>
       <c r="G100" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H100" s="16"/>
       <c r="I100" s="16"/>
@@ -13343,7 +13345,7 @@
         <v>476</v>
       </c>
       <c r="G101" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H101" s="16"/>
       <c r="I101" s="16"/>
@@ -13372,7 +13374,7 @@
         <v>476</v>
       </c>
       <c r="G102" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H102" s="16"/>
       <c r="I102" s="16"/>
@@ -13398,10 +13400,10 @@
         <v>447</v>
       </c>
       <c r="F103" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G103" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H103" s="7"/>
       <c r="I103" s="8"/>
@@ -13427,10 +13429,10 @@
         <v>447</v>
       </c>
       <c r="F104" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G104" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H104" s="7"/>
       <c r="I104" s="8"/>
@@ -13456,10 +13458,10 @@
         <v>447</v>
       </c>
       <c r="F105" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G105" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H105" s="7"/>
       <c r="I105" s="8"/>
@@ -13485,10 +13487,10 @@
         <v>447</v>
       </c>
       <c r="F106" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G106" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H106" s="7"/>
       <c r="I106" s="7"/>
@@ -13514,10 +13516,10 @@
         <v>444</v>
       </c>
       <c r="F107" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G107" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H107" s="7"/>
       <c r="I107" s="7"/>
@@ -13543,10 +13545,10 @@
         <v>444</v>
       </c>
       <c r="F108" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G108" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H108" s="7"/>
       <c r="I108" s="7"/>
@@ -13572,10 +13574,10 @@
         <v>444</v>
       </c>
       <c r="F109" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G109" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H109" s="7"/>
       <c r="I109" s="7"/>
@@ -13601,10 +13603,10 @@
         <v>444</v>
       </c>
       <c r="F110" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G110" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H110" s="8"/>
       <c r="I110" s="8"/>
@@ -13630,10 +13632,10 @@
         <v>444</v>
       </c>
       <c r="F111" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G111" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H111" s="7"/>
       <c r="I111" s="7"/>
@@ -13659,10 +13661,10 @@
         <v>444</v>
       </c>
       <c r="F112" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G112" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H112" s="7"/>
       <c r="I112" s="7"/>
@@ -13688,10 +13690,10 @@
         <v>444</v>
       </c>
       <c r="F113" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G113" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H113" s="7"/>
       <c r="I113" s="7"/>
@@ -13717,10 +13719,10 @@
         <v>444</v>
       </c>
       <c r="F114" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G114" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H114" s="9"/>
       <c r="I114" s="9"/>
@@ -13746,10 +13748,10 @@
         <v>444</v>
       </c>
       <c r="F115" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G115" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H115" s="9"/>
       <c r="I115" s="9"/>
@@ -13775,10 +13777,10 @@
         <v>448</v>
       </c>
       <c r="F116" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G116" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H116" s="7"/>
       <c r="I116" s="7"/>
@@ -13804,10 +13806,10 @@
         <v>448</v>
       </c>
       <c r="F117" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G117" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H117" s="7"/>
       <c r="I117" s="7"/>
@@ -13833,10 +13835,10 @@
         <v>448</v>
       </c>
       <c r="F118" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G118" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H118" s="7"/>
       <c r="I118" s="7"/>
@@ -13862,10 +13864,10 @@
         <v>448</v>
       </c>
       <c r="F119" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G119" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H119" s="7"/>
       <c r="I119" s="7"/>
@@ -13891,10 +13893,10 @@
         <v>449</v>
       </c>
       <c r="F120" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G120" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H120" s="7"/>
       <c r="I120" s="7"/>
@@ -13920,10 +13922,10 @@
         <v>449</v>
       </c>
       <c r="F121" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G121" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H121" s="7"/>
       <c r="I121" s="7"/>
@@ -13949,10 +13951,10 @@
         <v>449</v>
       </c>
       <c r="F122" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G122" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H122" s="7"/>
       <c r="I122" s="7"/>
@@ -13978,10 +13980,10 @@
         <v>449</v>
       </c>
       <c r="F123" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G123" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H123" s="9"/>
       <c r="I123" s="7"/>
@@ -14007,10 +14009,10 @@
         <v>449</v>
       </c>
       <c r="F124" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G124" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H124" s="9"/>
       <c r="I124" s="7"/>
@@ -14036,10 +14038,10 @@
         <v>449</v>
       </c>
       <c r="F125" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G125" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H125" s="9"/>
       <c r="I125" s="7"/>
@@ -14065,10 +14067,10 @@
         <v>450</v>
       </c>
       <c r="F126" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G126" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H126" s="7"/>
       <c r="I126" s="7"/>
@@ -14094,10 +14096,10 @@
         <v>450</v>
       </c>
       <c r="F127" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G127" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H127" s="7"/>
       <c r="I127" s="9"/>
@@ -14123,10 +14125,10 @@
         <v>444</v>
       </c>
       <c r="F128" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G128" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H128" s="7"/>
       <c r="I128" s="8"/>
@@ -14155,7 +14157,7 @@
         <v>243</v>
       </c>
       <c r="G129" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H129" s="7"/>
       <c r="I129" s="8"/>
@@ -14181,10 +14183,10 @@
         <v>444</v>
       </c>
       <c r="F130" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G130" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H130" s="7"/>
       <c r="I130" s="8"/>
@@ -14210,10 +14212,10 @@
         <v>444</v>
       </c>
       <c r="F131" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G131" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H131" s="7"/>
       <c r="I131" s="8"/>
@@ -14239,10 +14241,10 @@
         <v>469</v>
       </c>
       <c r="F132" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G132" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H132" s="7"/>
       <c r="I132" s="8"/>
@@ -14268,10 +14270,10 @@
         <v>469</v>
       </c>
       <c r="F133" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G133" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H133" s="7"/>
       <c r="I133" s="8"/>
@@ -14297,10 +14299,10 @@
         <v>449</v>
       </c>
       <c r="F134" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G134" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H134" s="7"/>
       <c r="I134" s="7"/>
@@ -14326,10 +14328,10 @@
         <v>444</v>
       </c>
       <c r="F135" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G135" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H135" s="7"/>
       <c r="I135" s="7"/>
@@ -14355,10 +14357,10 @@
         <v>444</v>
       </c>
       <c r="F136" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G136" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H136" s="7"/>
       <c r="I136" s="7"/>
@@ -14384,10 +14386,10 @@
         <v>444</v>
       </c>
       <c r="F137" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G137" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H137" s="7"/>
       <c r="I137" s="7"/>
@@ -14413,10 +14415,10 @@
         <v>444</v>
       </c>
       <c r="F138" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G138" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H138" s="7"/>
       <c r="I138" s="7"/>
@@ -14442,10 +14444,10 @@
         <v>444</v>
       </c>
       <c r="F139" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G139" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H139" s="7"/>
       <c r="I139" s="7"/>
@@ -14471,10 +14473,10 @@
         <v>449</v>
       </c>
       <c r="F140" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G140" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H140" s="7"/>
       <c r="I140" s="7"/>
@@ -14500,10 +14502,10 @@
         <v>449</v>
       </c>
       <c r="F141" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G141" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H141" s="7"/>
       <c r="I141" s="7"/>
@@ -14529,10 +14531,10 @@
         <v>449</v>
       </c>
       <c r="F142" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G142" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H142" s="7"/>
       <c r="I142" s="7"/>
@@ -14558,10 +14560,10 @@
         <v>449</v>
       </c>
       <c r="F143" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G143" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H143" s="7"/>
       <c r="I143" s="7"/>
@@ -14587,10 +14589,10 @@
         <v>449</v>
       </c>
       <c r="F144" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G144" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H144" s="7"/>
       <c r="I144" s="7"/>
@@ -14616,10 +14618,10 @@
         <v>444</v>
       </c>
       <c r="F145" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G145" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H145" s="7"/>
       <c r="I145" s="7"/>
@@ -14645,10 +14647,10 @@
         <v>444</v>
       </c>
       <c r="F146" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G146" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H146" s="7"/>
       <c r="I146" s="9"/>
@@ -14674,10 +14676,10 @@
         <v>444</v>
       </c>
       <c r="F147" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G147" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H147" s="7"/>
       <c r="I147" s="8"/>
@@ -14703,10 +14705,10 @@
         <v>444</v>
       </c>
       <c r="F148" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G148" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H148" s="8"/>
       <c r="I148" s="8"/>
@@ -14732,10 +14734,10 @@
         <v>451</v>
       </c>
       <c r="F149" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G149" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H149" s="7"/>
       <c r="I149" s="7"/>
@@ -14761,10 +14763,10 @@
         <v>451</v>
       </c>
       <c r="F150" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G150" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H150" s="7"/>
       <c r="I150" s="7"/>
@@ -14790,10 +14792,10 @@
         <v>451</v>
       </c>
       <c r="F151" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G151" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H151" s="7"/>
       <c r="I151" s="7"/>
@@ -14819,10 +14821,10 @@
         <v>451</v>
       </c>
       <c r="F152" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G152" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H152" s="7"/>
       <c r="I152" s="7"/>
@@ -14851,7 +14853,7 @@
         <v>476</v>
       </c>
       <c r="G153" s="15" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="H153" s="7"/>
       <c r="I153" s="8"/>
@@ -14880,7 +14882,7 @@
         <v>476</v>
       </c>
       <c r="G154" s="15" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="H154" s="7"/>
       <c r="I154" s="8"/>
@@ -14909,7 +14911,7 @@
         <v>476</v>
       </c>
       <c r="G155" s="15" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="H155" s="8"/>
       <c r="I155" s="7"/>
@@ -14938,7 +14940,7 @@
         <v>476</v>
       </c>
       <c r="G156" s="15" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="H156" s="8"/>
       <c r="I156" s="7"/>
@@ -14967,7 +14969,7 @@
         <v>476</v>
       </c>
       <c r="G157" s="15" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="H157" s="8"/>
       <c r="I157" s="8"/>
@@ -14996,7 +14998,7 @@
         <v>476</v>
       </c>
       <c r="G158" s="15" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="H158" s="8"/>
       <c r="I158" s="8"/>
@@ -15025,7 +15027,7 @@
         <v>476</v>
       </c>
       <c r="G159" s="15" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="H159" s="8"/>
       <c r="I159" s="8"/>
@@ -15054,7 +15056,7 @@
         <v>476</v>
       </c>
       <c r="G160" s="15" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="H160" s="8"/>
       <c r="I160" s="8"/>
@@ -15083,7 +15085,7 @@
         <v>476</v>
       </c>
       <c r="G161" s="15" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="H161" s="8"/>
       <c r="I161" s="8"/>
@@ -15112,7 +15114,7 @@
         <v>476</v>
       </c>
       <c r="G162" s="15" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="H162" s="8"/>
       <c r="I162" s="8"/>
@@ -15138,10 +15140,10 @@
         <v>444</v>
       </c>
       <c r="F163" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G163" s="15" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="H163" s="8"/>
       <c r="I163" s="8"/>
@@ -15167,10 +15169,10 @@
         <v>444</v>
       </c>
       <c r="F164" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G164" s="15" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="H164" s="8"/>
       <c r="I164" s="8"/>
@@ -15196,10 +15198,10 @@
         <v>444</v>
       </c>
       <c r="F165" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G165" s="15" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="H165" s="8"/>
       <c r="I165" s="8"/>
@@ -15228,7 +15230,7 @@
         <v>476</v>
       </c>
       <c r="G166" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H166" s="9"/>
       <c r="I166" s="10"/>
@@ -15257,7 +15259,7 @@
         <v>476</v>
       </c>
       <c r="G167" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H167" s="9"/>
       <c r="I167" s="10"/>
@@ -15286,7 +15288,7 @@
         <v>476</v>
       </c>
       <c r="G168" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H168" s="9"/>
       <c r="I168" s="10"/>
@@ -15315,7 +15317,7 @@
         <v>476</v>
       </c>
       <c r="G169" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H169" s="9"/>
       <c r="I169" s="10"/>
@@ -15341,10 +15343,10 @@
         <v>452</v>
       </c>
       <c r="F170" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G170" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H170" s="7"/>
       <c r="I170" s="10"/>
@@ -15370,10 +15372,10 @@
         <v>452</v>
       </c>
       <c r="F171" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G171" s="15" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="H171" s="8"/>
       <c r="I171" s="10"/>
@@ -15399,10 +15401,10 @@
         <v>452</v>
       </c>
       <c r="F172" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G172" s="15" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="H172" s="8"/>
       <c r="I172" s="10"/>
@@ -15428,10 +15430,10 @@
         <v>444</v>
       </c>
       <c r="F173" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G173" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H173" s="7"/>
       <c r="I173" s="7"/>
@@ -15457,10 +15459,10 @@
         <v>444</v>
       </c>
       <c r="F174" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G174" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H174" s="7"/>
       <c r="I174" s="7"/>
@@ -15486,10 +15488,10 @@
         <v>444</v>
       </c>
       <c r="F175" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G175" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H175" s="7"/>
       <c r="I175" s="7"/>
@@ -15515,10 +15517,10 @@
         <v>444</v>
       </c>
       <c r="F176" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G176" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H176" s="7"/>
       <c r="I176" s="7"/>
@@ -15544,10 +15546,10 @@
         <v>444</v>
       </c>
       <c r="F177" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G177" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H177" s="9"/>
       <c r="I177" s="9"/>
@@ -15573,10 +15575,10 @@
         <v>444</v>
       </c>
       <c r="F178" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G178" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H178" s="7"/>
       <c r="I178" s="7"/>
@@ -15602,10 +15604,10 @@
         <v>444</v>
       </c>
       <c r="F179" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G179" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H179" s="7"/>
       <c r="I179" s="7"/>
@@ -15631,10 +15633,10 @@
         <v>444</v>
       </c>
       <c r="F180" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G180" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H180" s="7"/>
       <c r="I180" s="7"/>
@@ -15660,10 +15662,10 @@
         <v>444</v>
       </c>
       <c r="F181" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G181" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H181" s="7"/>
       <c r="I181" s="7"/>
@@ -15689,10 +15691,10 @@
         <v>444</v>
       </c>
       <c r="F182" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G182" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H182" s="7"/>
       <c r="I182" s="7"/>
@@ -15718,10 +15720,10 @@
         <v>444</v>
       </c>
       <c r="F183" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G183" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H183" s="7"/>
       <c r="I183" s="9"/>
@@ -15747,10 +15749,10 @@
         <v>453</v>
       </c>
       <c r="F184" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G184" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H184" s="7"/>
       <c r="I184" s="7"/>
@@ -15776,10 +15778,10 @@
         <v>453</v>
       </c>
       <c r="F185" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G185" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H185" s="7"/>
       <c r="I185" s="7"/>
@@ -15805,10 +15807,10 @@
         <v>453</v>
       </c>
       <c r="F186" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G186" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H186" s="7"/>
       <c r="I186" s="7"/>
@@ -15834,10 +15836,10 @@
         <v>453</v>
       </c>
       <c r="F187" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G187" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H187" s="7"/>
       <c r="I187" s="8"/>
@@ -15863,10 +15865,10 @@
         <v>444</v>
       </c>
       <c r="F188" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G188" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H188" s="7"/>
       <c r="I188" s="7"/>
@@ -15892,10 +15894,10 @@
         <v>454</v>
       </c>
       <c r="F189" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G189" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H189" s="7"/>
       <c r="I189" s="9"/>
@@ -15921,10 +15923,10 @@
         <v>454</v>
       </c>
       <c r="F190" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G190" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H190" s="7"/>
       <c r="I190" s="9"/>
@@ -15950,10 +15952,10 @@
         <v>444</v>
       </c>
       <c r="F191" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G191" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H191" s="7"/>
       <c r="I191" s="8"/>
@@ -15979,10 +15981,10 @@
         <v>444</v>
       </c>
       <c r="F192" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G192" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H192" s="7"/>
       <c r="I192" s="7"/>
@@ -16008,10 +16010,10 @@
         <v>444</v>
       </c>
       <c r="F193" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G193" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H193" s="7"/>
       <c r="I193" s="8"/>
@@ -16037,10 +16039,10 @@
         <v>474</v>
       </c>
       <c r="F194" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G194" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H194" s="7"/>
       <c r="I194" s="8"/>
@@ -16069,7 +16071,7 @@
         <v>476</v>
       </c>
       <c r="G195" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H195" s="16"/>
       <c r="I195" s="16"/>
@@ -16095,10 +16097,10 @@
         <v>444</v>
       </c>
       <c r="F196" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G196" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H196" s="7"/>
       <c r="I196" s="8"/>
@@ -16124,10 +16126,10 @@
         <v>444</v>
       </c>
       <c r="F197" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G197" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H197" s="7"/>
       <c r="I197" s="8"/>
@@ -16153,10 +16155,10 @@
         <v>444</v>
       </c>
       <c r="F198" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G198" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H198" s="7"/>
       <c r="I198" s="8"/>
@@ -16182,10 +16184,10 @@
         <v>455</v>
       </c>
       <c r="F199" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G199" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H199" s="7"/>
       <c r="I199" s="7"/>
@@ -16211,10 +16213,10 @@
         <v>455</v>
       </c>
       <c r="F200" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G200" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H200" s="7"/>
       <c r="I200" s="7"/>
@@ -16240,10 +16242,10 @@
         <v>455</v>
       </c>
       <c r="F201" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G201" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H201" s="7"/>
       <c r="I201" s="7"/>
@@ -16269,10 +16271,10 @@
         <v>455</v>
       </c>
       <c r="F202" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G202" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H202" s="7"/>
       <c r="I202" s="7"/>
@@ -16295,13 +16297,13 @@
         <v>391</v>
       </c>
       <c r="E203" s="6" t="s">
+        <v>484</v>
+      </c>
+      <c r="F203" t="s">
         <v>485</v>
       </c>
-      <c r="F203" t="s">
-        <v>486</v>
-      </c>
       <c r="G203" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H203" s="7"/>
       <c r="I203" s="7"/>
@@ -16324,13 +16326,13 @@
         <v>393</v>
       </c>
       <c r="E204" s="6" t="s">
+        <v>484</v>
+      </c>
+      <c r="F204" t="s">
         <v>485</v>
       </c>
-      <c r="F204" t="s">
-        <v>486</v>
-      </c>
       <c r="G204" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H204" s="7"/>
       <c r="I204" s="7"/>
@@ -16353,13 +16355,13 @@
         <v>395</v>
       </c>
       <c r="E205" s="6" t="s">
+        <v>484</v>
+      </c>
+      <c r="F205" t="s">
         <v>485</v>
       </c>
-      <c r="F205" t="s">
-        <v>486</v>
-      </c>
       <c r="G205" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H205" s="7"/>
       <c r="I205" s="7"/>
@@ -16382,13 +16384,13 @@
         <v>397</v>
       </c>
       <c r="E206" s="6" t="s">
+        <v>484</v>
+      </c>
+      <c r="F206" t="s">
         <v>485</v>
       </c>
-      <c r="F206" t="s">
-        <v>486</v>
-      </c>
       <c r="G206" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H206" s="7"/>
       <c r="I206" s="7"/>
@@ -16411,13 +16413,13 @@
         <v>399</v>
       </c>
       <c r="E207" s="6" t="s">
+        <v>484</v>
+      </c>
+      <c r="F207" t="s">
         <v>485</v>
       </c>
-      <c r="F207" t="s">
-        <v>486</v>
-      </c>
       <c r="G207" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H207" s="7"/>
       <c r="I207" s="7"/>
@@ -16440,13 +16442,13 @@
         <v>401</v>
       </c>
       <c r="E208" s="6" t="s">
+        <v>484</v>
+      </c>
+      <c r="F208" t="s">
         <v>485</v>
       </c>
-      <c r="F208" t="s">
-        <v>486</v>
-      </c>
       <c r="G208" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H208" s="7"/>
       <c r="I208" s="7"/>
@@ -16469,13 +16471,13 @@
         <v>403</v>
       </c>
       <c r="E209" s="6" t="s">
+        <v>484</v>
+      </c>
+      <c r="F209" t="s">
         <v>485</v>
       </c>
-      <c r="F209" t="s">
-        <v>486</v>
-      </c>
       <c r="G209" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H209" s="7"/>
       <c r="I209" s="7"/>
@@ -16498,13 +16500,13 @@
         <v>405</v>
       </c>
       <c r="E210" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="F210" t="s">
         <v>404</v>
       </c>
       <c r="G210" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H210" s="7"/>
       <c r="I210" s="7"/>
@@ -16527,13 +16529,13 @@
         <v>407</v>
       </c>
       <c r="E211" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="F211" t="s">
         <v>404</v>
       </c>
       <c r="G211" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H211" s="7"/>
       <c r="I211" s="9"/>
@@ -16556,13 +16558,13 @@
         <v>409</v>
       </c>
       <c r="E212" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="F212" t="s">
         <v>404</v>
       </c>
       <c r="G212" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H212" s="7"/>
       <c r="I212" s="7"/>
@@ -16588,10 +16590,10 @@
         <v>454</v>
       </c>
       <c r="F213" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G213" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H213" s="7"/>
       <c r="I213" s="7"/>
@@ -16617,10 +16619,10 @@
         <v>454</v>
       </c>
       <c r="F214" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G214" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H214" s="7"/>
       <c r="I214" s="7"/>
@@ -16646,10 +16648,10 @@
         <v>454</v>
       </c>
       <c r="F215" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G215" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H215" s="7"/>
       <c r="I215" s="7"/>
@@ -16678,7 +16680,7 @@
         <v>416</v>
       </c>
       <c r="G216" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H216" s="7"/>
       <c r="I216" s="7"/>
@@ -16707,7 +16709,7 @@
         <v>416</v>
       </c>
       <c r="G217" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H217" s="7"/>
       <c r="I217" s="7"/>
@@ -16736,7 +16738,7 @@
         <v>416</v>
       </c>
       <c r="G218" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H218" s="7"/>
       <c r="I218" s="7"/>
@@ -16765,7 +16767,7 @@
         <v>422</v>
       </c>
       <c r="G219" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H219" s="7"/>
       <c r="I219" s="7"/>
@@ -16794,7 +16796,7 @@
         <v>422</v>
       </c>
       <c r="G220" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H220" s="7"/>
       <c r="I220" s="7"/>
@@ -16823,7 +16825,7 @@
         <v>422</v>
       </c>
       <c r="G221" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H221" s="7"/>
       <c r="I221" s="7"/>
@@ -16852,7 +16854,7 @@
         <v>428</v>
       </c>
       <c r="G222" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H222" s="7"/>
       <c r="I222" s="7"/>
@@ -16881,7 +16883,7 @@
         <v>428</v>
       </c>
       <c r="G223" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H223" s="7"/>
       <c r="I223" s="7"/>
@@ -16910,7 +16912,7 @@
         <v>428</v>
       </c>
       <c r="G224" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H224" s="7"/>
       <c r="I224" s="7"/>
@@ -16939,7 +16941,7 @@
         <v>434</v>
       </c>
       <c r="G225" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H225" s="7"/>
       <c r="I225" s="7"/>
@@ -16968,7 +16970,7 @@
         <v>434</v>
       </c>
       <c r="G226" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H226" s="7"/>
       <c r="I226" s="7"/>
@@ -16997,7 +16999,7 @@
         <v>434</v>
       </c>
       <c r="G227" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H227" s="7"/>
       <c r="I227" s="7"/>
@@ -17026,7 +17028,7 @@
         <v>434</v>
       </c>
       <c r="G228" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H228" s="7"/>
       <c r="I228" s="7"/>
@@ -17039,8 +17041,8 @@
   <autoFilter ref="A1:M228"/>
   <printOptions horizontalCentered="1" gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
-  <pageSetup scale="58" fitToHeight="0" orientation="landscape"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup scale="58" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Update READMEs for listing 3.7
</commit_message>
<xml_diff>
--- a/Listings.xlsx
+++ b/Listings.xlsx
@@ -2161,19 +2161,19 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Doug:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Listing is Oracle-specific</t>
+            <charset val="1"/>
+          </rPr>
+          <t>Doug:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+DB2 has different implementation of materialized view - see listing 3.6</t>
         </r>
       </text>
     </comment>
@@ -2185,19 +2185,19 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Doug:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Listing is Oracle-specific</t>
+            <charset val="1"/>
+          </rPr>
+          <t>Doug:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Access does not support materialized views.</t>
         </r>
       </text>
     </comment>
@@ -2209,7 +2209,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t>Ben Clothier:</t>
         </r>
@@ -2218,7 +2218,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
 Implemented as an indexed view.</t>
@@ -2233,19 +2233,19 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Doug:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Listing is Oracle-specific</t>
+            <charset val="1"/>
+          </rPr>
+          <t>Doug:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+MySQL does not support materialized views.</t>
         </r>
       </text>
     </comment>
@@ -2257,7 +2257,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t>Ben Clothier:</t>
         </r>
@@ -2266,7 +2266,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
 Cannot test due to a licensing restriction.
@@ -9882,7 +9882,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -9963,32 +9963,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="8"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="7">
@@ -10408,7 +10382,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -10423,7 +10397,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L57" sqref="L57"/>
+      <selection pane="bottomLeft" activeCell="F55" sqref="F55:M55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Done testing MySQL - bug fixes
</commit_message>
<xml_diff>
--- a/Listings.xlsx
+++ b/Listings.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="27022"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="8415" yWindow="0" windowWidth="22425" windowHeight="17520"/>
+    <workbookView xWindow="820" yWindow="140" windowWidth="22420" windowHeight="17520"/>
   </bookViews>
   <sheets>
     <sheet name="Listings" sheetId="1" r:id="rId1"/>
@@ -1889,6 +1889,30 @@
         </r>
       </text>
     </comment>
+    <comment ref="K46" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>John Viescas:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Not included because MySQL is case-insensitive.</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="I47" authorId="0">
       <text>
         <r>
@@ -7599,7 +7623,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Access does not support Common Table Expressions.</t>
+Access does not support recursive Common Table Expressions.</t>
         </r>
       </text>
     </comment>
@@ -7887,7 +7911,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Access does not support Common Table Expressions.</t>
+Emulated using saved queries.</t>
         </r>
       </text>
     </comment>
@@ -7935,7 +7959,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Access does not support Common Table Expressions.</t>
+Emulated using saved queries.</t>
         </r>
       </text>
     </comment>
@@ -7983,7 +8007,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Access does not support Common Table Expressions.</t>
+Emulated using saved queries.</t>
         </r>
       </text>
     </comment>
@@ -8400,7 +8424,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1148" uniqueCount="492">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1148" uniqueCount="493">
   <si>
     <t>Chapter</t>
   </si>
@@ -9876,6 +9900,9 @@
   </si>
   <si>
     <t>Item20***Example</t>
+  </si>
+  <si>
+    <t>Item55Example, SalesOrdersSample</t>
   </si>
 </sst>
 </file>
@@ -10073,9 +10100,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -10106,11 +10141,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="14">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="8" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="10" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="12" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal_Listings_1" xfId="1"/>
   </cellStyles>
@@ -10395,27 +10438,27 @@
   </sheetPr>
   <dimension ref="A1:M228"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F55" sqref="F55:M55"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="106.85546875" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="26" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="11" width="10.7109375" customWidth="1"/>
+    <col min="2" max="2" width="5.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="106.83203125" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="30.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.6640625" customWidth="1"/>
+    <col min="8" max="11" width="10.6640625" customWidth="1"/>
     <col min="12" max="12" width="11" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.7109375" customWidth="1"/>
-    <col min="19" max="19" width="8.85546875" customWidth="1"/>
+    <col min="13" max="13" width="10.6640625" customWidth="1"/>
+    <col min="19" max="19" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -10456,7 +10499,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -10479,7 +10522,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -10508,7 +10551,7 @@
       <c r="L3" s="7"/>
       <c r="M3" s="7"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13">
       <c r="A4" s="3">
         <v>1</v>
       </c>
@@ -10537,7 +10580,7 @@
       <c r="L4" s="7"/>
       <c r="M4" s="7"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13">
       <c r="A5" s="3">
         <v>1</v>
       </c>
@@ -10566,7 +10609,7 @@
       <c r="L5" s="7"/>
       <c r="M5" s="7"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13">
       <c r="A6" s="3">
         <v>1</v>
       </c>
@@ -10595,7 +10638,7 @@
       <c r="L6" s="7"/>
       <c r="M6" s="7"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13">
       <c r="A7" s="3">
         <v>1</v>
       </c>
@@ -10624,7 +10667,7 @@
       <c r="L7" s="7"/>
       <c r="M7" s="7"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13">
       <c r="A8" s="3">
         <v>1</v>
       </c>
@@ -10653,7 +10696,7 @@
       <c r="L8" s="8"/>
       <c r="M8" s="8"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13">
       <c r="A9" s="3">
         <v>1</v>
       </c>
@@ -10682,7 +10725,7 @@
       <c r="L9" s="7"/>
       <c r="M9" s="8"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13">
       <c r="A10" s="3">
         <v>1</v>
       </c>
@@ -10711,7 +10754,7 @@
       <c r="L10" s="7"/>
       <c r="M10" s="8"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13">
       <c r="A11" s="3">
         <v>1</v>
       </c>
@@ -10740,7 +10783,7 @@
       <c r="L11" s="7"/>
       <c r="M11" s="7"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13">
       <c r="A12" s="3">
         <v>1</v>
       </c>
@@ -10769,7 +10812,7 @@
       <c r="L12" s="7"/>
       <c r="M12" s="7"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13">
       <c r="A13" s="3">
         <v>1</v>
       </c>
@@ -10798,7 +10841,7 @@
       <c r="L13" s="7"/>
       <c r="M13" s="7"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13">
       <c r="A14" s="3">
         <v>1</v>
       </c>
@@ -10827,7 +10870,7 @@
       <c r="L14" s="7"/>
       <c r="M14" s="7"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13">
       <c r="A15" s="3">
         <v>1</v>
       </c>
@@ -10850,7 +10893,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13">
       <c r="A16" s="3">
         <v>1</v>
       </c>
@@ -10873,7 +10916,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13">
       <c r="A17" s="3">
         <v>2</v>
       </c>
@@ -10902,7 +10945,7 @@
       <c r="L17" s="8"/>
       <c r="M17" s="8"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13">
       <c r="A18" s="3">
         <v>2</v>
       </c>
@@ -10931,7 +10974,7 @@
       <c r="L18" s="8"/>
       <c r="M18" s="8"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13">
       <c r="A19" s="3">
         <v>2</v>
       </c>
@@ -10960,7 +11003,7 @@
       <c r="L19" s="8"/>
       <c r="M19" s="8"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13">
       <c r="A20" s="3">
         <v>2</v>
       </c>
@@ -10989,7 +11032,7 @@
       <c r="L20" s="8"/>
       <c r="M20" s="8"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13">
       <c r="A21" s="3">
         <v>2</v>
       </c>
@@ -11018,7 +11061,7 @@
       <c r="L21" s="7"/>
       <c r="M21" s="8"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13">
       <c r="A22" s="3">
         <v>2</v>
       </c>
@@ -11047,7 +11090,7 @@
       <c r="L22" s="7"/>
       <c r="M22" s="8"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13">
       <c r="A23" s="3">
         <v>2</v>
       </c>
@@ -11076,7 +11119,7 @@
       <c r="L23" s="8"/>
       <c r="M23" s="7"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13">
       <c r="A24" s="3">
         <v>2</v>
       </c>
@@ -11105,7 +11148,7 @@
       <c r="L24" s="7"/>
       <c r="M24" s="7"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13">
       <c r="A25" s="3">
         <v>2</v>
       </c>
@@ -11134,7 +11177,7 @@
       <c r="L25" s="7"/>
       <c r="M25" s="7"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13">
       <c r="A26" s="3">
         <v>2</v>
       </c>
@@ -11163,7 +11206,7 @@
       <c r="L26" s="7"/>
       <c r="M26" s="7"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13">
       <c r="A27" s="3">
         <v>2</v>
       </c>
@@ -11192,7 +11235,7 @@
       <c r="L27" s="7"/>
       <c r="M27" s="7"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13">
       <c r="A28" s="3">
         <v>2</v>
       </c>
@@ -11221,7 +11264,7 @@
       <c r="L28" s="7"/>
       <c r="M28" s="7"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13">
       <c r="A29" s="3">
         <v>2</v>
       </c>
@@ -11250,7 +11293,7 @@
       <c r="L29" s="7"/>
       <c r="M29" s="7"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13">
       <c r="A30" s="3">
         <v>2</v>
       </c>
@@ -11279,7 +11322,7 @@
       <c r="L30" s="7"/>
       <c r="M30" s="7"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13">
       <c r="A31" s="3">
         <v>2</v>
       </c>
@@ -11308,7 +11351,7 @@
       <c r="L31" s="7"/>
       <c r="M31" s="7"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13">
       <c r="A32" s="3">
         <v>2</v>
       </c>
@@ -11337,7 +11380,7 @@
       <c r="L32" s="7"/>
       <c r="M32" s="7"/>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13">
       <c r="A33" s="3">
         <v>2</v>
       </c>
@@ -11366,7 +11409,7 @@
       <c r="L33" s="7"/>
       <c r="M33" s="7"/>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13">
       <c r="A34" s="3">
         <v>2</v>
       </c>
@@ -11395,7 +11438,7 @@
       <c r="L34" s="7"/>
       <c r="M34" s="7"/>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13">
       <c r="A35" s="3">
         <v>2</v>
       </c>
@@ -11424,7 +11467,7 @@
       <c r="L35" s="9"/>
       <c r="M35" s="7"/>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13">
       <c r="A36" s="3">
         <v>2</v>
       </c>
@@ -11453,7 +11496,7 @@
       <c r="L36" s="9"/>
       <c r="M36" s="7"/>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13">
       <c r="A37" s="3">
         <v>2</v>
       </c>
@@ -11482,7 +11525,7 @@
       <c r="L37" s="7"/>
       <c r="M37" s="7"/>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13">
       <c r="A38" s="3">
         <v>2</v>
       </c>
@@ -11511,7 +11554,7 @@
       <c r="L38" s="7"/>
       <c r="M38" s="7"/>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13">
       <c r="A39" s="3">
         <v>2</v>
       </c>
@@ -11540,7 +11583,7 @@
       <c r="L39" s="7"/>
       <c r="M39" s="7"/>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13">
       <c r="A40" s="3">
         <v>2</v>
       </c>
@@ -11569,7 +11612,7 @@
       <c r="L40" s="7"/>
       <c r="M40" s="7"/>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13">
       <c r="A41" s="3">
         <v>2</v>
       </c>
@@ -11598,7 +11641,7 @@
       <c r="L41" s="7"/>
       <c r="M41" s="7"/>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13">
       <c r="A42" s="3">
         <v>2</v>
       </c>
@@ -11622,7 +11665,7 @@
       </c>
       <c r="J42" s="11"/>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13">
       <c r="A43" s="3">
         <v>2</v>
       </c>
@@ -11646,7 +11689,7 @@
       </c>
       <c r="J43" s="11"/>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13">
       <c r="A44" s="3">
         <v>2</v>
       </c>
@@ -11675,7 +11718,7 @@
       <c r="L44" s="7"/>
       <c r="M44" s="7"/>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13">
       <c r="A45" s="3">
         <v>2</v>
       </c>
@@ -11704,7 +11747,7 @@
       <c r="L45" s="7"/>
       <c r="M45" s="7"/>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13">
       <c r="A46" s="3">
         <v>2</v>
       </c>
@@ -11729,11 +11772,11 @@
       <c r="H46" s="7"/>
       <c r="I46" s="8"/>
       <c r="J46" s="7"/>
-      <c r="K46" s="7"/>
+      <c r="K46" s="9"/>
       <c r="L46" s="7"/>
       <c r="M46" s="7"/>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13">
       <c r="A47" s="3">
         <v>2</v>
       </c>
@@ -11762,7 +11805,7 @@
       <c r="L47" s="7"/>
       <c r="M47" s="7"/>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13">
       <c r="A48" s="3">
         <v>2</v>
       </c>
@@ -11791,7 +11834,7 @@
       <c r="L48" s="7"/>
       <c r="M48" s="7"/>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13">
       <c r="A49" s="3">
         <v>3</v>
       </c>
@@ -11820,7 +11863,7 @@
       <c r="L49" s="7"/>
       <c r="M49" s="7"/>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13">
       <c r="A50" s="3">
         <v>3</v>
       </c>
@@ -11849,7 +11892,7 @@
       <c r="L50" s="7"/>
       <c r="M50" s="7"/>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13">
       <c r="A51" s="3">
         <v>3</v>
       </c>
@@ -11878,7 +11921,7 @@
       <c r="L51" s="7"/>
       <c r="M51" s="7"/>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13">
       <c r="A52" s="3">
         <v>3</v>
       </c>
@@ -11907,7 +11950,7 @@
       <c r="L52" s="7"/>
       <c r="M52" s="7"/>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13">
       <c r="A53" s="3">
         <v>3</v>
       </c>
@@ -11936,7 +11979,7 @@
       <c r="L53" s="7"/>
       <c r="M53" s="7"/>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13">
       <c r="A54" s="3">
         <v>3</v>
       </c>
@@ -11965,7 +12008,7 @@
       <c r="L54" s="8"/>
       <c r="M54" s="8"/>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13">
       <c r="A55" s="3">
         <v>3</v>
       </c>
@@ -11994,7 +12037,7 @@
       <c r="L55" s="9"/>
       <c r="M55" s="7"/>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:13">
       <c r="A56" s="3">
         <v>3</v>
       </c>
@@ -12023,7 +12066,7 @@
       <c r="L56" s="7"/>
       <c r="M56" s="7"/>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:13">
       <c r="A57" s="3">
         <v>3</v>
       </c>
@@ -12052,7 +12095,7 @@
       <c r="L57" s="7"/>
       <c r="M57" s="7"/>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:13">
       <c r="A58" s="3">
         <v>3</v>
       </c>
@@ -12081,7 +12124,7 @@
       <c r="L58" s="7"/>
       <c r="M58" s="7"/>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:13">
       <c r="A59" s="3">
         <v>3</v>
       </c>
@@ -12110,7 +12153,7 @@
       <c r="L59" s="9"/>
       <c r="M59" s="7"/>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:13">
       <c r="A60" s="3">
         <v>4</v>
       </c>
@@ -12139,7 +12182,7 @@
       <c r="L60" s="7"/>
       <c r="M60" s="7"/>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:13">
       <c r="A61" s="3">
         <v>4</v>
       </c>
@@ -12168,7 +12211,7 @@
       <c r="L61" s="7"/>
       <c r="M61" s="7"/>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:13">
       <c r="A62" s="3">
         <v>4</v>
       </c>
@@ -12197,7 +12240,7 @@
       <c r="L62" s="7"/>
       <c r="M62" s="7"/>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:13">
       <c r="A63" s="3">
         <v>4</v>
       </c>
@@ -12226,7 +12269,7 @@
       <c r="L63" s="7"/>
       <c r="M63" s="7"/>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:13">
       <c r="A64" s="3">
         <v>4</v>
       </c>
@@ -12255,7 +12298,7 @@
       <c r="L64" s="7"/>
       <c r="M64" s="7"/>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:13">
       <c r="A65" s="3">
         <v>4</v>
       </c>
@@ -12284,7 +12327,7 @@
       <c r="L65" s="7"/>
       <c r="M65" s="7"/>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:13">
       <c r="A66" s="3">
         <v>4</v>
       </c>
@@ -12313,7 +12356,7 @@
       <c r="L66" s="16"/>
       <c r="M66" s="16"/>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:13">
       <c r="A67" s="3">
         <v>4</v>
       </c>
@@ -12342,7 +12385,7 @@
       <c r="L67" s="7"/>
       <c r="M67" s="7"/>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:13">
       <c r="A68" s="3">
         <v>4</v>
       </c>
@@ -12371,7 +12414,7 @@
       <c r="L68" s="7"/>
       <c r="M68" s="7"/>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:13">
       <c r="A69" s="3">
         <v>4</v>
       </c>
@@ -12400,7 +12443,7 @@
       <c r="L69" s="7"/>
       <c r="M69" s="7"/>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:13">
       <c r="A70" s="3">
         <v>4</v>
       </c>
@@ -12429,7 +12472,7 @@
       <c r="L70" s="7"/>
       <c r="M70" s="7"/>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:13">
       <c r="A71" s="3">
         <v>4</v>
       </c>
@@ -12458,7 +12501,7 @@
       <c r="L71" s="7"/>
       <c r="M71" s="7"/>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:13">
       <c r="A72" s="3">
         <v>4</v>
       </c>
@@ -12487,7 +12530,7 @@
       <c r="L72" s="7"/>
       <c r="M72" s="7"/>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:13">
       <c r="A73" s="3">
         <v>4</v>
       </c>
@@ -12516,7 +12559,7 @@
       <c r="L73" s="7"/>
       <c r="M73" s="7"/>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:13">
       <c r="A74" s="3">
         <v>4</v>
       </c>
@@ -12545,7 +12588,7 @@
       <c r="L74" s="7"/>
       <c r="M74" s="7"/>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:13">
       <c r="A75" s="3">
         <v>4</v>
       </c>
@@ -12574,7 +12617,7 @@
       <c r="L75" s="7"/>
       <c r="M75" s="7"/>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:13">
       <c r="A76" s="3">
         <v>4</v>
       </c>
@@ -12603,7 +12646,7 @@
       <c r="L76" s="7"/>
       <c r="M76" s="7"/>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:13">
       <c r="A77" s="3">
         <v>4</v>
       </c>
@@ -12632,7 +12675,7 @@
       <c r="L77" s="7"/>
       <c r="M77" s="7"/>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:13">
       <c r="A78" s="3">
         <v>4</v>
       </c>
@@ -12661,7 +12704,7 @@
       <c r="L78" s="7"/>
       <c r="M78" s="7"/>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:13">
       <c r="A79" s="3">
         <v>4</v>
       </c>
@@ -12690,7 +12733,7 @@
       <c r="L79" s="7"/>
       <c r="M79" s="7"/>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:13">
       <c r="A80" s="3">
         <v>4</v>
       </c>
@@ -12719,7 +12762,7 @@
       <c r="L80" s="7"/>
       <c r="M80" s="7"/>
     </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:13">
       <c r="A81" s="3">
         <v>4</v>
       </c>
@@ -12748,7 +12791,7 @@
       <c r="L81" s="7"/>
       <c r="M81" s="7"/>
     </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:13">
       <c r="A82" s="3">
         <v>4</v>
       </c>
@@ -12777,7 +12820,7 @@
       <c r="L82" s="7"/>
       <c r="M82" s="7"/>
     </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:13">
       <c r="A83" s="3">
         <v>4</v>
       </c>
@@ -12806,7 +12849,7 @@
       <c r="L83" s="7"/>
       <c r="M83" s="7"/>
     </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:13">
       <c r="A84" s="3">
         <v>4</v>
       </c>
@@ -12835,7 +12878,7 @@
       <c r="L84" s="7"/>
       <c r="M84" s="7"/>
     </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:13">
       <c r="A85" s="3">
         <v>4</v>
       </c>
@@ -12864,7 +12907,7 @@
       <c r="L85" s="7"/>
       <c r="M85" s="7"/>
     </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:13">
       <c r="A86" s="3">
         <v>4</v>
       </c>
@@ -12893,7 +12936,7 @@
       <c r="L86" s="7"/>
       <c r="M86" s="7"/>
     </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:13">
       <c r="A87" s="3">
         <v>4</v>
       </c>
@@ -12922,7 +12965,7 @@
       <c r="L87" s="7"/>
       <c r="M87" s="7"/>
     </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:13">
       <c r="A88" s="3">
         <v>4</v>
       </c>
@@ -12951,7 +12994,7 @@
       <c r="L88" s="7"/>
       <c r="M88" s="7"/>
     </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:13">
       <c r="A89" s="3">
         <v>4</v>
       </c>
@@ -12980,7 +13023,7 @@
       <c r="L89" s="7"/>
       <c r="M89" s="7"/>
     </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:13">
       <c r="A90" s="3">
         <v>4</v>
       </c>
@@ -13009,7 +13052,7 @@
       <c r="L90" s="7"/>
       <c r="M90" s="7"/>
     </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:13">
       <c r="A91" s="3">
         <v>4</v>
       </c>
@@ -13038,7 +13081,7 @@
       <c r="L91" s="7"/>
       <c r="M91" s="7"/>
     </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:13">
       <c r="A92" s="3">
         <v>4</v>
       </c>
@@ -13067,7 +13110,7 @@
       <c r="L92" s="7"/>
       <c r="M92" s="7"/>
     </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:13">
       <c r="A93" s="3">
         <v>4</v>
       </c>
@@ -13096,7 +13139,7 @@
       <c r="L93" s="7"/>
       <c r="M93" s="7"/>
     </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:13">
       <c r="A94" s="3">
         <v>4</v>
       </c>
@@ -13125,7 +13168,7 @@
       <c r="L94" s="7"/>
       <c r="M94" s="7"/>
     </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:13">
       <c r="A95" s="3">
         <v>4</v>
       </c>
@@ -13154,7 +13197,7 @@
       <c r="L95" s="7"/>
       <c r="M95" s="7"/>
     </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:13">
       <c r="A96" s="3">
         <v>4</v>
       </c>
@@ -13183,7 +13226,7 @@
       <c r="L96" s="7"/>
       <c r="M96" s="7"/>
     </row>
-    <row r="97" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:13">
       <c r="A97" s="3">
         <v>4</v>
       </c>
@@ -13212,7 +13255,7 @@
       <c r="L97" s="7"/>
       <c r="M97" s="7"/>
     </row>
-    <row r="98" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:13">
       <c r="A98" s="3">
         <v>4</v>
       </c>
@@ -13241,7 +13284,7 @@
       <c r="L98" s="7"/>
       <c r="M98" s="7"/>
     </row>
-    <row r="99" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:13">
       <c r="A99" s="3">
         <v>4</v>
       </c>
@@ -13270,7 +13313,7 @@
       <c r="L99" s="7"/>
       <c r="M99" s="7"/>
     </row>
-    <row r="100" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:13">
       <c r="A100" s="3">
         <v>5</v>
       </c>
@@ -13299,7 +13342,7 @@
       <c r="L100" s="16"/>
       <c r="M100" s="16"/>
     </row>
-    <row r="101" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:13">
       <c r="A101" s="3">
         <v>5</v>
       </c>
@@ -13328,7 +13371,7 @@
       <c r="L101" s="16"/>
       <c r="M101" s="16"/>
     </row>
-    <row r="102" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:13">
       <c r="A102" s="3">
         <v>5</v>
       </c>
@@ -13357,7 +13400,7 @@
       <c r="L102" s="16"/>
       <c r="M102" s="16"/>
     </row>
-    <row r="103" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:13">
       <c r="A103" s="3">
         <v>5</v>
       </c>
@@ -13386,7 +13429,7 @@
       <c r="L103" s="7"/>
       <c r="M103" s="7"/>
     </row>
-    <row r="104" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:13">
       <c r="A104" s="3">
         <v>5</v>
       </c>
@@ -13415,7 +13458,7 @@
       <c r="L104" s="7"/>
       <c r="M104" s="7"/>
     </row>
-    <row r="105" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:13">
       <c r="A105" s="3">
         <v>5</v>
       </c>
@@ -13444,7 +13487,7 @@
       <c r="L105" s="7"/>
       <c r="M105" s="7"/>
     </row>
-    <row r="106" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:13">
       <c r="A106" s="3">
         <v>5</v>
       </c>
@@ -13473,7 +13516,7 @@
       <c r="L106" s="7"/>
       <c r="M106" s="7"/>
     </row>
-    <row r="107" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:13">
       <c r="A107" s="3">
         <v>5</v>
       </c>
@@ -13487,7 +13530,7 @@
         <v>200</v>
       </c>
       <c r="E107" t="s">
-        <v>444</v>
+        <v>447</v>
       </c>
       <c r="F107" t="s">
         <v>485</v>
@@ -13502,7 +13545,7 @@
       <c r="L107" s="7"/>
       <c r="M107" s="7"/>
     </row>
-    <row r="108" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:13">
       <c r="A108" s="3">
         <v>5</v>
       </c>
@@ -13516,7 +13559,7 @@
         <v>202</v>
       </c>
       <c r="E108" t="s">
-        <v>444</v>
+        <v>447</v>
       </c>
       <c r="F108" t="s">
         <v>485</v>
@@ -13531,7 +13574,7 @@
       <c r="L108" s="7"/>
       <c r="M108" s="7"/>
     </row>
-    <row r="109" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:13">
       <c r="A109" s="3">
         <v>5</v>
       </c>
@@ -13560,7 +13603,7 @@
       <c r="L109" s="7"/>
       <c r="M109" s="7"/>
     </row>
-    <row r="110" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:13">
       <c r="A110" s="3">
         <v>5</v>
       </c>
@@ -13589,7 +13632,7 @@
       <c r="L110" s="8"/>
       <c r="M110" s="7"/>
     </row>
-    <row r="111" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:13">
       <c r="A111" s="3">
         <v>5</v>
       </c>
@@ -13618,7 +13661,7 @@
       <c r="L111" s="7"/>
       <c r="M111" s="7"/>
     </row>
-    <row r="112" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:13">
       <c r="A112" s="3">
         <v>5</v>
       </c>
@@ -13647,7 +13690,7 @@
       <c r="L112" s="7"/>
       <c r="M112" s="7"/>
     </row>
-    <row r="113" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:13">
       <c r="A113" s="3">
         <v>5</v>
       </c>
@@ -13676,7 +13719,7 @@
       <c r="L113" s="7"/>
       <c r="M113" s="7"/>
     </row>
-    <row r="114" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:13">
       <c r="A114" s="3">
         <v>5</v>
       </c>
@@ -13705,7 +13748,7 @@
       <c r="L114" s="9"/>
       <c r="M114" s="7"/>
     </row>
-    <row r="115" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:13">
       <c r="A115" s="3">
         <v>5</v>
       </c>
@@ -13734,7 +13777,7 @@
       <c r="L115" s="9"/>
       <c r="M115" s="7"/>
     </row>
-    <row r="116" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:13">
       <c r="A116" s="3">
         <v>5</v>
       </c>
@@ -13763,7 +13806,7 @@
       <c r="L116" s="7"/>
       <c r="M116" s="7"/>
     </row>
-    <row r="117" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:13">
       <c r="A117" s="3">
         <v>5</v>
       </c>
@@ -13792,7 +13835,7 @@
       <c r="L117" s="7"/>
       <c r="M117" s="7"/>
     </row>
-    <row r="118" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:13">
       <c r="A118" s="3">
         <v>5</v>
       </c>
@@ -13821,7 +13864,7 @@
       <c r="L118" s="7"/>
       <c r="M118" s="7"/>
     </row>
-    <row r="119" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:13">
       <c r="A119" s="3">
         <v>5</v>
       </c>
@@ -13850,7 +13893,7 @@
       <c r="L119" s="7"/>
       <c r="M119" s="7"/>
     </row>
-    <row r="120" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:13">
       <c r="A120" s="3">
         <v>5</v>
       </c>
@@ -13879,7 +13922,7 @@
       <c r="L120" s="7"/>
       <c r="M120" s="7"/>
     </row>
-    <row r="121" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:13">
       <c r="A121" s="3">
         <v>5</v>
       </c>
@@ -13908,7 +13951,7 @@
       <c r="L121" s="7"/>
       <c r="M121" s="7"/>
     </row>
-    <row r="122" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:13">
       <c r="A122" s="3">
         <v>5</v>
       </c>
@@ -13937,7 +13980,7 @@
       <c r="L122" s="7"/>
       <c r="M122" s="7"/>
     </row>
-    <row r="123" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:13">
       <c r="A123" s="3">
         <v>5</v>
       </c>
@@ -13966,7 +14009,7 @@
       <c r="L123" s="7"/>
       <c r="M123" s="9"/>
     </row>
-    <row r="124" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:13">
       <c r="A124" s="3">
         <v>5</v>
       </c>
@@ -13995,7 +14038,7 @@
       <c r="L124" s="7"/>
       <c r="M124" s="9"/>
     </row>
-    <row r="125" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:13">
       <c r="A125" s="3">
         <v>5</v>
       </c>
@@ -14024,7 +14067,7 @@
       <c r="L125" s="7"/>
       <c r="M125" s="9"/>
     </row>
-    <row r="126" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:13">
       <c r="A126" s="3">
         <v>5</v>
       </c>
@@ -14053,7 +14096,7 @@
       <c r="L126" s="7"/>
       <c r="M126" s="7"/>
     </row>
-    <row r="127" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:13">
       <c r="A127" s="3">
         <v>5</v>
       </c>
@@ -14082,7 +14125,7 @@
       <c r="L127" s="9"/>
       <c r="M127" s="7"/>
     </row>
-    <row r="128" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:13">
       <c r="A128" s="3">
         <v>5</v>
       </c>
@@ -14111,7 +14154,7 @@
       <c r="L128" s="7"/>
       <c r="M128" s="7"/>
     </row>
-    <row r="129" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:13">
       <c r="A129" s="3">
         <v>5</v>
       </c>
@@ -14140,7 +14183,7 @@
       <c r="L129" s="7"/>
       <c r="M129" s="7"/>
     </row>
-    <row r="130" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:13">
       <c r="A130" s="3">
         <v>5</v>
       </c>
@@ -14169,7 +14212,7 @@
       <c r="L130" s="7"/>
       <c r="M130" s="7"/>
     </row>
-    <row r="131" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:13">
       <c r="A131" s="3">
         <v>5</v>
       </c>
@@ -14198,7 +14241,7 @@
       <c r="L131" s="7"/>
       <c r="M131" s="7"/>
     </row>
-    <row r="132" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:13">
       <c r="A132" s="3">
         <v>5</v>
       </c>
@@ -14227,7 +14270,7 @@
       <c r="L132" s="7"/>
       <c r="M132" s="7"/>
     </row>
-    <row r="133" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:13">
       <c r="A133" s="3">
         <v>5</v>
       </c>
@@ -14256,7 +14299,7 @@
       <c r="L133" s="7"/>
       <c r="M133" s="7"/>
     </row>
-    <row r="134" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:13">
       <c r="A134" s="3">
         <v>6</v>
       </c>
@@ -14285,7 +14328,7 @@
       <c r="L134" s="7"/>
       <c r="M134" s="7"/>
     </row>
-    <row r="135" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:13">
       <c r="A135" s="3">
         <v>6</v>
       </c>
@@ -14314,7 +14357,7 @@
       <c r="L135" s="7"/>
       <c r="M135" s="7"/>
     </row>
-    <row r="136" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:13">
       <c r="A136" s="3">
         <v>6</v>
       </c>
@@ -14343,7 +14386,7 @@
       <c r="L136" s="7"/>
       <c r="M136" s="7"/>
     </row>
-    <row r="137" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:13">
       <c r="A137" s="3">
         <v>6</v>
       </c>
@@ -14372,7 +14415,7 @@
       <c r="L137" s="7"/>
       <c r="M137" s="7"/>
     </row>
-    <row r="138" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:13">
       <c r="A138" s="3">
         <v>6</v>
       </c>
@@ -14401,7 +14444,7 @@
       <c r="L138" s="7"/>
       <c r="M138" s="7"/>
     </row>
-    <row r="139" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:13">
       <c r="A139" s="3">
         <v>6</v>
       </c>
@@ -14430,7 +14473,7 @@
       <c r="L139" s="7"/>
       <c r="M139" s="7"/>
     </row>
-    <row r="140" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:13">
       <c r="A140" s="3">
         <v>6</v>
       </c>
@@ -14459,7 +14502,7 @@
       <c r="L140" s="7"/>
       <c r="M140" s="7"/>
     </row>
-    <row r="141" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:13">
       <c r="A141" s="3">
         <v>6</v>
       </c>
@@ -14488,7 +14531,7 @@
       <c r="L141" s="7"/>
       <c r="M141" s="7"/>
     </row>
-    <row r="142" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:13">
       <c r="A142" s="3">
         <v>6</v>
       </c>
@@ -14517,7 +14560,7 @@
       <c r="L142" s="7"/>
       <c r="M142" s="7"/>
     </row>
-    <row r="143" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:13">
       <c r="A143" s="3">
         <v>6</v>
       </c>
@@ -14546,7 +14589,7 @@
       <c r="L143" s="7"/>
       <c r="M143" s="7"/>
     </row>
-    <row r="144" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:13">
       <c r="A144" s="3">
         <v>6</v>
       </c>
@@ -14575,7 +14618,7 @@
       <c r="L144" s="7"/>
       <c r="M144" s="7"/>
     </row>
-    <row r="145" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:13">
       <c r="A145" s="3">
         <v>6</v>
       </c>
@@ -14604,7 +14647,7 @@
       <c r="L145" s="7"/>
       <c r="M145" s="7"/>
     </row>
-    <row r="146" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:13">
       <c r="A146" s="3">
         <v>6</v>
       </c>
@@ -14633,7 +14676,7 @@
       <c r="L146" s="7"/>
       <c r="M146" s="7"/>
     </row>
-    <row r="147" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:13">
       <c r="A147" s="3">
         <v>6</v>
       </c>
@@ -14662,7 +14705,7 @@
       <c r="L147" s="7"/>
       <c r="M147" s="7"/>
     </row>
-    <row r="148" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:13">
       <c r="A148" s="3">
         <v>6</v>
       </c>
@@ -14691,7 +14734,7 @@
       <c r="L148" s="7"/>
       <c r="M148" s="7"/>
     </row>
-    <row r="149" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:13">
       <c r="A149" s="3">
         <v>6</v>
       </c>
@@ -14720,7 +14763,7 @@
       <c r="L149" s="7"/>
       <c r="M149" s="7"/>
     </row>
-    <row r="150" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:13">
       <c r="A150" s="3">
         <v>6</v>
       </c>
@@ -14749,7 +14792,7 @@
       <c r="L150" s="7"/>
       <c r="M150" s="7"/>
     </row>
-    <row r="151" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:13">
       <c r="A151" s="3">
         <v>6</v>
       </c>
@@ -14778,7 +14821,7 @@
       <c r="L151" s="7"/>
       <c r="M151" s="7"/>
     </row>
-    <row r="152" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:13">
       <c r="A152" s="3">
         <v>6</v>
       </c>
@@ -14807,7 +14850,7 @@
       <c r="L152" s="7"/>
       <c r="M152" s="7"/>
     </row>
-    <row r="153" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:13">
       <c r="A153" s="3">
         <v>7</v>
       </c>
@@ -14836,7 +14879,7 @@
       <c r="L153" s="8"/>
       <c r="M153" s="8"/>
     </row>
-    <row r="154" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:13">
       <c r="A154" s="3">
         <v>7</v>
       </c>
@@ -14865,7 +14908,7 @@
       <c r="L154" s="8"/>
       <c r="M154" s="8"/>
     </row>
-    <row r="155" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:13">
       <c r="A155" s="3">
         <v>7</v>
       </c>
@@ -14894,7 +14937,7 @@
       <c r="L155" s="8"/>
       <c r="M155" s="8"/>
     </row>
-    <row r="156" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:13">
       <c r="A156" s="3">
         <v>7</v>
       </c>
@@ -14923,7 +14966,7 @@
       <c r="L156" s="8"/>
       <c r="M156" s="8"/>
     </row>
-    <row r="157" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:13">
       <c r="A157" s="3">
         <v>7</v>
       </c>
@@ -14952,7 +14995,7 @@
       <c r="L157" s="8"/>
       <c r="M157" s="8"/>
     </row>
-    <row r="158" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:13">
       <c r="A158" s="3">
         <v>7</v>
       </c>
@@ -14981,7 +15024,7 @@
       <c r="L158" s="8"/>
       <c r="M158" s="8"/>
     </row>
-    <row r="159" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:13">
       <c r="A159" s="3">
         <v>7</v>
       </c>
@@ -15010,7 +15053,7 @@
       <c r="L159" s="8"/>
       <c r="M159" s="8"/>
     </row>
-    <row r="160" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:13">
       <c r="A160" s="3">
         <v>7</v>
       </c>
@@ -15039,7 +15082,7 @@
       <c r="L160" s="8"/>
       <c r="M160" s="8"/>
     </row>
-    <row r="161" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:13">
       <c r="A161" s="3">
         <v>7</v>
       </c>
@@ -15068,7 +15111,7 @@
       <c r="L161" s="7"/>
       <c r="M161" s="8"/>
     </row>
-    <row r="162" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:13">
       <c r="A162" s="3">
         <v>7</v>
       </c>
@@ -15097,7 +15140,7 @@
       <c r="L162" s="7"/>
       <c r="M162" s="8"/>
     </row>
-    <row r="163" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:13">
       <c r="A163" s="3">
         <v>7</v>
       </c>
@@ -15126,7 +15169,7 @@
       <c r="L163" s="8"/>
       <c r="M163" s="7"/>
     </row>
-    <row r="164" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:13">
       <c r="A164" s="3">
         <v>7</v>
       </c>
@@ -15155,7 +15198,7 @@
       <c r="L164" s="8"/>
       <c r="M164" s="7"/>
     </row>
-    <row r="165" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:13">
       <c r="A165" s="3">
         <v>7</v>
       </c>
@@ -15184,7 +15227,7 @@
       <c r="L165" s="8"/>
       <c r="M165" s="7"/>
     </row>
-    <row r="166" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:13">
       <c r="A166" s="3">
         <v>7</v>
       </c>
@@ -15213,7 +15256,7 @@
       <c r="L166" s="8"/>
       <c r="M166" s="7"/>
     </row>
-    <row r="167" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:13">
       <c r="A167" s="3">
         <v>7</v>
       </c>
@@ -15242,7 +15285,7 @@
       <c r="L167" s="8"/>
       <c r="M167" s="7"/>
     </row>
-    <row r="168" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:13">
       <c r="A168" s="3">
         <v>7</v>
       </c>
@@ -15271,7 +15314,7 @@
       <c r="L168" s="8"/>
       <c r="M168" s="7"/>
     </row>
-    <row r="169" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:13">
       <c r="A169" s="3">
         <v>7</v>
       </c>
@@ -15300,7 +15343,7 @@
       <c r="L169" s="8"/>
       <c r="M169" s="7"/>
     </row>
-    <row r="170" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:13">
       <c r="A170" s="3">
         <v>7</v>
       </c>
@@ -15329,7 +15372,7 @@
       <c r="L170" s="7"/>
       <c r="M170" s="7"/>
     </row>
-    <row r="171" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:13">
       <c r="A171" s="3">
         <v>7</v>
       </c>
@@ -15358,7 +15401,7 @@
       <c r="L171" s="8"/>
       <c r="M171" s="8"/>
     </row>
-    <row r="172" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:13">
       <c r="A172" s="3">
         <v>7</v>
       </c>
@@ -15387,7 +15430,7 @@
       <c r="L172" s="8"/>
       <c r="M172" s="8"/>
     </row>
-    <row r="173" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:13">
       <c r="A173" s="3">
         <v>7</v>
       </c>
@@ -15416,7 +15459,7 @@
       <c r="L173" s="7"/>
       <c r="M173" s="7"/>
     </row>
-    <row r="174" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:13">
       <c r="A174" s="3">
         <v>7</v>
       </c>
@@ -15445,7 +15488,7 @@
       <c r="L174" s="7"/>
       <c r="M174" s="7"/>
     </row>
-    <row r="175" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:13">
       <c r="A175" s="3">
         <v>7</v>
       </c>
@@ -15474,7 +15517,7 @@
       <c r="L175" s="7"/>
       <c r="M175" s="7"/>
     </row>
-    <row r="176" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:13">
       <c r="A176" s="3">
         <v>7</v>
       </c>
@@ -15503,7 +15546,7 @@
       <c r="L176" s="7"/>
       <c r="M176" s="7"/>
     </row>
-    <row r="177" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:13">
       <c r="A177" s="3">
         <v>7</v>
       </c>
@@ -15532,7 +15575,7 @@
       <c r="L177" s="9"/>
       <c r="M177" s="9"/>
     </row>
-    <row r="178" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:13">
       <c r="A178" s="3">
         <v>8</v>
       </c>
@@ -15561,7 +15604,7 @@
       <c r="L178" s="7"/>
       <c r="M178" s="7"/>
     </row>
-    <row r="179" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:13">
       <c r="A179" s="3">
         <v>8</v>
       </c>
@@ -15590,7 +15633,7 @@
       <c r="L179" s="7"/>
       <c r="M179" s="7"/>
     </row>
-    <row r="180" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:13">
       <c r="A180" s="3">
         <v>8</v>
       </c>
@@ -15619,7 +15662,7 @@
       <c r="L180" s="7"/>
       <c r="M180" s="7"/>
     </row>
-    <row r="181" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:13">
       <c r="A181" s="3">
         <v>8</v>
       </c>
@@ -15648,7 +15691,7 @@
       <c r="L181" s="7"/>
       <c r="M181" s="7"/>
     </row>
-    <row r="182" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:13">
       <c r="A182" s="3">
         <v>8</v>
       </c>
@@ -15677,7 +15720,7 @@
       <c r="L182" s="7"/>
       <c r="M182" s="7"/>
     </row>
-    <row r="183" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:13">
       <c r="A183" s="3">
         <v>8</v>
       </c>
@@ -15706,7 +15749,7 @@
       <c r="L183" s="7"/>
       <c r="M183" s="7"/>
     </row>
-    <row r="184" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:13">
       <c r="A184" s="3">
         <v>8</v>
       </c>
@@ -15735,7 +15778,7 @@
       <c r="L184" s="7"/>
       <c r="M184" s="7"/>
     </row>
-    <row r="185" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:13">
       <c r="A185" s="3">
         <v>8</v>
       </c>
@@ -15764,7 +15807,7 @@
       <c r="L185" s="7"/>
       <c r="M185" s="7"/>
     </row>
-    <row r="186" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:13">
       <c r="A186" s="3">
         <v>8</v>
       </c>
@@ -15793,7 +15836,7 @@
       <c r="L186" s="7"/>
       <c r="M186" s="7"/>
     </row>
-    <row r="187" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:13">
       <c r="A187" s="3">
         <v>8</v>
       </c>
@@ -15822,7 +15865,7 @@
       <c r="L187" s="7"/>
       <c r="M187" s="7"/>
     </row>
-    <row r="188" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:13">
       <c r="A188" s="3">
         <v>8</v>
       </c>
@@ -15851,7 +15894,7 @@
       <c r="L188" s="7"/>
       <c r="M188" s="7"/>
     </row>
-    <row r="189" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:13">
       <c r="A189" s="3">
         <v>8</v>
       </c>
@@ -15880,7 +15923,7 @@
       <c r="L189" s="7"/>
       <c r="M189" s="7"/>
     </row>
-    <row r="190" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:13">
       <c r="A190" s="3">
         <v>8</v>
       </c>
@@ -15909,7 +15952,7 @@
       <c r="L190" s="7"/>
       <c r="M190" s="7"/>
     </row>
-    <row r="191" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:13">
       <c r="A191" s="3">
         <v>9</v>
       </c>
@@ -15938,7 +15981,7 @@
       <c r="L191" s="7"/>
       <c r="M191" s="7"/>
     </row>
-    <row r="192" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:13">
       <c r="A192" s="3">
         <v>9</v>
       </c>
@@ -15967,7 +16010,7 @@
       <c r="L192" s="7"/>
       <c r="M192" s="7"/>
     </row>
-    <row r="193" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:13">
       <c r="A193" s="3">
         <v>9</v>
       </c>
@@ -15996,7 +16039,7 @@
       <c r="L193" s="7"/>
       <c r="M193" s="7"/>
     </row>
-    <row r="194" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:13">
       <c r="A194" s="3">
         <v>9</v>
       </c>
@@ -16025,7 +16068,7 @@
       <c r="L194" s="7"/>
       <c r="M194" s="7"/>
     </row>
-    <row r="195" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:13">
       <c r="A195" s="3">
         <v>9</v>
       </c>
@@ -16054,7 +16097,7 @@
       <c r="L195" s="16"/>
       <c r="M195" s="16"/>
     </row>
-    <row r="196" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:13">
       <c r="A196" s="3">
         <v>9</v>
       </c>
@@ -16077,13 +16120,13 @@
         <v>488</v>
       </c>
       <c r="H196" s="7"/>
-      <c r="I196" s="8"/>
+      <c r="I196" s="9"/>
       <c r="J196" s="7"/>
       <c r="K196" s="9"/>
       <c r="L196" s="7"/>
       <c r="M196" s="7"/>
     </row>
-    <row r="197" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:13">
       <c r="A197" s="3">
         <v>9</v>
       </c>
@@ -16106,13 +16149,13 @@
         <v>488</v>
       </c>
       <c r="H197" s="7"/>
-      <c r="I197" s="8"/>
+      <c r="I197" s="9"/>
       <c r="J197" s="7"/>
       <c r="K197" s="9"/>
       <c r="L197" s="7"/>
       <c r="M197" s="7"/>
     </row>
-    <row r="198" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:13">
       <c r="A198" s="3">
         <v>9</v>
       </c>
@@ -16135,13 +16178,13 @@
         <v>488</v>
       </c>
       <c r="H198" s="7"/>
-      <c r="I198" s="8"/>
+      <c r="I198" s="9"/>
       <c r="J198" s="7"/>
       <c r="K198" s="9"/>
       <c r="L198" s="7"/>
       <c r="M198" s="7"/>
     </row>
-    <row r="199" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:13">
       <c r="A199" s="3">
         <v>9</v>
       </c>
@@ -16170,7 +16213,7 @@
       <c r="L199" s="7"/>
       <c r="M199" s="7"/>
     </row>
-    <row r="200" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:13">
       <c r="A200" s="3">
         <v>9</v>
       </c>
@@ -16199,7 +16242,7 @@
       <c r="L200" s="7"/>
       <c r="M200" s="7"/>
     </row>
-    <row r="201" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:13">
       <c r="A201" s="3">
         <v>9</v>
       </c>
@@ -16228,7 +16271,7 @@
       <c r="L201" s="7"/>
       <c r="M201" s="7"/>
     </row>
-    <row r="202" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:13">
       <c r="A202" s="3">
         <v>9</v>
       </c>
@@ -16257,7 +16300,7 @@
       <c r="L202" s="7"/>
       <c r="M202" s="7"/>
     </row>
-    <row r="203" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:13">
       <c r="A203" s="3">
         <v>9</v>
       </c>
@@ -16271,7 +16314,7 @@
         <v>391</v>
       </c>
       <c r="E203" s="6" t="s">
-        <v>484</v>
+        <v>444</v>
       </c>
       <c r="F203" t="s">
         <v>485</v>
@@ -16286,7 +16329,7 @@
       <c r="L203" s="7"/>
       <c r="M203" s="7"/>
     </row>
-    <row r="204" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:13">
       <c r="A204" s="3">
         <v>9</v>
       </c>
@@ -16315,7 +16358,7 @@
       <c r="L204" s="7"/>
       <c r="M204" s="7"/>
     </row>
-    <row r="205" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:13">
       <c r="A205" s="3">
         <v>9</v>
       </c>
@@ -16329,7 +16372,7 @@
         <v>395</v>
       </c>
       <c r="E205" s="6" t="s">
-        <v>484</v>
+        <v>492</v>
       </c>
       <c r="F205" t="s">
         <v>485</v>
@@ -16344,7 +16387,7 @@
       <c r="L205" s="7"/>
       <c r="M205" s="7"/>
     </row>
-    <row r="206" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:13">
       <c r="A206" s="3">
         <v>9</v>
       </c>
@@ -16373,7 +16416,7 @@
       <c r="L206" s="7"/>
       <c r="M206" s="7"/>
     </row>
-    <row r="207" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:13">
       <c r="A207" s="3">
         <v>9</v>
       </c>
@@ -16402,7 +16445,7 @@
       <c r="L207" s="7"/>
       <c r="M207" s="7"/>
     </row>
-    <row r="208" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:13">
       <c r="A208" s="3">
         <v>9</v>
       </c>
@@ -16431,7 +16474,7 @@
       <c r="L208" s="7"/>
       <c r="M208" s="7"/>
     </row>
-    <row r="209" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:13">
       <c r="A209" s="3">
         <v>9</v>
       </c>
@@ -16445,7 +16488,7 @@
         <v>403</v>
       </c>
       <c r="E209" s="6" t="s">
-        <v>484</v>
+        <v>444</v>
       </c>
       <c r="F209" t="s">
         <v>485</v>
@@ -16460,7 +16503,7 @@
       <c r="L209" s="7"/>
       <c r="M209" s="7"/>
     </row>
-    <row r="210" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:13">
       <c r="A210" s="3">
         <v>9</v>
       </c>
@@ -16489,7 +16532,7 @@
       <c r="L210" s="7"/>
       <c r="M210" s="7"/>
     </row>
-    <row r="211" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:13">
       <c r="A211" s="3">
         <v>9</v>
       </c>
@@ -16518,7 +16561,7 @@
       <c r="L211" s="9"/>
       <c r="M211" s="9"/>
     </row>
-    <row r="212" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:13">
       <c r="A212" s="3">
         <v>9</v>
       </c>
@@ -16547,7 +16590,7 @@
       <c r="L212" s="7"/>
       <c r="M212" s="7"/>
     </row>
-    <row r="213" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:13">
       <c r="A213" s="3">
         <v>9</v>
       </c>
@@ -16576,7 +16619,7 @@
       <c r="L213" s="7"/>
       <c r="M213" s="7"/>
     </row>
-    <row r="214" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:13">
       <c r="A214" s="3">
         <v>9</v>
       </c>
@@ -16605,7 +16648,7 @@
       <c r="L214" s="7"/>
       <c r="M214" s="7"/>
     </row>
-    <row r="215" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:13">
       <c r="A215" s="3">
         <v>9</v>
       </c>
@@ -16634,7 +16677,7 @@
       <c r="L215" s="7"/>
       <c r="M215" s="7"/>
     </row>
-    <row r="216" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:13">
       <c r="A216" s="3">
         <v>10</v>
       </c>
@@ -16663,7 +16706,7 @@
       <c r="L216" s="7"/>
       <c r="M216" s="7"/>
     </row>
-    <row r="217" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:13">
       <c r="A217" s="3">
         <v>10</v>
       </c>
@@ -16692,7 +16735,7 @@
       <c r="L217" s="7"/>
       <c r="M217" s="7"/>
     </row>
-    <row r="218" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:13">
       <c r="A218" s="3">
         <v>10</v>
       </c>
@@ -16721,7 +16764,7 @@
       <c r="L218" s="7"/>
       <c r="M218" s="7"/>
     </row>
-    <row r="219" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:13">
       <c r="A219" s="3">
         <v>10</v>
       </c>
@@ -16750,7 +16793,7 @@
       <c r="L219" s="7"/>
       <c r="M219" s="7"/>
     </row>
-    <row r="220" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:13">
       <c r="A220" s="3">
         <v>10</v>
       </c>
@@ -16779,7 +16822,7 @@
       <c r="L220" s="7"/>
       <c r="M220" s="7"/>
     </row>
-    <row r="221" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:13">
       <c r="A221" s="3">
         <v>10</v>
       </c>
@@ -16808,7 +16851,7 @@
       <c r="L221" s="7"/>
       <c r="M221" s="7"/>
     </row>
-    <row r="222" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:13">
       <c r="A222" s="3">
         <v>10</v>
       </c>
@@ -16837,7 +16880,7 @@
       <c r="L222" s="7"/>
       <c r="M222" s="7"/>
     </row>
-    <row r="223" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:13">
       <c r="A223" s="3">
         <v>10</v>
       </c>
@@ -16866,7 +16909,7 @@
       <c r="L223" s="7"/>
       <c r="M223" s="7"/>
     </row>
-    <row r="224" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:13">
       <c r="A224" s="3">
         <v>10</v>
       </c>
@@ -16895,7 +16938,7 @@
       <c r="L224" s="7"/>
       <c r="M224" s="7"/>
     </row>
-    <row r="225" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:13">
       <c r="A225" s="3">
         <v>10</v>
       </c>
@@ -16924,7 +16967,7 @@
       <c r="L225" s="7"/>
       <c r="M225" s="7"/>
     </row>
-    <row r="226" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:13">
       <c r="A226" s="3">
         <v>10</v>
       </c>
@@ -16953,7 +16996,7 @@
       <c r="L226" s="7"/>
       <c r="M226" s="7"/>
     </row>
-    <row r="227" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:13">
       <c r="A227" s="3">
         <v>10</v>
       </c>
@@ -16982,7 +17025,7 @@
       <c r="L227" s="7"/>
       <c r="M227" s="7"/>
     </row>
-    <row r="228" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:13">
       <c r="A228" s="3">
         <v>10</v>
       </c>
@@ -17015,8 +17058,8 @@
   <autoFilter ref="A1:M228"/>
   <printOptions horizontalCentered="1" gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
-  <pageSetup scale="58" fitToHeight="0" orientation="landscape" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <pageSetup scale="58" fitToHeight="0" orientation="landscape"/>
+  <legacyDrawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Resize comments for readability
</commit_message>
<xml_diff>
--- a/Listings.xlsx
+++ b/Listings.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="27022"/>
-  <workbookPr autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="820" yWindow="140" windowWidth="22420" windowHeight="17520"/>
+    <workbookView xWindow="825" yWindow="135" windowWidth="22425" windowHeight="17520"/>
   </bookViews>
   <sheets>
     <sheet name="Listings" sheetId="1" r:id="rId1"/>
@@ -10425,7 +10425,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -10433,32 +10433,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+  <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:M228"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C1" sqref="C1:C1048576"/>
+      <pane ySplit="1" topLeftCell="A200" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="106.83203125" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="30.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.6640625" customWidth="1"/>
-    <col min="8" max="11" width="10.6640625" customWidth="1"/>
+    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="106.85546875" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="30.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.7109375" customWidth="1"/>
+    <col min="8" max="11" width="10.7109375" customWidth="1"/>
     <col min="12" max="12" width="11" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.6640625" customWidth="1"/>
-    <col min="19" max="19" width="8.83203125" customWidth="1"/>
+    <col min="13" max="13" width="10.7109375" customWidth="1"/>
+    <col min="19" max="19" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -10499,7 +10499,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -10522,7 +10522,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -10551,7 +10551,7 @@
       <c r="L3" s="7"/>
       <c r="M3" s="7"/>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>1</v>
       </c>
@@ -10580,7 +10580,7 @@
       <c r="L4" s="7"/>
       <c r="M4" s="7"/>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>1</v>
       </c>
@@ -10609,7 +10609,7 @@
       <c r="L5" s="7"/>
       <c r="M5" s="7"/>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>1</v>
       </c>
@@ -10638,7 +10638,7 @@
       <c r="L6" s="7"/>
       <c r="M6" s="7"/>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>1</v>
       </c>
@@ -10667,7 +10667,7 @@
       <c r="L7" s="7"/>
       <c r="M7" s="7"/>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>1</v>
       </c>
@@ -10696,7 +10696,7 @@
       <c r="L8" s="8"/>
       <c r="M8" s="8"/>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>1</v>
       </c>
@@ -10725,7 +10725,7 @@
       <c r="L9" s="7"/>
       <c r="M9" s="8"/>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>1</v>
       </c>
@@ -10754,7 +10754,7 @@
       <c r="L10" s="7"/>
       <c r="M10" s="8"/>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>1</v>
       </c>
@@ -10783,7 +10783,7 @@
       <c r="L11" s="7"/>
       <c r="M11" s="7"/>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>1</v>
       </c>
@@ -10812,7 +10812,7 @@
       <c r="L12" s="7"/>
       <c r="M12" s="7"/>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>1</v>
       </c>
@@ -10841,7 +10841,7 @@
       <c r="L13" s="7"/>
       <c r="M13" s="7"/>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>1</v>
       </c>
@@ -10870,7 +10870,7 @@
       <c r="L14" s="7"/>
       <c r="M14" s="7"/>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>1</v>
       </c>
@@ -10893,7 +10893,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="16" spans="1:13">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>1</v>
       </c>
@@ -10916,7 +10916,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="17" spans="1:13">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>2</v>
       </c>
@@ -10945,7 +10945,7 @@
       <c r="L17" s="8"/>
       <c r="M17" s="8"/>
     </row>
-    <row r="18" spans="1:13">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>2</v>
       </c>
@@ -10974,7 +10974,7 @@
       <c r="L18" s="8"/>
       <c r="M18" s="8"/>
     </row>
-    <row r="19" spans="1:13">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>2</v>
       </c>
@@ -11003,7 +11003,7 @@
       <c r="L19" s="8"/>
       <c r="M19" s="8"/>
     </row>
-    <row r="20" spans="1:13">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>2</v>
       </c>
@@ -11032,7 +11032,7 @@
       <c r="L20" s="8"/>
       <c r="M20" s="8"/>
     </row>
-    <row r="21" spans="1:13">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>2</v>
       </c>
@@ -11061,7 +11061,7 @@
       <c r="L21" s="7"/>
       <c r="M21" s="8"/>
     </row>
-    <row r="22" spans="1:13">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>2</v>
       </c>
@@ -11090,7 +11090,7 @@
       <c r="L22" s="7"/>
       <c r="M22" s="8"/>
     </row>
-    <row r="23" spans="1:13">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>2</v>
       </c>
@@ -11119,7 +11119,7 @@
       <c r="L23" s="8"/>
       <c r="M23" s="7"/>
     </row>
-    <row r="24" spans="1:13">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>2</v>
       </c>
@@ -11148,7 +11148,7 @@
       <c r="L24" s="7"/>
       <c r="M24" s="7"/>
     </row>
-    <row r="25" spans="1:13">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>2</v>
       </c>
@@ -11177,7 +11177,7 @@
       <c r="L25" s="7"/>
       <c r="M25" s="7"/>
     </row>
-    <row r="26" spans="1:13">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>2</v>
       </c>
@@ -11206,7 +11206,7 @@
       <c r="L26" s="7"/>
       <c r="M26" s="7"/>
     </row>
-    <row r="27" spans="1:13">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>2</v>
       </c>
@@ -11235,7 +11235,7 @@
       <c r="L27" s="7"/>
       <c r="M27" s="7"/>
     </row>
-    <row r="28" spans="1:13">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>2</v>
       </c>
@@ -11264,7 +11264,7 @@
       <c r="L28" s="7"/>
       <c r="M28" s="7"/>
     </row>
-    <row r="29" spans="1:13">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>2</v>
       </c>
@@ -11293,7 +11293,7 @@
       <c r="L29" s="7"/>
       <c r="M29" s="7"/>
     </row>
-    <row r="30" spans="1:13">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>2</v>
       </c>
@@ -11322,7 +11322,7 @@
       <c r="L30" s="7"/>
       <c r="M30" s="7"/>
     </row>
-    <row r="31" spans="1:13">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>2</v>
       </c>
@@ -11351,7 +11351,7 @@
       <c r="L31" s="7"/>
       <c r="M31" s="7"/>
     </row>
-    <row r="32" spans="1:13">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>2</v>
       </c>
@@ -11380,7 +11380,7 @@
       <c r="L32" s="7"/>
       <c r="M32" s="7"/>
     </row>
-    <row r="33" spans="1:13">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>2</v>
       </c>
@@ -11409,7 +11409,7 @@
       <c r="L33" s="7"/>
       <c r="M33" s="7"/>
     </row>
-    <row r="34" spans="1:13">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>2</v>
       </c>
@@ -11438,7 +11438,7 @@
       <c r="L34" s="7"/>
       <c r="M34" s="7"/>
     </row>
-    <row r="35" spans="1:13">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>2</v>
       </c>
@@ -11467,7 +11467,7 @@
       <c r="L35" s="9"/>
       <c r="M35" s="7"/>
     </row>
-    <row r="36" spans="1:13">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>2</v>
       </c>
@@ -11496,7 +11496,7 @@
       <c r="L36" s="9"/>
       <c r="M36" s="7"/>
     </row>
-    <row r="37" spans="1:13">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>2</v>
       </c>
@@ -11525,7 +11525,7 @@
       <c r="L37" s="7"/>
       <c r="M37" s="7"/>
     </row>
-    <row r="38" spans="1:13">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
         <v>2</v>
       </c>
@@ -11554,7 +11554,7 @@
       <c r="L38" s="7"/>
       <c r="M38" s="7"/>
     </row>
-    <row r="39" spans="1:13">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>2</v>
       </c>
@@ -11583,7 +11583,7 @@
       <c r="L39" s="7"/>
       <c r="M39" s="7"/>
     </row>
-    <row r="40" spans="1:13">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
         <v>2</v>
       </c>
@@ -11612,7 +11612,7 @@
       <c r="L40" s="7"/>
       <c r="M40" s="7"/>
     </row>
-    <row r="41" spans="1:13">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <v>2</v>
       </c>
@@ -11641,7 +11641,7 @@
       <c r="L41" s="7"/>
       <c r="M41" s="7"/>
     </row>
-    <row r="42" spans="1:13">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
         <v>2</v>
       </c>
@@ -11665,7 +11665,7 @@
       </c>
       <c r="J42" s="11"/>
     </row>
-    <row r="43" spans="1:13">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
         <v>2</v>
       </c>
@@ -11689,7 +11689,7 @@
       </c>
       <c r="J43" s="11"/>
     </row>
-    <row r="44" spans="1:13">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
         <v>2</v>
       </c>
@@ -11718,7 +11718,7 @@
       <c r="L44" s="7"/>
       <c r="M44" s="7"/>
     </row>
-    <row r="45" spans="1:13">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
         <v>2</v>
       </c>
@@ -11747,7 +11747,7 @@
       <c r="L45" s="7"/>
       <c r="M45" s="7"/>
     </row>
-    <row r="46" spans="1:13">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
         <v>2</v>
       </c>
@@ -11776,7 +11776,7 @@
       <c r="L46" s="7"/>
       <c r="M46" s="7"/>
     </row>
-    <row r="47" spans="1:13">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
         <v>2</v>
       </c>
@@ -11805,7 +11805,7 @@
       <c r="L47" s="7"/>
       <c r="M47" s="7"/>
     </row>
-    <row r="48" spans="1:13">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
         <v>2</v>
       </c>
@@ -11834,7 +11834,7 @@
       <c r="L48" s="7"/>
       <c r="M48" s="7"/>
     </row>
-    <row r="49" spans="1:13">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
         <v>3</v>
       </c>
@@ -11863,7 +11863,7 @@
       <c r="L49" s="7"/>
       <c r="M49" s="7"/>
     </row>
-    <row r="50" spans="1:13">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" s="3">
         <v>3</v>
       </c>
@@ -11892,7 +11892,7 @@
       <c r="L50" s="7"/>
       <c r="M50" s="7"/>
     </row>
-    <row r="51" spans="1:13">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" s="3">
         <v>3</v>
       </c>
@@ -11921,7 +11921,7 @@
       <c r="L51" s="7"/>
       <c r="M51" s="7"/>
     </row>
-    <row r="52" spans="1:13">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" s="3">
         <v>3</v>
       </c>
@@ -11950,7 +11950,7 @@
       <c r="L52" s="7"/>
       <c r="M52" s="7"/>
     </row>
-    <row r="53" spans="1:13">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" s="3">
         <v>3</v>
       </c>
@@ -11979,7 +11979,7 @@
       <c r="L53" s="7"/>
       <c r="M53" s="7"/>
     </row>
-    <row r="54" spans="1:13">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" s="3">
         <v>3</v>
       </c>
@@ -12008,7 +12008,7 @@
       <c r="L54" s="8"/>
       <c r="M54" s="8"/>
     </row>
-    <row r="55" spans="1:13">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55" s="3">
         <v>3</v>
       </c>
@@ -12037,7 +12037,7 @@
       <c r="L55" s="9"/>
       <c r="M55" s="7"/>
     </row>
-    <row r="56" spans="1:13">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" s="3">
         <v>3</v>
       </c>
@@ -12066,7 +12066,7 @@
       <c r="L56" s="7"/>
       <c r="M56" s="7"/>
     </row>
-    <row r="57" spans="1:13">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57" s="3">
         <v>3</v>
       </c>
@@ -12095,7 +12095,7 @@
       <c r="L57" s="7"/>
       <c r="M57" s="7"/>
     </row>
-    <row r="58" spans="1:13">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58" s="3">
         <v>3</v>
       </c>
@@ -12124,7 +12124,7 @@
       <c r="L58" s="7"/>
       <c r="M58" s="7"/>
     </row>
-    <row r="59" spans="1:13">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59" s="3">
         <v>3</v>
       </c>
@@ -12153,7 +12153,7 @@
       <c r="L59" s="9"/>
       <c r="M59" s="7"/>
     </row>
-    <row r="60" spans="1:13">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60" s="3">
         <v>4</v>
       </c>
@@ -12182,7 +12182,7 @@
       <c r="L60" s="7"/>
       <c r="M60" s="7"/>
     </row>
-    <row r="61" spans="1:13">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61" s="3">
         <v>4</v>
       </c>
@@ -12211,7 +12211,7 @@
       <c r="L61" s="7"/>
       <c r="M61" s="7"/>
     </row>
-    <row r="62" spans="1:13">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A62" s="3">
         <v>4</v>
       </c>
@@ -12240,7 +12240,7 @@
       <c r="L62" s="7"/>
       <c r="M62" s="7"/>
     </row>
-    <row r="63" spans="1:13">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63" s="3">
         <v>4</v>
       </c>
@@ -12269,7 +12269,7 @@
       <c r="L63" s="7"/>
       <c r="M63" s="7"/>
     </row>
-    <row r="64" spans="1:13">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A64" s="3">
         <v>4</v>
       </c>
@@ -12298,7 +12298,7 @@
       <c r="L64" s="7"/>
       <c r="M64" s="7"/>
     </row>
-    <row r="65" spans="1:13">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A65" s="3">
         <v>4</v>
       </c>
@@ -12327,7 +12327,7 @@
       <c r="L65" s="7"/>
       <c r="M65" s="7"/>
     </row>
-    <row r="66" spans="1:13">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A66" s="3">
         <v>4</v>
       </c>
@@ -12356,7 +12356,7 @@
       <c r="L66" s="16"/>
       <c r="M66" s="16"/>
     </row>
-    <row r="67" spans="1:13">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A67" s="3">
         <v>4</v>
       </c>
@@ -12385,7 +12385,7 @@
       <c r="L67" s="7"/>
       <c r="M67" s="7"/>
     </row>
-    <row r="68" spans="1:13">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A68" s="3">
         <v>4</v>
       </c>
@@ -12414,7 +12414,7 @@
       <c r="L68" s="7"/>
       <c r="M68" s="7"/>
     </row>
-    <row r="69" spans="1:13">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A69" s="3">
         <v>4</v>
       </c>
@@ -12443,7 +12443,7 @@
       <c r="L69" s="7"/>
       <c r="M69" s="7"/>
     </row>
-    <row r="70" spans="1:13">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A70" s="3">
         <v>4</v>
       </c>
@@ -12472,7 +12472,7 @@
       <c r="L70" s="7"/>
       <c r="M70" s="7"/>
     </row>
-    <row r="71" spans="1:13">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A71" s="3">
         <v>4</v>
       </c>
@@ -12501,7 +12501,7 @@
       <c r="L71" s="7"/>
       <c r="M71" s="7"/>
     </row>
-    <row r="72" spans="1:13">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A72" s="3">
         <v>4</v>
       </c>
@@ -12530,7 +12530,7 @@
       <c r="L72" s="7"/>
       <c r="M72" s="7"/>
     </row>
-    <row r="73" spans="1:13">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A73" s="3">
         <v>4</v>
       </c>
@@ -12559,7 +12559,7 @@
       <c r="L73" s="7"/>
       <c r="M73" s="7"/>
     </row>
-    <row r="74" spans="1:13">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A74" s="3">
         <v>4</v>
       </c>
@@ -12588,7 +12588,7 @@
       <c r="L74" s="7"/>
       <c r="M74" s="7"/>
     </row>
-    <row r="75" spans="1:13">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A75" s="3">
         <v>4</v>
       </c>
@@ -12617,7 +12617,7 @@
       <c r="L75" s="7"/>
       <c r="M75" s="7"/>
     </row>
-    <row r="76" spans="1:13">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A76" s="3">
         <v>4</v>
       </c>
@@ -12646,7 +12646,7 @@
       <c r="L76" s="7"/>
       <c r="M76" s="7"/>
     </row>
-    <row r="77" spans="1:13">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A77" s="3">
         <v>4</v>
       </c>
@@ -12675,7 +12675,7 @@
       <c r="L77" s="7"/>
       <c r="M77" s="7"/>
     </row>
-    <row r="78" spans="1:13">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A78" s="3">
         <v>4</v>
       </c>
@@ -12704,7 +12704,7 @@
       <c r="L78" s="7"/>
       <c r="M78" s="7"/>
     </row>
-    <row r="79" spans="1:13">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A79" s="3">
         <v>4</v>
       </c>
@@ -12733,7 +12733,7 @@
       <c r="L79" s="7"/>
       <c r="M79" s="7"/>
     </row>
-    <row r="80" spans="1:13">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A80" s="3">
         <v>4</v>
       </c>
@@ -12762,7 +12762,7 @@
       <c r="L80" s="7"/>
       <c r="M80" s="7"/>
     </row>
-    <row r="81" spans="1:13">
+    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A81" s="3">
         <v>4</v>
       </c>
@@ -12791,7 +12791,7 @@
       <c r="L81" s="7"/>
       <c r="M81" s="7"/>
     </row>
-    <row r="82" spans="1:13">
+    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A82" s="3">
         <v>4</v>
       </c>
@@ -12820,7 +12820,7 @@
       <c r="L82" s="7"/>
       <c r="M82" s="7"/>
     </row>
-    <row r="83" spans="1:13">
+    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A83" s="3">
         <v>4</v>
       </c>
@@ -12849,7 +12849,7 @@
       <c r="L83" s="7"/>
       <c r="M83" s="7"/>
     </row>
-    <row r="84" spans="1:13">
+    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A84" s="3">
         <v>4</v>
       </c>
@@ -12878,7 +12878,7 @@
       <c r="L84" s="7"/>
       <c r="M84" s="7"/>
     </row>
-    <row r="85" spans="1:13">
+    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A85" s="3">
         <v>4</v>
       </c>
@@ -12907,7 +12907,7 @@
       <c r="L85" s="7"/>
       <c r="M85" s="7"/>
     </row>
-    <row r="86" spans="1:13">
+    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A86" s="3">
         <v>4</v>
       </c>
@@ -12936,7 +12936,7 @@
       <c r="L86" s="7"/>
       <c r="M86" s="7"/>
     </row>
-    <row r="87" spans="1:13">
+    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A87" s="3">
         <v>4</v>
       </c>
@@ -12965,7 +12965,7 @@
       <c r="L87" s="7"/>
       <c r="M87" s="7"/>
     </row>
-    <row r="88" spans="1:13">
+    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A88" s="3">
         <v>4</v>
       </c>
@@ -12994,7 +12994,7 @@
       <c r="L88" s="7"/>
       <c r="M88" s="7"/>
     </row>
-    <row r="89" spans="1:13">
+    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A89" s="3">
         <v>4</v>
       </c>
@@ -13023,7 +13023,7 @@
       <c r="L89" s="7"/>
       <c r="M89" s="7"/>
     </row>
-    <row r="90" spans="1:13">
+    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A90" s="3">
         <v>4</v>
       </c>
@@ -13052,7 +13052,7 @@
       <c r="L90" s="7"/>
       <c r="M90" s="7"/>
     </row>
-    <row r="91" spans="1:13">
+    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A91" s="3">
         <v>4</v>
       </c>
@@ -13081,7 +13081,7 @@
       <c r="L91" s="7"/>
       <c r="M91" s="7"/>
     </row>
-    <row r="92" spans="1:13">
+    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A92" s="3">
         <v>4</v>
       </c>
@@ -13110,7 +13110,7 @@
       <c r="L92" s="7"/>
       <c r="M92" s="7"/>
     </row>
-    <row r="93" spans="1:13">
+    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A93" s="3">
         <v>4</v>
       </c>
@@ -13139,7 +13139,7 @@
       <c r="L93" s="7"/>
       <c r="M93" s="7"/>
     </row>
-    <row r="94" spans="1:13">
+    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A94" s="3">
         <v>4</v>
       </c>
@@ -13168,7 +13168,7 @@
       <c r="L94" s="7"/>
       <c r="M94" s="7"/>
     </row>
-    <row r="95" spans="1:13">
+    <row r="95" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A95" s="3">
         <v>4</v>
       </c>
@@ -13197,7 +13197,7 @@
       <c r="L95" s="7"/>
       <c r="M95" s="7"/>
     </row>
-    <row r="96" spans="1:13">
+    <row r="96" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A96" s="3">
         <v>4</v>
       </c>
@@ -13226,7 +13226,7 @@
       <c r="L96" s="7"/>
       <c r="M96" s="7"/>
     </row>
-    <row r="97" spans="1:13">
+    <row r="97" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A97" s="3">
         <v>4</v>
       </c>
@@ -13255,7 +13255,7 @@
       <c r="L97" s="7"/>
       <c r="M97" s="7"/>
     </row>
-    <row r="98" spans="1:13">
+    <row r="98" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A98" s="3">
         <v>4</v>
       </c>
@@ -13284,7 +13284,7 @@
       <c r="L98" s="7"/>
       <c r="M98" s="7"/>
     </row>
-    <row r="99" spans="1:13">
+    <row r="99" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A99" s="3">
         <v>4</v>
       </c>
@@ -13313,7 +13313,7 @@
       <c r="L99" s="7"/>
       <c r="M99" s="7"/>
     </row>
-    <row r="100" spans="1:13">
+    <row r="100" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A100" s="3">
         <v>5</v>
       </c>
@@ -13342,7 +13342,7 @@
       <c r="L100" s="16"/>
       <c r="M100" s="16"/>
     </row>
-    <row r="101" spans="1:13">
+    <row r="101" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A101" s="3">
         <v>5</v>
       </c>
@@ -13371,7 +13371,7 @@
       <c r="L101" s="16"/>
       <c r="M101" s="16"/>
     </row>
-    <row r="102" spans="1:13">
+    <row r="102" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A102" s="3">
         <v>5</v>
       </c>
@@ -13400,7 +13400,7 @@
       <c r="L102" s="16"/>
       <c r="M102" s="16"/>
     </row>
-    <row r="103" spans="1:13">
+    <row r="103" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A103" s="3">
         <v>5</v>
       </c>
@@ -13429,7 +13429,7 @@
       <c r="L103" s="7"/>
       <c r="M103" s="7"/>
     </row>
-    <row r="104" spans="1:13">
+    <row r="104" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A104" s="3">
         <v>5</v>
       </c>
@@ -13458,7 +13458,7 @@
       <c r="L104" s="7"/>
       <c r="M104" s="7"/>
     </row>
-    <row r="105" spans="1:13">
+    <row r="105" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A105" s="3">
         <v>5</v>
       </c>
@@ -13487,7 +13487,7 @@
       <c r="L105" s="7"/>
       <c r="M105" s="7"/>
     </row>
-    <row r="106" spans="1:13">
+    <row r="106" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A106" s="3">
         <v>5</v>
       </c>
@@ -13516,7 +13516,7 @@
       <c r="L106" s="7"/>
       <c r="M106" s="7"/>
     </row>
-    <row r="107" spans="1:13">
+    <row r="107" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A107" s="3">
         <v>5</v>
       </c>
@@ -13545,7 +13545,7 @@
       <c r="L107" s="7"/>
       <c r="M107" s="7"/>
     </row>
-    <row r="108" spans="1:13">
+    <row r="108" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A108" s="3">
         <v>5</v>
       </c>
@@ -13574,7 +13574,7 @@
       <c r="L108" s="7"/>
       <c r="M108" s="7"/>
     </row>
-    <row r="109" spans="1:13">
+    <row r="109" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A109" s="3">
         <v>5</v>
       </c>
@@ -13603,7 +13603,7 @@
       <c r="L109" s="7"/>
       <c r="M109" s="7"/>
     </row>
-    <row r="110" spans="1:13">
+    <row r="110" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A110" s="3">
         <v>5</v>
       </c>
@@ -13632,7 +13632,7 @@
       <c r="L110" s="8"/>
       <c r="M110" s="7"/>
     </row>
-    <row r="111" spans="1:13">
+    <row r="111" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A111" s="3">
         <v>5</v>
       </c>
@@ -13661,7 +13661,7 @@
       <c r="L111" s="7"/>
       <c r="M111" s="7"/>
     </row>
-    <row r="112" spans="1:13">
+    <row r="112" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A112" s="3">
         <v>5</v>
       </c>
@@ -13690,7 +13690,7 @@
       <c r="L112" s="7"/>
       <c r="M112" s="7"/>
     </row>
-    <row r="113" spans="1:13">
+    <row r="113" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A113" s="3">
         <v>5</v>
       </c>
@@ -13719,7 +13719,7 @@
       <c r="L113" s="7"/>
       <c r="M113" s="7"/>
     </row>
-    <row r="114" spans="1:13">
+    <row r="114" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A114" s="3">
         <v>5</v>
       </c>
@@ -13748,7 +13748,7 @@
       <c r="L114" s="9"/>
       <c r="M114" s="7"/>
     </row>
-    <row r="115" spans="1:13">
+    <row r="115" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A115" s="3">
         <v>5</v>
       </c>
@@ -13777,7 +13777,7 @@
       <c r="L115" s="9"/>
       <c r="M115" s="7"/>
     </row>
-    <row r="116" spans="1:13">
+    <row r="116" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A116" s="3">
         <v>5</v>
       </c>
@@ -13806,7 +13806,7 @@
       <c r="L116" s="7"/>
       <c r="M116" s="7"/>
     </row>
-    <row r="117" spans="1:13">
+    <row r="117" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A117" s="3">
         <v>5</v>
       </c>
@@ -13835,7 +13835,7 @@
       <c r="L117" s="7"/>
       <c r="M117" s="7"/>
     </row>
-    <row r="118" spans="1:13">
+    <row r="118" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A118" s="3">
         <v>5</v>
       </c>
@@ -13864,7 +13864,7 @@
       <c r="L118" s="7"/>
       <c r="M118" s="7"/>
     </row>
-    <row r="119" spans="1:13">
+    <row r="119" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A119" s="3">
         <v>5</v>
       </c>
@@ -13893,7 +13893,7 @@
       <c r="L119" s="7"/>
       <c r="M119" s="7"/>
     </row>
-    <row r="120" spans="1:13">
+    <row r="120" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A120" s="3">
         <v>5</v>
       </c>
@@ -13922,7 +13922,7 @@
       <c r="L120" s="7"/>
       <c r="M120" s="7"/>
     </row>
-    <row r="121" spans="1:13">
+    <row r="121" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A121" s="3">
         <v>5</v>
       </c>
@@ -13951,7 +13951,7 @@
       <c r="L121" s="7"/>
       <c r="M121" s="7"/>
     </row>
-    <row r="122" spans="1:13">
+    <row r="122" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A122" s="3">
         <v>5</v>
       </c>
@@ -13980,7 +13980,7 @@
       <c r="L122" s="7"/>
       <c r="M122" s="7"/>
     </row>
-    <row r="123" spans="1:13">
+    <row r="123" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A123" s="3">
         <v>5</v>
       </c>
@@ -14009,7 +14009,7 @@
       <c r="L123" s="7"/>
       <c r="M123" s="9"/>
     </row>
-    <row r="124" spans="1:13">
+    <row r="124" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A124" s="3">
         <v>5</v>
       </c>
@@ -14038,7 +14038,7 @@
       <c r="L124" s="7"/>
       <c r="M124" s="9"/>
     </row>
-    <row r="125" spans="1:13">
+    <row r="125" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A125" s="3">
         <v>5</v>
       </c>
@@ -14067,7 +14067,7 @@
       <c r="L125" s="7"/>
       <c r="M125" s="9"/>
     </row>
-    <row r="126" spans="1:13">
+    <row r="126" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A126" s="3">
         <v>5</v>
       </c>
@@ -14096,7 +14096,7 @@
       <c r="L126" s="7"/>
       <c r="M126" s="7"/>
     </row>
-    <row r="127" spans="1:13">
+    <row r="127" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A127" s="3">
         <v>5</v>
       </c>
@@ -14125,7 +14125,7 @@
       <c r="L127" s="9"/>
       <c r="M127" s="7"/>
     </row>
-    <row r="128" spans="1:13">
+    <row r="128" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A128" s="3">
         <v>5</v>
       </c>
@@ -14154,7 +14154,7 @@
       <c r="L128" s="7"/>
       <c r="M128" s="7"/>
     </row>
-    <row r="129" spans="1:13">
+    <row r="129" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A129" s="3">
         <v>5</v>
       </c>
@@ -14183,7 +14183,7 @@
       <c r="L129" s="7"/>
       <c r="M129" s="7"/>
     </row>
-    <row r="130" spans="1:13">
+    <row r="130" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A130" s="3">
         <v>5</v>
       </c>
@@ -14212,7 +14212,7 @@
       <c r="L130" s="7"/>
       <c r="M130" s="7"/>
     </row>
-    <row r="131" spans="1:13">
+    <row r="131" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A131" s="3">
         <v>5</v>
       </c>
@@ -14241,7 +14241,7 @@
       <c r="L131" s="7"/>
       <c r="M131" s="7"/>
     </row>
-    <row r="132" spans="1:13">
+    <row r="132" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A132" s="3">
         <v>5</v>
       </c>
@@ -14270,7 +14270,7 @@
       <c r="L132" s="7"/>
       <c r="M132" s="7"/>
     </row>
-    <row r="133" spans="1:13">
+    <row r="133" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A133" s="3">
         <v>5</v>
       </c>
@@ -14299,7 +14299,7 @@
       <c r="L133" s="7"/>
       <c r="M133" s="7"/>
     </row>
-    <row r="134" spans="1:13">
+    <row r="134" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A134" s="3">
         <v>6</v>
       </c>
@@ -14328,7 +14328,7 @@
       <c r="L134" s="7"/>
       <c r="M134" s="7"/>
     </row>
-    <row r="135" spans="1:13">
+    <row r="135" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A135" s="3">
         <v>6</v>
       </c>
@@ -14357,7 +14357,7 @@
       <c r="L135" s="7"/>
       <c r="M135" s="7"/>
     </row>
-    <row r="136" spans="1:13">
+    <row r="136" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A136" s="3">
         <v>6</v>
       </c>
@@ -14386,7 +14386,7 @@
       <c r="L136" s="7"/>
       <c r="M136" s="7"/>
     </row>
-    <row r="137" spans="1:13">
+    <row r="137" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A137" s="3">
         <v>6</v>
       </c>
@@ -14415,7 +14415,7 @@
       <c r="L137" s="7"/>
       <c r="M137" s="7"/>
     </row>
-    <row r="138" spans="1:13">
+    <row r="138" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A138" s="3">
         <v>6</v>
       </c>
@@ -14444,7 +14444,7 @@
       <c r="L138" s="7"/>
       <c r="M138" s="7"/>
     </row>
-    <row r="139" spans="1:13">
+    <row r="139" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A139" s="3">
         <v>6</v>
       </c>
@@ -14473,7 +14473,7 @@
       <c r="L139" s="7"/>
       <c r="M139" s="7"/>
     </row>
-    <row r="140" spans="1:13">
+    <row r="140" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A140" s="3">
         <v>6</v>
       </c>
@@ -14502,7 +14502,7 @@
       <c r="L140" s="7"/>
       <c r="M140" s="7"/>
     </row>
-    <row r="141" spans="1:13">
+    <row r="141" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A141" s="3">
         <v>6</v>
       </c>
@@ -14531,7 +14531,7 @@
       <c r="L141" s="7"/>
       <c r="M141" s="7"/>
     </row>
-    <row r="142" spans="1:13">
+    <row r="142" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A142" s="3">
         <v>6</v>
       </c>
@@ -14560,7 +14560,7 @@
       <c r="L142" s="7"/>
       <c r="M142" s="7"/>
     </row>
-    <row r="143" spans="1:13">
+    <row r="143" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A143" s="3">
         <v>6</v>
       </c>
@@ -14589,7 +14589,7 @@
       <c r="L143" s="7"/>
       <c r="M143" s="7"/>
     </row>
-    <row r="144" spans="1:13">
+    <row r="144" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A144" s="3">
         <v>6</v>
       </c>
@@ -14618,7 +14618,7 @@
       <c r="L144" s="7"/>
       <c r="M144" s="7"/>
     </row>
-    <row r="145" spans="1:13">
+    <row r="145" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A145" s="3">
         <v>6</v>
       </c>
@@ -14647,7 +14647,7 @@
       <c r="L145" s="7"/>
       <c r="M145" s="7"/>
     </row>
-    <row r="146" spans="1:13">
+    <row r="146" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A146" s="3">
         <v>6</v>
       </c>
@@ -14676,7 +14676,7 @@
       <c r="L146" s="7"/>
       <c r="M146" s="7"/>
     </row>
-    <row r="147" spans="1:13">
+    <row r="147" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A147" s="3">
         <v>6</v>
       </c>
@@ -14705,7 +14705,7 @@
       <c r="L147" s="7"/>
       <c r="M147" s="7"/>
     </row>
-    <row r="148" spans="1:13">
+    <row r="148" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A148" s="3">
         <v>6</v>
       </c>
@@ -14734,7 +14734,7 @@
       <c r="L148" s="7"/>
       <c r="M148" s="7"/>
     </row>
-    <row r="149" spans="1:13">
+    <row r="149" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A149" s="3">
         <v>6</v>
       </c>
@@ -14763,7 +14763,7 @@
       <c r="L149" s="7"/>
       <c r="M149" s="7"/>
     </row>
-    <row r="150" spans="1:13">
+    <row r="150" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A150" s="3">
         <v>6</v>
       </c>
@@ -14792,7 +14792,7 @@
       <c r="L150" s="7"/>
       <c r="M150" s="7"/>
     </row>
-    <row r="151" spans="1:13">
+    <row r="151" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A151" s="3">
         <v>6</v>
       </c>
@@ -14821,7 +14821,7 @@
       <c r="L151" s="7"/>
       <c r="M151" s="7"/>
     </row>
-    <row r="152" spans="1:13">
+    <row r="152" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A152" s="3">
         <v>6</v>
       </c>
@@ -14850,7 +14850,7 @@
       <c r="L152" s="7"/>
       <c r="M152" s="7"/>
     </row>
-    <row r="153" spans="1:13">
+    <row r="153" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A153" s="3">
         <v>7</v>
       </c>
@@ -14879,7 +14879,7 @@
       <c r="L153" s="8"/>
       <c r="M153" s="8"/>
     </row>
-    <row r="154" spans="1:13">
+    <row r="154" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A154" s="3">
         <v>7</v>
       </c>
@@ -14908,7 +14908,7 @@
       <c r="L154" s="8"/>
       <c r="M154" s="8"/>
     </row>
-    <row r="155" spans="1:13">
+    <row r="155" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A155" s="3">
         <v>7</v>
       </c>
@@ -14937,7 +14937,7 @@
       <c r="L155" s="8"/>
       <c r="M155" s="8"/>
     </row>
-    <row r="156" spans="1:13">
+    <row r="156" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A156" s="3">
         <v>7</v>
       </c>
@@ -14966,7 +14966,7 @@
       <c r="L156" s="8"/>
       <c r="M156" s="8"/>
     </row>
-    <row r="157" spans="1:13">
+    <row r="157" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A157" s="3">
         <v>7</v>
       </c>
@@ -14995,7 +14995,7 @@
       <c r="L157" s="8"/>
       <c r="M157" s="8"/>
     </row>
-    <row r="158" spans="1:13">
+    <row r="158" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A158" s="3">
         <v>7</v>
       </c>
@@ -15024,7 +15024,7 @@
       <c r="L158" s="8"/>
       <c r="M158" s="8"/>
     </row>
-    <row r="159" spans="1:13">
+    <row r="159" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A159" s="3">
         <v>7</v>
       </c>
@@ -15053,7 +15053,7 @@
       <c r="L159" s="8"/>
       <c r="M159" s="8"/>
     </row>
-    <row r="160" spans="1:13">
+    <row r="160" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A160" s="3">
         <v>7</v>
       </c>
@@ -15082,7 +15082,7 @@
       <c r="L160" s="8"/>
       <c r="M160" s="8"/>
     </row>
-    <row r="161" spans="1:13">
+    <row r="161" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A161" s="3">
         <v>7</v>
       </c>
@@ -15111,7 +15111,7 @@
       <c r="L161" s="7"/>
       <c r="M161" s="8"/>
     </row>
-    <row r="162" spans="1:13">
+    <row r="162" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A162" s="3">
         <v>7</v>
       </c>
@@ -15140,7 +15140,7 @@
       <c r="L162" s="7"/>
       <c r="M162" s="8"/>
     </row>
-    <row r="163" spans="1:13">
+    <row r="163" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A163" s="3">
         <v>7</v>
       </c>
@@ -15169,7 +15169,7 @@
       <c r="L163" s="8"/>
       <c r="M163" s="7"/>
     </row>
-    <row r="164" spans="1:13">
+    <row r="164" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A164" s="3">
         <v>7</v>
       </c>
@@ -15198,7 +15198,7 @@
       <c r="L164" s="8"/>
       <c r="M164" s="7"/>
     </row>
-    <row r="165" spans="1:13">
+    <row r="165" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A165" s="3">
         <v>7</v>
       </c>
@@ -15227,7 +15227,7 @@
       <c r="L165" s="8"/>
       <c r="M165" s="7"/>
     </row>
-    <row r="166" spans="1:13">
+    <row r="166" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A166" s="3">
         <v>7</v>
       </c>
@@ -15256,7 +15256,7 @@
       <c r="L166" s="8"/>
       <c r="M166" s="7"/>
     </row>
-    <row r="167" spans="1:13">
+    <row r="167" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A167" s="3">
         <v>7</v>
       </c>
@@ -15285,7 +15285,7 @@
       <c r="L167" s="8"/>
       <c r="M167" s="7"/>
     </row>
-    <row r="168" spans="1:13">
+    <row r="168" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A168" s="3">
         <v>7</v>
       </c>
@@ -15314,7 +15314,7 @@
       <c r="L168" s="8"/>
       <c r="M168" s="7"/>
     </row>
-    <row r="169" spans="1:13">
+    <row r="169" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A169" s="3">
         <v>7</v>
       </c>
@@ -15343,7 +15343,7 @@
       <c r="L169" s="8"/>
       <c r="M169" s="7"/>
     </row>
-    <row r="170" spans="1:13">
+    <row r="170" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A170" s="3">
         <v>7</v>
       </c>
@@ -15372,7 +15372,7 @@
       <c r="L170" s="7"/>
       <c r="M170" s="7"/>
     </row>
-    <row r="171" spans="1:13">
+    <row r="171" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A171" s="3">
         <v>7</v>
       </c>
@@ -15401,7 +15401,7 @@
       <c r="L171" s="8"/>
       <c r="M171" s="8"/>
     </row>
-    <row r="172" spans="1:13">
+    <row r="172" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A172" s="3">
         <v>7</v>
       </c>
@@ -15430,7 +15430,7 @@
       <c r="L172" s="8"/>
       <c r="M172" s="8"/>
     </row>
-    <row r="173" spans="1:13">
+    <row r="173" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A173" s="3">
         <v>7</v>
       </c>
@@ -15459,7 +15459,7 @@
       <c r="L173" s="7"/>
       <c r="M173" s="7"/>
     </row>
-    <row r="174" spans="1:13">
+    <row r="174" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A174" s="3">
         <v>7</v>
       </c>
@@ -15488,7 +15488,7 @@
       <c r="L174" s="7"/>
       <c r="M174" s="7"/>
     </row>
-    <row r="175" spans="1:13">
+    <row r="175" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A175" s="3">
         <v>7</v>
       </c>
@@ -15517,7 +15517,7 @@
       <c r="L175" s="7"/>
       <c r="M175" s="7"/>
     </row>
-    <row r="176" spans="1:13">
+    <row r="176" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A176" s="3">
         <v>7</v>
       </c>
@@ -15546,7 +15546,7 @@
       <c r="L176" s="7"/>
       <c r="M176" s="7"/>
     </row>
-    <row r="177" spans="1:13">
+    <row r="177" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A177" s="3">
         <v>7</v>
       </c>
@@ -15575,7 +15575,7 @@
       <c r="L177" s="9"/>
       <c r="M177" s="9"/>
     </row>
-    <row r="178" spans="1:13">
+    <row r="178" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A178" s="3">
         <v>8</v>
       </c>
@@ -15604,7 +15604,7 @@
       <c r="L178" s="7"/>
       <c r="M178" s="7"/>
     </row>
-    <row r="179" spans="1:13">
+    <row r="179" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A179" s="3">
         <v>8</v>
       </c>
@@ -15633,7 +15633,7 @@
       <c r="L179" s="7"/>
       <c r="M179" s="7"/>
     </row>
-    <row r="180" spans="1:13">
+    <row r="180" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A180" s="3">
         <v>8</v>
       </c>
@@ -15662,7 +15662,7 @@
       <c r="L180" s="7"/>
       <c r="M180" s="7"/>
     </row>
-    <row r="181" spans="1:13">
+    <row r="181" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A181" s="3">
         <v>8</v>
       </c>
@@ -15691,7 +15691,7 @@
       <c r="L181" s="7"/>
       <c r="M181" s="7"/>
     </row>
-    <row r="182" spans="1:13">
+    <row r="182" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A182" s="3">
         <v>8</v>
       </c>
@@ -15720,7 +15720,7 @@
       <c r="L182" s="7"/>
       <c r="M182" s="7"/>
     </row>
-    <row r="183" spans="1:13">
+    <row r="183" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A183" s="3">
         <v>8</v>
       </c>
@@ -15749,7 +15749,7 @@
       <c r="L183" s="7"/>
       <c r="M183" s="7"/>
     </row>
-    <row r="184" spans="1:13">
+    <row r="184" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A184" s="3">
         <v>8</v>
       </c>
@@ -15778,7 +15778,7 @@
       <c r="L184" s="7"/>
       <c r="M184" s="7"/>
     </row>
-    <row r="185" spans="1:13">
+    <row r="185" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A185" s="3">
         <v>8</v>
       </c>
@@ -15807,7 +15807,7 @@
       <c r="L185" s="7"/>
       <c r="M185" s="7"/>
     </row>
-    <row r="186" spans="1:13">
+    <row r="186" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A186" s="3">
         <v>8</v>
       </c>
@@ -15836,7 +15836,7 @@
       <c r="L186" s="7"/>
       <c r="M186" s="7"/>
     </row>
-    <row r="187" spans="1:13">
+    <row r="187" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A187" s="3">
         <v>8</v>
       </c>
@@ -15865,7 +15865,7 @@
       <c r="L187" s="7"/>
       <c r="M187" s="7"/>
     </row>
-    <row r="188" spans="1:13">
+    <row r="188" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A188" s="3">
         <v>8</v>
       </c>
@@ -15894,7 +15894,7 @@
       <c r="L188" s="7"/>
       <c r="M188" s="7"/>
     </row>
-    <row r="189" spans="1:13">
+    <row r="189" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A189" s="3">
         <v>8</v>
       </c>
@@ -15923,7 +15923,7 @@
       <c r="L189" s="7"/>
       <c r="M189" s="7"/>
     </row>
-    <row r="190" spans="1:13">
+    <row r="190" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A190" s="3">
         <v>8</v>
       </c>
@@ -15952,7 +15952,7 @@
       <c r="L190" s="7"/>
       <c r="M190" s="7"/>
     </row>
-    <row r="191" spans="1:13">
+    <row r="191" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A191" s="3">
         <v>9</v>
       </c>
@@ -15981,7 +15981,7 @@
       <c r="L191" s="7"/>
       <c r="M191" s="7"/>
     </row>
-    <row r="192" spans="1:13">
+    <row r="192" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A192" s="3">
         <v>9</v>
       </c>
@@ -16010,7 +16010,7 @@
       <c r="L192" s="7"/>
       <c r="M192" s="7"/>
     </row>
-    <row r="193" spans="1:13">
+    <row r="193" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A193" s="3">
         <v>9</v>
       </c>
@@ -16039,7 +16039,7 @@
       <c r="L193" s="7"/>
       <c r="M193" s="7"/>
     </row>
-    <row r="194" spans="1:13">
+    <row r="194" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A194" s="3">
         <v>9</v>
       </c>
@@ -16068,7 +16068,7 @@
       <c r="L194" s="7"/>
       <c r="M194" s="7"/>
     </row>
-    <row r="195" spans="1:13">
+    <row r="195" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A195" s="3">
         <v>9</v>
       </c>
@@ -16097,7 +16097,7 @@
       <c r="L195" s="16"/>
       <c r="M195" s="16"/>
     </row>
-    <row r="196" spans="1:13">
+    <row r="196" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A196" s="3">
         <v>9</v>
       </c>
@@ -16126,7 +16126,7 @@
       <c r="L196" s="7"/>
       <c r="M196" s="7"/>
     </row>
-    <row r="197" spans="1:13">
+    <row r="197" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A197" s="3">
         <v>9</v>
       </c>
@@ -16155,7 +16155,7 @@
       <c r="L197" s="7"/>
       <c r="M197" s="7"/>
     </row>
-    <row r="198" spans="1:13">
+    <row r="198" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A198" s="3">
         <v>9</v>
       </c>
@@ -16184,7 +16184,7 @@
       <c r="L198" s="7"/>
       <c r="M198" s="7"/>
     </row>
-    <row r="199" spans="1:13">
+    <row r="199" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A199" s="3">
         <v>9</v>
       </c>
@@ -16213,7 +16213,7 @@
       <c r="L199" s="7"/>
       <c r="M199" s="7"/>
     </row>
-    <row r="200" spans="1:13">
+    <row r="200" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A200" s="3">
         <v>9</v>
       </c>
@@ -16242,7 +16242,7 @@
       <c r="L200" s="7"/>
       <c r="M200" s="7"/>
     </row>
-    <row r="201" spans="1:13">
+    <row r="201" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A201" s="3">
         <v>9</v>
       </c>
@@ -16271,7 +16271,7 @@
       <c r="L201" s="7"/>
       <c r="M201" s="7"/>
     </row>
-    <row r="202" spans="1:13">
+    <row r="202" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A202" s="3">
         <v>9</v>
       </c>
@@ -16300,7 +16300,7 @@
       <c r="L202" s="7"/>
       <c r="M202" s="7"/>
     </row>
-    <row r="203" spans="1:13">
+    <row r="203" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A203" s="3">
         <v>9</v>
       </c>
@@ -16329,7 +16329,7 @@
       <c r="L203" s="7"/>
       <c r="M203" s="7"/>
     </row>
-    <row r="204" spans="1:13">
+    <row r="204" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A204" s="3">
         <v>9</v>
       </c>
@@ -16358,7 +16358,7 @@
       <c r="L204" s="7"/>
       <c r="M204" s="7"/>
     </row>
-    <row r="205" spans="1:13">
+    <row r="205" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A205" s="3">
         <v>9</v>
       </c>
@@ -16387,7 +16387,7 @@
       <c r="L205" s="7"/>
       <c r="M205" s="7"/>
     </row>
-    <row r="206" spans="1:13">
+    <row r="206" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A206" s="3">
         <v>9</v>
       </c>
@@ -16416,7 +16416,7 @@
       <c r="L206" s="7"/>
       <c r="M206" s="7"/>
     </row>
-    <row r="207" spans="1:13">
+    <row r="207" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A207" s="3">
         <v>9</v>
       </c>
@@ -16445,7 +16445,7 @@
       <c r="L207" s="7"/>
       <c r="M207" s="7"/>
     </row>
-    <row r="208" spans="1:13">
+    <row r="208" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A208" s="3">
         <v>9</v>
       </c>
@@ -16474,7 +16474,7 @@
       <c r="L208" s="7"/>
       <c r="M208" s="7"/>
     </row>
-    <row r="209" spans="1:13">
+    <row r="209" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A209" s="3">
         <v>9</v>
       </c>
@@ -16503,7 +16503,7 @@
       <c r="L209" s="7"/>
       <c r="M209" s="7"/>
     </row>
-    <row r="210" spans="1:13">
+    <row r="210" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A210" s="3">
         <v>9</v>
       </c>
@@ -16532,7 +16532,7 @@
       <c r="L210" s="7"/>
       <c r="M210" s="7"/>
     </row>
-    <row r="211" spans="1:13">
+    <row r="211" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A211" s="3">
         <v>9</v>
       </c>
@@ -16561,7 +16561,7 @@
       <c r="L211" s="9"/>
       <c r="M211" s="9"/>
     </row>
-    <row r="212" spans="1:13">
+    <row r="212" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A212" s="3">
         <v>9</v>
       </c>
@@ -16590,7 +16590,7 @@
       <c r="L212" s="7"/>
       <c r="M212" s="7"/>
     </row>
-    <row r="213" spans="1:13">
+    <row r="213" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A213" s="3">
         <v>9</v>
       </c>
@@ -16619,7 +16619,7 @@
       <c r="L213" s="7"/>
       <c r="M213" s="7"/>
     </row>
-    <row r="214" spans="1:13">
+    <row r="214" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A214" s="3">
         <v>9</v>
       </c>
@@ -16648,7 +16648,7 @@
       <c r="L214" s="7"/>
       <c r="M214" s="7"/>
     </row>
-    <row r="215" spans="1:13">
+    <row r="215" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A215" s="3">
         <v>9</v>
       </c>
@@ -16677,7 +16677,7 @@
       <c r="L215" s="7"/>
       <c r="M215" s="7"/>
     </row>
-    <row r="216" spans="1:13">
+    <row r="216" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A216" s="3">
         <v>10</v>
       </c>
@@ -16706,7 +16706,7 @@
       <c r="L216" s="7"/>
       <c r="M216" s="7"/>
     </row>
-    <row r="217" spans="1:13">
+    <row r="217" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A217" s="3">
         <v>10</v>
       </c>
@@ -16735,7 +16735,7 @@
       <c r="L217" s="7"/>
       <c r="M217" s="7"/>
     </row>
-    <row r="218" spans="1:13">
+    <row r="218" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A218" s="3">
         <v>10</v>
       </c>
@@ -16764,7 +16764,7 @@
       <c r="L218" s="7"/>
       <c r="M218" s="7"/>
     </row>
-    <row r="219" spans="1:13">
+    <row r="219" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A219" s="3">
         <v>10</v>
       </c>
@@ -16793,7 +16793,7 @@
       <c r="L219" s="7"/>
       <c r="M219" s="7"/>
     </row>
-    <row r="220" spans="1:13">
+    <row r="220" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A220" s="3">
         <v>10</v>
       </c>
@@ -16822,7 +16822,7 @@
       <c r="L220" s="7"/>
       <c r="M220" s="7"/>
     </row>
-    <row r="221" spans="1:13">
+    <row r="221" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A221" s="3">
         <v>10</v>
       </c>
@@ -16851,7 +16851,7 @@
       <c r="L221" s="7"/>
       <c r="M221" s="7"/>
     </row>
-    <row r="222" spans="1:13">
+    <row r="222" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A222" s="3">
         <v>10</v>
       </c>
@@ -16880,7 +16880,7 @@
       <c r="L222" s="7"/>
       <c r="M222" s="7"/>
     </row>
-    <row r="223" spans="1:13">
+    <row r="223" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A223" s="3">
         <v>10</v>
       </c>
@@ -16909,7 +16909,7 @@
       <c r="L223" s="7"/>
       <c r="M223" s="7"/>
     </row>
-    <row r="224" spans="1:13">
+    <row r="224" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A224" s="3">
         <v>10</v>
       </c>
@@ -16938,7 +16938,7 @@
       <c r="L224" s="7"/>
       <c r="M224" s="7"/>
     </row>
-    <row r="225" spans="1:13">
+    <row r="225" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A225" s="3">
         <v>10</v>
       </c>
@@ -16967,7 +16967,7 @@
       <c r="L225" s="7"/>
       <c r="M225" s="7"/>
     </row>
-    <row r="226" spans="1:13">
+    <row r="226" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A226" s="3">
         <v>10</v>
       </c>
@@ -16996,7 +16996,7 @@
       <c r="L226" s="7"/>
       <c r="M226" s="7"/>
     </row>
-    <row r="227" spans="1:13">
+    <row r="227" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A227" s="3">
         <v>10</v>
       </c>
@@ -17025,7 +17025,7 @@
       <c r="L227" s="7"/>
       <c r="M227" s="7"/>
     </row>
-    <row r="228" spans="1:13">
+    <row r="228" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A228" s="3">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
Summary of Listings - applicable database systems
</commit_message>
<xml_diff>
--- a/Listings.xlsx
+++ b/Listings.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="27322"/>
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="825" yWindow="135" windowWidth="22425" windowHeight="17520"/>
+    <workbookView xWindow="820" yWindow="140" windowWidth="22420" windowHeight="17520"/>
   </bookViews>
   <sheets>
     <sheet name="Listings" sheetId="1" r:id="rId1"/>
@@ -10425,7 +10425,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -10439,26 +10439,26 @@
   <dimension ref="A1:M228"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A200" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K10" sqref="K10"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="106.85546875" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="30.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.7109375" customWidth="1"/>
-    <col min="8" max="11" width="10.7109375" customWidth="1"/>
+    <col min="2" max="2" width="5.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="106.83203125" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="30.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.6640625" customWidth="1"/>
+    <col min="8" max="11" width="10.6640625" customWidth="1"/>
     <col min="12" max="12" width="11" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.7109375" customWidth="1"/>
-    <col min="19" max="19" width="8.85546875" customWidth="1"/>
+    <col min="13" max="13" width="10.6640625" customWidth="1"/>
+    <col min="19" max="19" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -10499,7 +10499,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -10522,7 +10522,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -10551,7 +10551,7 @@
       <c r="L3" s="7"/>
       <c r="M3" s="7"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13">
       <c r="A4" s="3">
         <v>1</v>
       </c>
@@ -10580,7 +10580,7 @@
       <c r="L4" s="7"/>
       <c r="M4" s="7"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13">
       <c r="A5" s="3">
         <v>1</v>
       </c>
@@ -10609,7 +10609,7 @@
       <c r="L5" s="7"/>
       <c r="M5" s="7"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13">
       <c r="A6" s="3">
         <v>1</v>
       </c>
@@ -10638,7 +10638,7 @@
       <c r="L6" s="7"/>
       <c r="M6" s="7"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13">
       <c r="A7" s="3">
         <v>1</v>
       </c>
@@ -10667,7 +10667,7 @@
       <c r="L7" s="7"/>
       <c r="M7" s="7"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13">
       <c r="A8" s="3">
         <v>1</v>
       </c>
@@ -10696,7 +10696,7 @@
       <c r="L8" s="8"/>
       <c r="M8" s="8"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13">
       <c r="A9" s="3">
         <v>1</v>
       </c>
@@ -10725,7 +10725,7 @@
       <c r="L9" s="7"/>
       <c r="M9" s="8"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13">
       <c r="A10" s="3">
         <v>1</v>
       </c>
@@ -10754,7 +10754,7 @@
       <c r="L10" s="7"/>
       <c r="M10" s="8"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13">
       <c r="A11" s="3">
         <v>1</v>
       </c>
@@ -10783,7 +10783,7 @@
       <c r="L11" s="7"/>
       <c r="M11" s="7"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13">
       <c r="A12" s="3">
         <v>1</v>
       </c>
@@ -10812,7 +10812,7 @@
       <c r="L12" s="7"/>
       <c r="M12" s="7"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13">
       <c r="A13" s="3">
         <v>1</v>
       </c>
@@ -10841,7 +10841,7 @@
       <c r="L13" s="7"/>
       <c r="M13" s="7"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13">
       <c r="A14" s="3">
         <v>1</v>
       </c>
@@ -10870,7 +10870,7 @@
       <c r="L14" s="7"/>
       <c r="M14" s="7"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13">
       <c r="A15" s="3">
         <v>1</v>
       </c>
@@ -10893,7 +10893,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13">
       <c r="A16" s="3">
         <v>1</v>
       </c>
@@ -10916,7 +10916,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13">
       <c r="A17" s="3">
         <v>2</v>
       </c>
@@ -10945,7 +10945,7 @@
       <c r="L17" s="8"/>
       <c r="M17" s="8"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13">
       <c r="A18" s="3">
         <v>2</v>
       </c>
@@ -10974,7 +10974,7 @@
       <c r="L18" s="8"/>
       <c r="M18" s="8"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13">
       <c r="A19" s="3">
         <v>2</v>
       </c>
@@ -11003,7 +11003,7 @@
       <c r="L19" s="8"/>
       <c r="M19" s="8"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13">
       <c r="A20" s="3">
         <v>2</v>
       </c>
@@ -11032,7 +11032,7 @@
       <c r="L20" s="8"/>
       <c r="M20" s="8"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13">
       <c r="A21" s="3">
         <v>2</v>
       </c>
@@ -11061,7 +11061,7 @@
       <c r="L21" s="7"/>
       <c r="M21" s="8"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13">
       <c r="A22" s="3">
         <v>2</v>
       </c>
@@ -11090,7 +11090,7 @@
       <c r="L22" s="7"/>
       <c r="M22" s="8"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13">
       <c r="A23" s="3">
         <v>2</v>
       </c>
@@ -11119,7 +11119,7 @@
       <c r="L23" s="8"/>
       <c r="M23" s="7"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13">
       <c r="A24" s="3">
         <v>2</v>
       </c>
@@ -11148,7 +11148,7 @@
       <c r="L24" s="7"/>
       <c r="M24" s="7"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13">
       <c r="A25" s="3">
         <v>2</v>
       </c>
@@ -11177,7 +11177,7 @@
       <c r="L25" s="7"/>
       <c r="M25" s="7"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13">
       <c r="A26" s="3">
         <v>2</v>
       </c>
@@ -11206,7 +11206,7 @@
       <c r="L26" s="7"/>
       <c r="M26" s="7"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13">
       <c r="A27" s="3">
         <v>2</v>
       </c>
@@ -11235,7 +11235,7 @@
       <c r="L27" s="7"/>
       <c r="M27" s="7"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13">
       <c r="A28" s="3">
         <v>2</v>
       </c>
@@ -11264,7 +11264,7 @@
       <c r="L28" s="7"/>
       <c r="M28" s="7"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13">
       <c r="A29" s="3">
         <v>2</v>
       </c>
@@ -11293,7 +11293,7 @@
       <c r="L29" s="7"/>
       <c r="M29" s="7"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13">
       <c r="A30" s="3">
         <v>2</v>
       </c>
@@ -11322,7 +11322,7 @@
       <c r="L30" s="7"/>
       <c r="M30" s="7"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13">
       <c r="A31" s="3">
         <v>2</v>
       </c>
@@ -11351,7 +11351,7 @@
       <c r="L31" s="7"/>
       <c r="M31" s="7"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13">
       <c r="A32" s="3">
         <v>2</v>
       </c>
@@ -11380,7 +11380,7 @@
       <c r="L32" s="7"/>
       <c r="M32" s="7"/>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13">
       <c r="A33" s="3">
         <v>2</v>
       </c>
@@ -11409,7 +11409,7 @@
       <c r="L33" s="7"/>
       <c r="M33" s="7"/>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13">
       <c r="A34" s="3">
         <v>2</v>
       </c>
@@ -11438,7 +11438,7 @@
       <c r="L34" s="7"/>
       <c r="M34" s="7"/>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13">
       <c r="A35" s="3">
         <v>2</v>
       </c>
@@ -11467,7 +11467,7 @@
       <c r="L35" s="9"/>
       <c r="M35" s="7"/>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13">
       <c r="A36" s="3">
         <v>2</v>
       </c>
@@ -11496,7 +11496,7 @@
       <c r="L36" s="9"/>
       <c r="M36" s="7"/>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13">
       <c r="A37" s="3">
         <v>2</v>
       </c>
@@ -11525,7 +11525,7 @@
       <c r="L37" s="7"/>
       <c r="M37" s="7"/>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13">
       <c r="A38" s="3">
         <v>2</v>
       </c>
@@ -11554,7 +11554,7 @@
       <c r="L38" s="7"/>
       <c r="M38" s="7"/>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13">
       <c r="A39" s="3">
         <v>2</v>
       </c>
@@ -11583,7 +11583,7 @@
       <c r="L39" s="7"/>
       <c r="M39" s="7"/>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13">
       <c r="A40" s="3">
         <v>2</v>
       </c>
@@ -11612,7 +11612,7 @@
       <c r="L40" s="7"/>
       <c r="M40" s="7"/>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13">
       <c r="A41" s="3">
         <v>2</v>
       </c>
@@ -11641,7 +11641,7 @@
       <c r="L41" s="7"/>
       <c r="M41" s="7"/>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13">
       <c r="A42" s="3">
         <v>2</v>
       </c>
@@ -11665,7 +11665,7 @@
       </c>
       <c r="J42" s="11"/>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13">
       <c r="A43" s="3">
         <v>2</v>
       </c>
@@ -11689,7 +11689,7 @@
       </c>
       <c r="J43" s="11"/>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13">
       <c r="A44" s="3">
         <v>2</v>
       </c>
@@ -11718,7 +11718,7 @@
       <c r="L44" s="7"/>
       <c r="M44" s="7"/>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13">
       <c r="A45" s="3">
         <v>2</v>
       </c>
@@ -11747,7 +11747,7 @@
       <c r="L45" s="7"/>
       <c r="M45" s="7"/>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13">
       <c r="A46" s="3">
         <v>2</v>
       </c>
@@ -11776,7 +11776,7 @@
       <c r="L46" s="7"/>
       <c r="M46" s="7"/>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13">
       <c r="A47" s="3">
         <v>2</v>
       </c>
@@ -11805,7 +11805,7 @@
       <c r="L47" s="7"/>
       <c r="M47" s="7"/>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13">
       <c r="A48" s="3">
         <v>2</v>
       </c>
@@ -11834,7 +11834,7 @@
       <c r="L48" s="7"/>
       <c r="M48" s="7"/>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13">
       <c r="A49" s="3">
         <v>3</v>
       </c>
@@ -11863,7 +11863,7 @@
       <c r="L49" s="7"/>
       <c r="M49" s="7"/>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13">
       <c r="A50" s="3">
         <v>3</v>
       </c>
@@ -11892,7 +11892,7 @@
       <c r="L50" s="7"/>
       <c r="M50" s="7"/>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13">
       <c r="A51" s="3">
         <v>3</v>
       </c>
@@ -11921,7 +11921,7 @@
       <c r="L51" s="7"/>
       <c r="M51" s="7"/>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13">
       <c r="A52" s="3">
         <v>3</v>
       </c>
@@ -11950,7 +11950,7 @@
       <c r="L52" s="7"/>
       <c r="M52" s="7"/>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13">
       <c r="A53" s="3">
         <v>3</v>
       </c>
@@ -11979,7 +11979,7 @@
       <c r="L53" s="7"/>
       <c r="M53" s="7"/>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13">
       <c r="A54" s="3">
         <v>3</v>
       </c>
@@ -12008,7 +12008,7 @@
       <c r="L54" s="8"/>
       <c r="M54" s="8"/>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13">
       <c r="A55" s="3">
         <v>3</v>
       </c>
@@ -12037,7 +12037,7 @@
       <c r="L55" s="9"/>
       <c r="M55" s="7"/>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:13">
       <c r="A56" s="3">
         <v>3</v>
       </c>
@@ -12066,7 +12066,7 @@
       <c r="L56" s="7"/>
       <c r="M56" s="7"/>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:13">
       <c r="A57" s="3">
         <v>3</v>
       </c>
@@ -12095,7 +12095,7 @@
       <c r="L57" s="7"/>
       <c r="M57" s="7"/>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:13">
       <c r="A58" s="3">
         <v>3</v>
       </c>
@@ -12124,7 +12124,7 @@
       <c r="L58" s="7"/>
       <c r="M58" s="7"/>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:13">
       <c r="A59" s="3">
         <v>3</v>
       </c>
@@ -12153,7 +12153,7 @@
       <c r="L59" s="9"/>
       <c r="M59" s="7"/>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:13">
       <c r="A60" s="3">
         <v>4</v>
       </c>
@@ -12182,7 +12182,7 @@
       <c r="L60" s="7"/>
       <c r="M60" s="7"/>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:13">
       <c r="A61" s="3">
         <v>4</v>
       </c>
@@ -12211,7 +12211,7 @@
       <c r="L61" s="7"/>
       <c r="M61" s="7"/>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:13">
       <c r="A62" s="3">
         <v>4</v>
       </c>
@@ -12240,7 +12240,7 @@
       <c r="L62" s="7"/>
       <c r="M62" s="7"/>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:13">
       <c r="A63" s="3">
         <v>4</v>
       </c>
@@ -12269,7 +12269,7 @@
       <c r="L63" s="7"/>
       <c r="M63" s="7"/>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:13">
       <c r="A64" s="3">
         <v>4</v>
       </c>
@@ -12298,7 +12298,7 @@
       <c r="L64" s="7"/>
       <c r="M64" s="7"/>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:13">
       <c r="A65" s="3">
         <v>4</v>
       </c>
@@ -12327,7 +12327,7 @@
       <c r="L65" s="7"/>
       <c r="M65" s="7"/>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:13">
       <c r="A66" s="3">
         <v>4</v>
       </c>
@@ -12356,7 +12356,7 @@
       <c r="L66" s="16"/>
       <c r="M66" s="16"/>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:13">
       <c r="A67" s="3">
         <v>4</v>
       </c>
@@ -12385,7 +12385,7 @@
       <c r="L67" s="7"/>
       <c r="M67" s="7"/>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:13">
       <c r="A68" s="3">
         <v>4</v>
       </c>
@@ -12414,7 +12414,7 @@
       <c r="L68" s="7"/>
       <c r="M68" s="7"/>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:13">
       <c r="A69" s="3">
         <v>4</v>
       </c>
@@ -12443,7 +12443,7 @@
       <c r="L69" s="7"/>
       <c r="M69" s="7"/>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:13">
       <c r="A70" s="3">
         <v>4</v>
       </c>
@@ -12472,7 +12472,7 @@
       <c r="L70" s="7"/>
       <c r="M70" s="7"/>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:13">
       <c r="A71" s="3">
         <v>4</v>
       </c>
@@ -12501,7 +12501,7 @@
       <c r="L71" s="7"/>
       <c r="M71" s="7"/>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:13">
       <c r="A72" s="3">
         <v>4</v>
       </c>
@@ -12530,7 +12530,7 @@
       <c r="L72" s="7"/>
       <c r="M72" s="7"/>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:13">
       <c r="A73" s="3">
         <v>4</v>
       </c>
@@ -12559,7 +12559,7 @@
       <c r="L73" s="7"/>
       <c r="M73" s="7"/>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:13">
       <c r="A74" s="3">
         <v>4</v>
       </c>
@@ -12588,7 +12588,7 @@
       <c r="L74" s="7"/>
       <c r="M74" s="7"/>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:13">
       <c r="A75" s="3">
         <v>4</v>
       </c>
@@ -12617,7 +12617,7 @@
       <c r="L75" s="7"/>
       <c r="M75" s="7"/>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:13">
       <c r="A76" s="3">
         <v>4</v>
       </c>
@@ -12646,7 +12646,7 @@
       <c r="L76" s="7"/>
       <c r="M76" s="7"/>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:13">
       <c r="A77" s="3">
         <v>4</v>
       </c>
@@ -12675,7 +12675,7 @@
       <c r="L77" s="7"/>
       <c r="M77" s="7"/>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:13">
       <c r="A78" s="3">
         <v>4</v>
       </c>
@@ -12704,7 +12704,7 @@
       <c r="L78" s="7"/>
       <c r="M78" s="7"/>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:13">
       <c r="A79" s="3">
         <v>4</v>
       </c>
@@ -12733,7 +12733,7 @@
       <c r="L79" s="7"/>
       <c r="M79" s="7"/>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:13">
       <c r="A80" s="3">
         <v>4</v>
       </c>
@@ -12762,7 +12762,7 @@
       <c r="L80" s="7"/>
       <c r="M80" s="7"/>
     </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:13">
       <c r="A81" s="3">
         <v>4</v>
       </c>
@@ -12791,7 +12791,7 @@
       <c r="L81" s="7"/>
       <c r="M81" s="7"/>
     </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:13">
       <c r="A82" s="3">
         <v>4</v>
       </c>
@@ -12820,7 +12820,7 @@
       <c r="L82" s="7"/>
       <c r="M82" s="7"/>
     </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:13">
       <c r="A83" s="3">
         <v>4</v>
       </c>
@@ -12849,7 +12849,7 @@
       <c r="L83" s="7"/>
       <c r="M83" s="7"/>
     </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:13">
       <c r="A84" s="3">
         <v>4</v>
       </c>
@@ -12878,7 +12878,7 @@
       <c r="L84" s="7"/>
       <c r="M84" s="7"/>
     </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:13">
       <c r="A85" s="3">
         <v>4</v>
       </c>
@@ -12907,7 +12907,7 @@
       <c r="L85" s="7"/>
       <c r="M85" s="7"/>
     </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:13">
       <c r="A86" s="3">
         <v>4</v>
       </c>
@@ -12936,7 +12936,7 @@
       <c r="L86" s="7"/>
       <c r="M86" s="7"/>
     </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:13">
       <c r="A87" s="3">
         <v>4</v>
       </c>
@@ -12965,7 +12965,7 @@
       <c r="L87" s="7"/>
       <c r="M87" s="7"/>
     </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:13">
       <c r="A88" s="3">
         <v>4</v>
       </c>
@@ -12994,7 +12994,7 @@
       <c r="L88" s="7"/>
       <c r="M88" s="7"/>
     </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:13">
       <c r="A89" s="3">
         <v>4</v>
       </c>
@@ -13023,7 +13023,7 @@
       <c r="L89" s="7"/>
       <c r="M89" s="7"/>
     </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:13">
       <c r="A90" s="3">
         <v>4</v>
       </c>
@@ -13052,7 +13052,7 @@
       <c r="L90" s="7"/>
       <c r="M90" s="7"/>
     </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:13">
       <c r="A91" s="3">
         <v>4</v>
       </c>
@@ -13081,7 +13081,7 @@
       <c r="L91" s="7"/>
       <c r="M91" s="7"/>
     </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:13">
       <c r="A92" s="3">
         <v>4</v>
       </c>
@@ -13110,7 +13110,7 @@
       <c r="L92" s="7"/>
       <c r="M92" s="7"/>
     </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:13">
       <c r="A93" s="3">
         <v>4</v>
       </c>
@@ -13139,7 +13139,7 @@
       <c r="L93" s="7"/>
       <c r="M93" s="7"/>
     </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:13">
       <c r="A94" s="3">
         <v>4</v>
       </c>
@@ -13168,7 +13168,7 @@
       <c r="L94" s="7"/>
       <c r="M94" s="7"/>
     </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:13">
       <c r="A95" s="3">
         <v>4</v>
       </c>
@@ -13197,7 +13197,7 @@
       <c r="L95" s="7"/>
       <c r="M95" s="7"/>
     </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:13">
       <c r="A96" s="3">
         <v>4</v>
       </c>
@@ -13226,7 +13226,7 @@
       <c r="L96" s="7"/>
       <c r="M96" s="7"/>
     </row>
-    <row r="97" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:13">
       <c r="A97" s="3">
         <v>4</v>
       </c>
@@ -13255,7 +13255,7 @@
       <c r="L97" s="7"/>
       <c r="M97" s="7"/>
     </row>
-    <row r="98" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:13">
       <c r="A98" s="3">
         <v>4</v>
       </c>
@@ -13284,7 +13284,7 @@
       <c r="L98" s="7"/>
       <c r="M98" s="7"/>
     </row>
-    <row r="99" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:13">
       <c r="A99" s="3">
         <v>4</v>
       </c>
@@ -13313,7 +13313,7 @@
       <c r="L99" s="7"/>
       <c r="M99" s="7"/>
     </row>
-    <row r="100" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:13">
       <c r="A100" s="3">
         <v>5</v>
       </c>
@@ -13342,7 +13342,7 @@
       <c r="L100" s="16"/>
       <c r="M100" s="16"/>
     </row>
-    <row r="101" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:13">
       <c r="A101" s="3">
         <v>5</v>
       </c>
@@ -13371,7 +13371,7 @@
       <c r="L101" s="16"/>
       <c r="M101" s="16"/>
     </row>
-    <row r="102" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:13">
       <c r="A102" s="3">
         <v>5</v>
       </c>
@@ -13400,7 +13400,7 @@
       <c r="L102" s="16"/>
       <c r="M102" s="16"/>
     </row>
-    <row r="103" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:13">
       <c r="A103" s="3">
         <v>5</v>
       </c>
@@ -13429,7 +13429,7 @@
       <c r="L103" s="7"/>
       <c r="M103" s="7"/>
     </row>
-    <row r="104" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:13">
       <c r="A104" s="3">
         <v>5</v>
       </c>
@@ -13458,7 +13458,7 @@
       <c r="L104" s="7"/>
       <c r="M104" s="7"/>
     </row>
-    <row r="105" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:13">
       <c r="A105" s="3">
         <v>5</v>
       </c>
@@ -13487,7 +13487,7 @@
       <c r="L105" s="7"/>
       <c r="M105" s="7"/>
     </row>
-    <row r="106" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:13">
       <c r="A106" s="3">
         <v>5</v>
       </c>
@@ -13516,7 +13516,7 @@
       <c r="L106" s="7"/>
       <c r="M106" s="7"/>
     </row>
-    <row r="107" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:13">
       <c r="A107" s="3">
         <v>5</v>
       </c>
@@ -13545,7 +13545,7 @@
       <c r="L107" s="7"/>
       <c r="M107" s="7"/>
     </row>
-    <row r="108" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:13">
       <c r="A108" s="3">
         <v>5</v>
       </c>
@@ -13574,7 +13574,7 @@
       <c r="L108" s="7"/>
       <c r="M108" s="7"/>
     </row>
-    <row r="109" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:13">
       <c r="A109" s="3">
         <v>5</v>
       </c>
@@ -13603,7 +13603,7 @@
       <c r="L109" s="7"/>
       <c r="M109" s="7"/>
     </row>
-    <row r="110" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:13">
       <c r="A110" s="3">
         <v>5</v>
       </c>
@@ -13632,7 +13632,7 @@
       <c r="L110" s="8"/>
       <c r="M110" s="7"/>
     </row>
-    <row r="111" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:13">
       <c r="A111" s="3">
         <v>5</v>
       </c>
@@ -13661,7 +13661,7 @@
       <c r="L111" s="7"/>
       <c r="M111" s="7"/>
     </row>
-    <row r="112" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:13">
       <c r="A112" s="3">
         <v>5</v>
       </c>
@@ -13690,7 +13690,7 @@
       <c r="L112" s="7"/>
       <c r="M112" s="7"/>
     </row>
-    <row r="113" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:13">
       <c r="A113" s="3">
         <v>5</v>
       </c>
@@ -13719,7 +13719,7 @@
       <c r="L113" s="7"/>
       <c r="M113" s="7"/>
     </row>
-    <row r="114" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:13">
       <c r="A114" s="3">
         <v>5</v>
       </c>
@@ -13748,7 +13748,7 @@
       <c r="L114" s="9"/>
       <c r="M114" s="7"/>
     </row>
-    <row r="115" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:13">
       <c r="A115" s="3">
         <v>5</v>
       </c>
@@ -13777,7 +13777,7 @@
       <c r="L115" s="9"/>
       <c r="M115" s="7"/>
     </row>
-    <row r="116" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:13">
       <c r="A116" s="3">
         <v>5</v>
       </c>
@@ -13806,7 +13806,7 @@
       <c r="L116" s="7"/>
       <c r="M116" s="7"/>
     </row>
-    <row r="117" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:13">
       <c r="A117" s="3">
         <v>5</v>
       </c>
@@ -13835,7 +13835,7 @@
       <c r="L117" s="7"/>
       <c r="M117" s="7"/>
     </row>
-    <row r="118" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:13">
       <c r="A118" s="3">
         <v>5</v>
       </c>
@@ -13864,7 +13864,7 @@
       <c r="L118" s="7"/>
       <c r="M118" s="7"/>
     </row>
-    <row r="119" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:13">
       <c r="A119" s="3">
         <v>5</v>
       </c>
@@ -13893,7 +13893,7 @@
       <c r="L119" s="7"/>
       <c r="M119" s="7"/>
     </row>
-    <row r="120" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:13">
       <c r="A120" s="3">
         <v>5</v>
       </c>
@@ -13922,7 +13922,7 @@
       <c r="L120" s="7"/>
       <c r="M120" s="7"/>
     </row>
-    <row r="121" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:13">
       <c r="A121" s="3">
         <v>5</v>
       </c>
@@ -13951,7 +13951,7 @@
       <c r="L121" s="7"/>
       <c r="M121" s="7"/>
     </row>
-    <row r="122" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:13">
       <c r="A122" s="3">
         <v>5</v>
       </c>
@@ -13980,7 +13980,7 @@
       <c r="L122" s="7"/>
       <c r="M122" s="7"/>
     </row>
-    <row r="123" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:13">
       <c r="A123" s="3">
         <v>5</v>
       </c>
@@ -14009,7 +14009,7 @@
       <c r="L123" s="7"/>
       <c r="M123" s="9"/>
     </row>
-    <row r="124" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:13">
       <c r="A124" s="3">
         <v>5</v>
       </c>
@@ -14038,7 +14038,7 @@
       <c r="L124" s="7"/>
       <c r="M124" s="9"/>
     </row>
-    <row r="125" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:13">
       <c r="A125" s="3">
         <v>5</v>
       </c>
@@ -14067,7 +14067,7 @@
       <c r="L125" s="7"/>
       <c r="M125" s="9"/>
     </row>
-    <row r="126" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:13">
       <c r="A126" s="3">
         <v>5</v>
       </c>
@@ -14096,7 +14096,7 @@
       <c r="L126" s="7"/>
       <c r="M126" s="7"/>
     </row>
-    <row r="127" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:13">
       <c r="A127" s="3">
         <v>5</v>
       </c>
@@ -14125,7 +14125,7 @@
       <c r="L127" s="9"/>
       <c r="M127" s="7"/>
     </row>
-    <row r="128" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:13">
       <c r="A128" s="3">
         <v>5</v>
       </c>
@@ -14154,7 +14154,7 @@
       <c r="L128" s="7"/>
       <c r="M128" s="7"/>
     </row>
-    <row r="129" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:13">
       <c r="A129" s="3">
         <v>5</v>
       </c>
@@ -14183,7 +14183,7 @@
       <c r="L129" s="7"/>
       <c r="M129" s="7"/>
     </row>
-    <row r="130" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:13">
       <c r="A130" s="3">
         <v>5</v>
       </c>
@@ -14212,7 +14212,7 @@
       <c r="L130" s="7"/>
       <c r="M130" s="7"/>
     </row>
-    <row r="131" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:13">
       <c r="A131" s="3">
         <v>5</v>
       </c>
@@ -14241,7 +14241,7 @@
       <c r="L131" s="7"/>
       <c r="M131" s="7"/>
     </row>
-    <row r="132" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:13">
       <c r="A132" s="3">
         <v>5</v>
       </c>
@@ -14270,7 +14270,7 @@
       <c r="L132" s="7"/>
       <c r="M132" s="7"/>
     </row>
-    <row r="133" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:13">
       <c r="A133" s="3">
         <v>5</v>
       </c>
@@ -14299,7 +14299,7 @@
       <c r="L133" s="7"/>
       <c r="M133" s="7"/>
     </row>
-    <row r="134" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:13">
       <c r="A134" s="3">
         <v>6</v>
       </c>
@@ -14328,7 +14328,7 @@
       <c r="L134" s="7"/>
       <c r="M134" s="7"/>
     </row>
-    <row r="135" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:13">
       <c r="A135" s="3">
         <v>6</v>
       </c>
@@ -14357,7 +14357,7 @@
       <c r="L135" s="7"/>
       <c r="M135" s="7"/>
     </row>
-    <row r="136" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:13">
       <c r="A136" s="3">
         <v>6</v>
       </c>
@@ -14386,7 +14386,7 @@
       <c r="L136" s="7"/>
       <c r="M136" s="7"/>
     </row>
-    <row r="137" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:13">
       <c r="A137" s="3">
         <v>6</v>
       </c>
@@ -14415,7 +14415,7 @@
       <c r="L137" s="7"/>
       <c r="M137" s="7"/>
     </row>
-    <row r="138" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:13">
       <c r="A138" s="3">
         <v>6</v>
       </c>
@@ -14444,7 +14444,7 @@
       <c r="L138" s="7"/>
       <c r="M138" s="7"/>
     </row>
-    <row r="139" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:13">
       <c r="A139" s="3">
         <v>6</v>
       </c>
@@ -14473,7 +14473,7 @@
       <c r="L139" s="7"/>
       <c r="M139" s="7"/>
     </row>
-    <row r="140" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:13">
       <c r="A140" s="3">
         <v>6</v>
       </c>
@@ -14502,7 +14502,7 @@
       <c r="L140" s="7"/>
       <c r="M140" s="7"/>
     </row>
-    <row r="141" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:13">
       <c r="A141" s="3">
         <v>6</v>
       </c>
@@ -14531,7 +14531,7 @@
       <c r="L141" s="7"/>
       <c r="M141" s="7"/>
     </row>
-    <row r="142" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:13">
       <c r="A142" s="3">
         <v>6</v>
       </c>
@@ -14560,7 +14560,7 @@
       <c r="L142" s="7"/>
       <c r="M142" s="7"/>
     </row>
-    <row r="143" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:13">
       <c r="A143" s="3">
         <v>6</v>
       </c>
@@ -14589,7 +14589,7 @@
       <c r="L143" s="7"/>
       <c r="M143" s="7"/>
     </row>
-    <row r="144" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:13">
       <c r="A144" s="3">
         <v>6</v>
       </c>
@@ -14618,7 +14618,7 @@
       <c r="L144" s="7"/>
       <c r="M144" s="7"/>
     </row>
-    <row r="145" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:13">
       <c r="A145" s="3">
         <v>6</v>
       </c>
@@ -14647,7 +14647,7 @@
       <c r="L145" s="7"/>
       <c r="M145" s="7"/>
     </row>
-    <row r="146" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:13">
       <c r="A146" s="3">
         <v>6</v>
       </c>
@@ -14676,7 +14676,7 @@
       <c r="L146" s="7"/>
       <c r="M146" s="7"/>
     </row>
-    <row r="147" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:13">
       <c r="A147" s="3">
         <v>6</v>
       </c>
@@ -14705,7 +14705,7 @@
       <c r="L147" s="7"/>
       <c r="M147" s="7"/>
     </row>
-    <row r="148" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:13">
       <c r="A148" s="3">
         <v>6</v>
       </c>
@@ -14734,7 +14734,7 @@
       <c r="L148" s="7"/>
       <c r="M148" s="7"/>
     </row>
-    <row r="149" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:13">
       <c r="A149" s="3">
         <v>6</v>
       </c>
@@ -14763,7 +14763,7 @@
       <c r="L149" s="7"/>
       <c r="M149" s="7"/>
     </row>
-    <row r="150" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:13">
       <c r="A150" s="3">
         <v>6</v>
       </c>
@@ -14792,7 +14792,7 @@
       <c r="L150" s="7"/>
       <c r="M150" s="7"/>
     </row>
-    <row r="151" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:13">
       <c r="A151" s="3">
         <v>6</v>
       </c>
@@ -14821,7 +14821,7 @@
       <c r="L151" s="7"/>
       <c r="M151" s="7"/>
     </row>
-    <row r="152" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:13">
       <c r="A152" s="3">
         <v>6</v>
       </c>
@@ -14850,7 +14850,7 @@
       <c r="L152" s="7"/>
       <c r="M152" s="7"/>
     </row>
-    <row r="153" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:13">
       <c r="A153" s="3">
         <v>7</v>
       </c>
@@ -14879,7 +14879,7 @@
       <c r="L153" s="8"/>
       <c r="M153" s="8"/>
     </row>
-    <row r="154" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:13">
       <c r="A154" s="3">
         <v>7</v>
       </c>
@@ -14908,7 +14908,7 @@
       <c r="L154" s="8"/>
       <c r="M154" s="8"/>
     </row>
-    <row r="155" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:13">
       <c r="A155" s="3">
         <v>7</v>
       </c>
@@ -14937,7 +14937,7 @@
       <c r="L155" s="8"/>
       <c r="M155" s="8"/>
     </row>
-    <row r="156" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:13">
       <c r="A156" s="3">
         <v>7</v>
       </c>
@@ -14966,7 +14966,7 @@
       <c r="L156" s="8"/>
       <c r="M156" s="8"/>
     </row>
-    <row r="157" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:13">
       <c r="A157" s="3">
         <v>7</v>
       </c>
@@ -14995,7 +14995,7 @@
       <c r="L157" s="8"/>
       <c r="M157" s="8"/>
     </row>
-    <row r="158" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:13">
       <c r="A158" s="3">
         <v>7</v>
       </c>
@@ -15024,7 +15024,7 @@
       <c r="L158" s="8"/>
       <c r="M158" s="8"/>
     </row>
-    <row r="159" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:13">
       <c r="A159" s="3">
         <v>7</v>
       </c>
@@ -15053,7 +15053,7 @@
       <c r="L159" s="8"/>
       <c r="M159" s="8"/>
     </row>
-    <row r="160" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:13">
       <c r="A160" s="3">
         <v>7</v>
       </c>
@@ -15082,7 +15082,7 @@
       <c r="L160" s="8"/>
       <c r="M160" s="8"/>
     </row>
-    <row r="161" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:13">
       <c r="A161" s="3">
         <v>7</v>
       </c>
@@ -15111,7 +15111,7 @@
       <c r="L161" s="7"/>
       <c r="M161" s="8"/>
     </row>
-    <row r="162" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:13">
       <c r="A162" s="3">
         <v>7</v>
       </c>
@@ -15140,7 +15140,7 @@
       <c r="L162" s="7"/>
       <c r="M162" s="8"/>
     </row>
-    <row r="163" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:13">
       <c r="A163" s="3">
         <v>7</v>
       </c>
@@ -15169,7 +15169,7 @@
       <c r="L163" s="8"/>
       <c r="M163" s="7"/>
     </row>
-    <row r="164" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:13">
       <c r="A164" s="3">
         <v>7</v>
       </c>
@@ -15198,7 +15198,7 @@
       <c r="L164" s="8"/>
       <c r="M164" s="7"/>
     </row>
-    <row r="165" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:13">
       <c r="A165" s="3">
         <v>7</v>
       </c>
@@ -15227,7 +15227,7 @@
       <c r="L165" s="8"/>
       <c r="M165" s="7"/>
     </row>
-    <row r="166" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:13">
       <c r="A166" s="3">
         <v>7</v>
       </c>
@@ -15256,7 +15256,7 @@
       <c r="L166" s="8"/>
       <c r="M166" s="7"/>
     </row>
-    <row r="167" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:13">
       <c r="A167" s="3">
         <v>7</v>
       </c>
@@ -15285,7 +15285,7 @@
       <c r="L167" s="8"/>
       <c r="M167" s="7"/>
     </row>
-    <row r="168" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:13">
       <c r="A168" s="3">
         <v>7</v>
       </c>
@@ -15314,7 +15314,7 @@
       <c r="L168" s="8"/>
       <c r="M168" s="7"/>
     </row>
-    <row r="169" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:13">
       <c r="A169" s="3">
         <v>7</v>
       </c>
@@ -15343,7 +15343,7 @@
       <c r="L169" s="8"/>
       <c r="M169" s="7"/>
     </row>
-    <row r="170" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:13">
       <c r="A170" s="3">
         <v>7</v>
       </c>
@@ -15372,7 +15372,7 @@
       <c r="L170" s="7"/>
       <c r="M170" s="7"/>
     </row>
-    <row r="171" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:13">
       <c r="A171" s="3">
         <v>7</v>
       </c>
@@ -15401,7 +15401,7 @@
       <c r="L171" s="8"/>
       <c r="M171" s="8"/>
     </row>
-    <row r="172" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:13">
       <c r="A172" s="3">
         <v>7</v>
       </c>
@@ -15430,7 +15430,7 @@
       <c r="L172" s="8"/>
       <c r="M172" s="8"/>
     </row>
-    <row r="173" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:13">
       <c r="A173" s="3">
         <v>7</v>
       </c>
@@ -15459,7 +15459,7 @@
       <c r="L173" s="7"/>
       <c r="M173" s="7"/>
     </row>
-    <row r="174" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:13">
       <c r="A174" s="3">
         <v>7</v>
       </c>
@@ -15488,7 +15488,7 @@
       <c r="L174" s="7"/>
       <c r="M174" s="7"/>
     </row>
-    <row r="175" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:13">
       <c r="A175" s="3">
         <v>7</v>
       </c>
@@ -15517,7 +15517,7 @@
       <c r="L175" s="7"/>
       <c r="M175" s="7"/>
     </row>
-    <row r="176" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:13">
       <c r="A176" s="3">
         <v>7</v>
       </c>
@@ -15546,7 +15546,7 @@
       <c r="L176" s="7"/>
       <c r="M176" s="7"/>
     </row>
-    <row r="177" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:13">
       <c r="A177" s="3">
         <v>7</v>
       </c>
@@ -15575,7 +15575,7 @@
       <c r="L177" s="9"/>
       <c r="M177" s="9"/>
     </row>
-    <row r="178" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:13">
       <c r="A178" s="3">
         <v>8</v>
       </c>
@@ -15604,7 +15604,7 @@
       <c r="L178" s="7"/>
       <c r="M178" s="7"/>
     </row>
-    <row r="179" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:13">
       <c r="A179" s="3">
         <v>8</v>
       </c>
@@ -15633,7 +15633,7 @@
       <c r="L179" s="7"/>
       <c r="M179" s="7"/>
     </row>
-    <row r="180" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:13">
       <c r="A180" s="3">
         <v>8</v>
       </c>
@@ -15662,7 +15662,7 @@
       <c r="L180" s="7"/>
       <c r="M180" s="7"/>
     </row>
-    <row r="181" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:13">
       <c r="A181" s="3">
         <v>8</v>
       </c>
@@ -15691,7 +15691,7 @@
       <c r="L181" s="7"/>
       <c r="M181" s="7"/>
     </row>
-    <row r="182" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:13">
       <c r="A182" s="3">
         <v>8</v>
       </c>
@@ -15720,7 +15720,7 @@
       <c r="L182" s="7"/>
       <c r="M182" s="7"/>
     </row>
-    <row r="183" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:13">
       <c r="A183" s="3">
         <v>8</v>
       </c>
@@ -15749,7 +15749,7 @@
       <c r="L183" s="7"/>
       <c r="M183" s="7"/>
     </row>
-    <row r="184" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:13">
       <c r="A184" s="3">
         <v>8</v>
       </c>
@@ -15778,7 +15778,7 @@
       <c r="L184" s="7"/>
       <c r="M184" s="7"/>
     </row>
-    <row r="185" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:13">
       <c r="A185" s="3">
         <v>8</v>
       </c>
@@ -15807,7 +15807,7 @@
       <c r="L185" s="7"/>
       <c r="M185" s="7"/>
     </row>
-    <row r="186" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:13">
       <c r="A186" s="3">
         <v>8</v>
       </c>
@@ -15836,7 +15836,7 @@
       <c r="L186" s="7"/>
       <c r="M186" s="7"/>
     </row>
-    <row r="187" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:13">
       <c r="A187" s="3">
         <v>8</v>
       </c>
@@ -15865,7 +15865,7 @@
       <c r="L187" s="7"/>
       <c r="M187" s="7"/>
     </row>
-    <row r="188" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:13">
       <c r="A188" s="3">
         <v>8</v>
       </c>
@@ -15894,7 +15894,7 @@
       <c r="L188" s="7"/>
       <c r="M188" s="7"/>
     </row>
-    <row r="189" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:13">
       <c r="A189" s="3">
         <v>8</v>
       </c>
@@ -15923,7 +15923,7 @@
       <c r="L189" s="7"/>
       <c r="M189" s="7"/>
     </row>
-    <row r="190" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:13">
       <c r="A190" s="3">
         <v>8</v>
       </c>
@@ -15952,7 +15952,7 @@
       <c r="L190" s="7"/>
       <c r="M190" s="7"/>
     </row>
-    <row r="191" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:13">
       <c r="A191" s="3">
         <v>9</v>
       </c>
@@ -15981,7 +15981,7 @@
       <c r="L191" s="7"/>
       <c r="M191" s="7"/>
     </row>
-    <row r="192" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:13">
       <c r="A192" s="3">
         <v>9</v>
       </c>
@@ -16010,7 +16010,7 @@
       <c r="L192" s="7"/>
       <c r="M192" s="7"/>
     </row>
-    <row r="193" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:13">
       <c r="A193" s="3">
         <v>9</v>
       </c>
@@ -16039,7 +16039,7 @@
       <c r="L193" s="7"/>
       <c r="M193" s="7"/>
     </row>
-    <row r="194" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:13">
       <c r="A194" s="3">
         <v>9</v>
       </c>
@@ -16068,7 +16068,7 @@
       <c r="L194" s="7"/>
       <c r="M194" s="7"/>
     </row>
-    <row r="195" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:13">
       <c r="A195" s="3">
         <v>9</v>
       </c>
@@ -16097,7 +16097,7 @@
       <c r="L195" s="16"/>
       <c r="M195" s="16"/>
     </row>
-    <row r="196" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:13">
       <c r="A196" s="3">
         <v>9</v>
       </c>
@@ -16126,7 +16126,7 @@
       <c r="L196" s="7"/>
       <c r="M196" s="7"/>
     </row>
-    <row r="197" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:13">
       <c r="A197" s="3">
         <v>9</v>
       </c>
@@ -16155,7 +16155,7 @@
       <c r="L197" s="7"/>
       <c r="M197" s="7"/>
     </row>
-    <row r="198" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:13">
       <c r="A198" s="3">
         <v>9</v>
       </c>
@@ -16184,7 +16184,7 @@
       <c r="L198" s="7"/>
       <c r="M198" s="7"/>
     </row>
-    <row r="199" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:13">
       <c r="A199" s="3">
         <v>9</v>
       </c>
@@ -16213,7 +16213,7 @@
       <c r="L199" s="7"/>
       <c r="M199" s="7"/>
     </row>
-    <row r="200" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:13">
       <c r="A200" s="3">
         <v>9</v>
       </c>
@@ -16242,7 +16242,7 @@
       <c r="L200" s="7"/>
       <c r="M200" s="7"/>
     </row>
-    <row r="201" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:13">
       <c r="A201" s="3">
         <v>9</v>
       </c>
@@ -16271,7 +16271,7 @@
       <c r="L201" s="7"/>
       <c r="M201" s="7"/>
     </row>
-    <row r="202" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:13">
       <c r="A202" s="3">
         <v>9</v>
       </c>
@@ -16300,7 +16300,7 @@
       <c r="L202" s="7"/>
       <c r="M202" s="7"/>
     </row>
-    <row r="203" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:13">
       <c r="A203" s="3">
         <v>9</v>
       </c>
@@ -16329,7 +16329,7 @@
       <c r="L203" s="7"/>
       <c r="M203" s="7"/>
     </row>
-    <row r="204" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:13">
       <c r="A204" s="3">
         <v>9</v>
       </c>
@@ -16358,7 +16358,7 @@
       <c r="L204" s="7"/>
       <c r="M204" s="7"/>
     </row>
-    <row r="205" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:13">
       <c r="A205" s="3">
         <v>9</v>
       </c>
@@ -16387,7 +16387,7 @@
       <c r="L205" s="7"/>
       <c r="M205" s="7"/>
     </row>
-    <row r="206" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:13">
       <c r="A206" s="3">
         <v>9</v>
       </c>
@@ -16416,7 +16416,7 @@
       <c r="L206" s="7"/>
       <c r="M206" s="7"/>
     </row>
-    <row r="207" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:13">
       <c r="A207" s="3">
         <v>9</v>
       </c>
@@ -16445,7 +16445,7 @@
       <c r="L207" s="7"/>
       <c r="M207" s="7"/>
     </row>
-    <row r="208" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:13">
       <c r="A208" s="3">
         <v>9</v>
       </c>
@@ -16474,7 +16474,7 @@
       <c r="L208" s="7"/>
       <c r="M208" s="7"/>
     </row>
-    <row r="209" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:13">
       <c r="A209" s="3">
         <v>9</v>
       </c>
@@ -16503,7 +16503,7 @@
       <c r="L209" s="7"/>
       <c r="M209" s="7"/>
     </row>
-    <row r="210" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:13">
       <c r="A210" s="3">
         <v>9</v>
       </c>
@@ -16532,7 +16532,7 @@
       <c r="L210" s="7"/>
       <c r="M210" s="7"/>
     </row>
-    <row r="211" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:13">
       <c r="A211" s="3">
         <v>9</v>
       </c>
@@ -16561,7 +16561,7 @@
       <c r="L211" s="9"/>
       <c r="M211" s="9"/>
     </row>
-    <row r="212" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:13">
       <c r="A212" s="3">
         <v>9</v>
       </c>
@@ -16590,7 +16590,7 @@
       <c r="L212" s="7"/>
       <c r="M212" s="7"/>
     </row>
-    <row r="213" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:13">
       <c r="A213" s="3">
         <v>9</v>
       </c>
@@ -16619,7 +16619,7 @@
       <c r="L213" s="7"/>
       <c r="M213" s="7"/>
     </row>
-    <row r="214" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:13">
       <c r="A214" s="3">
         <v>9</v>
       </c>
@@ -16648,7 +16648,7 @@
       <c r="L214" s="7"/>
       <c r="M214" s="7"/>
     </row>
-    <row r="215" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:13">
       <c r="A215" s="3">
         <v>9</v>
       </c>
@@ -16677,7 +16677,7 @@
       <c r="L215" s="7"/>
       <c r="M215" s="7"/>
     </row>
-    <row r="216" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:13">
       <c r="A216" s="3">
         <v>10</v>
       </c>
@@ -16706,7 +16706,7 @@
       <c r="L216" s="7"/>
       <c r="M216" s="7"/>
     </row>
-    <row r="217" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:13">
       <c r="A217" s="3">
         <v>10</v>
       </c>
@@ -16735,7 +16735,7 @@
       <c r="L217" s="7"/>
       <c r="M217" s="7"/>
     </row>
-    <row r="218" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:13">
       <c r="A218" s="3">
         <v>10</v>
       </c>
@@ -16764,7 +16764,7 @@
       <c r="L218" s="7"/>
       <c r="M218" s="7"/>
     </row>
-    <row r="219" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:13">
       <c r="A219" s="3">
         <v>10</v>
       </c>
@@ -16793,7 +16793,7 @@
       <c r="L219" s="7"/>
       <c r="M219" s="7"/>
     </row>
-    <row r="220" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:13">
       <c r="A220" s="3">
         <v>10</v>
       </c>
@@ -16822,7 +16822,7 @@
       <c r="L220" s="7"/>
       <c r="M220" s="7"/>
     </row>
-    <row r="221" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:13">
       <c r="A221" s="3">
         <v>10</v>
       </c>
@@ -16851,7 +16851,7 @@
       <c r="L221" s="7"/>
       <c r="M221" s="7"/>
     </row>
-    <row r="222" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:13">
       <c r="A222" s="3">
         <v>10</v>
       </c>
@@ -16880,7 +16880,7 @@
       <c r="L222" s="7"/>
       <c r="M222" s="7"/>
     </row>
-    <row r="223" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:13">
       <c r="A223" s="3">
         <v>10</v>
       </c>
@@ -16909,7 +16909,7 @@
       <c r="L223" s="7"/>
       <c r="M223" s="7"/>
     </row>
-    <row r="224" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:13">
       <c r="A224" s="3">
         <v>10</v>
       </c>
@@ -16938,7 +16938,7 @@
       <c r="L224" s="7"/>
       <c r="M224" s="7"/>
     </row>
-    <row r="225" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:13">
       <c r="A225" s="3">
         <v>10</v>
       </c>
@@ -16967,7 +16967,7 @@
       <c r="L225" s="7"/>
       <c r="M225" s="7"/>
     </row>
-    <row r="226" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:13">
       <c r="A226" s="3">
         <v>10</v>
       </c>
@@ -16996,7 +16996,7 @@
       <c r="L226" s="7"/>
       <c r="M226" s="7"/>
     </row>
-    <row r="227" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:13">
       <c r="A227" s="3">
         <v>10</v>
       </c>
@@ -17025,7 +17025,7 @@
       <c r="L227" s="7"/>
       <c r="M227" s="7"/>
     </row>
-    <row r="228" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:13">
       <c r="A228" s="3">
         <v>10</v>
       </c>

</xml_diff>